<commit_message>
PREG -> CRI adress
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
+++ b/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6684B80C-F1E9-4865-804A-BAF05A0AD27B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F13492-002F-4311-AFC3-03ED3421B9EE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2562" uniqueCount="814">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2593" uniqueCount="822">
   <si>
     <t>setting_name</t>
   </si>
@@ -2489,6 +2489,30 @@
   </si>
   <si>
     <t>data('vping') == '2'</t>
+  </si>
+  <si>
+    <t>data('REGID') != null</t>
+  </si>
+  <si>
+    <t>data('MOMA') == '1'</t>
+  </si>
+  <si>
+    <t>data('mor')</t>
+  </si>
+  <si>
+    <t>data('casa')</t>
+  </si>
+  <si>
+    <t>data('fogao')</t>
+  </si>
+  <si>
+    <t>mor</t>
+  </si>
+  <si>
+    <t>casa</t>
+  </si>
+  <si>
+    <t>fogau</t>
   </si>
 </sst>
 </file>
@@ -4552,11 +4576,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
-  <dimension ref="A1:C218"/>
+  <dimension ref="A1:C222"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A201" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A207" sqref="A207"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A204" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C221" sqref="C221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6863,6 +6887,39 @@
       </c>
       <c r="C218" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>819</v>
+      </c>
+      <c r="B220" t="s">
+        <v>25</v>
+      </c>
+      <c r="C220" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>820</v>
+      </c>
+      <c r="B221" t="s">
+        <v>25</v>
+      </c>
+      <c r="C221" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>821</v>
+      </c>
+      <c r="B222" t="s">
+        <v>25</v>
+      </c>
+      <c r="C222" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -6963,11 +7020,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7127,218 +7184,317 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" t="s">
-        <v>52</v>
-      </c>
-      <c r="G13" t="s">
-        <v>53</v>
-      </c>
-      <c r="H13" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>50</v>
       </c>
-      <c r="E14" t="s">
-        <v>54</v>
+      <c r="E14" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="F14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H14" t="s">
-        <v>56</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>57</v>
+        <v>257</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H15" t="s">
+        <v>56</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
         <v>25</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F16" t="s">
         <v>58</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G16" t="s">
         <v>59</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H16" t="s">
         <v>59</v>
       </c>
-      <c r="J15" s="12"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="J16" s="12"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F21" t="s">
+        <v>113</v>
+      </c>
+      <c r="G21" t="s">
+        <v>312</v>
+      </c>
+      <c r="H21" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>126</v>
+      </c>
+      <c r="F23" t="s">
+        <v>66</v>
+      </c>
+      <c r="I23" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>126</v>
+      </c>
+      <c r="F24" t="s">
+        <v>68</v>
+      </c>
+      <c r="I24" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>126</v>
+      </c>
+      <c r="F25" t="s">
+        <v>70</v>
+      </c>
+      <c r="I25" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
         <v>25</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F30" t="s">
         <v>66</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G30" t="s">
         <v>67</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H30" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
         <v>25</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F31" t="s">
         <v>68</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G31" t="s">
         <v>69</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H31" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
         <v>25</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F32" t="s">
         <v>70</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G32" t="s">
         <v>71</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H32" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
         <v>72</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F35" t="s">
         <v>89</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G35" t="s">
         <v>90</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H35" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
-        <v>22</v>
-      </c>
-      <c r="E26" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38" t="s">
         <v>93</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F38" t="s">
         <v>94</v>
       </c>
-      <c r="G26" s="6" t="s">
+      <c r="G38" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="H38" s="6" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>88</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C39" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D28" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
         <v>72</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F40" t="s">
         <v>102</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="G40" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="H40" s="6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-      <c r="B31" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="15"/>
+      <c r="B43" t="s">
         <v>88</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C43" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
         <v>786</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
-      <c r="B33" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="15"/>
+      <c r="B45" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>260</v>
       </c>
     </row>
@@ -7909,8 +8065,8 @@
   <dimension ref="A1:M169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B90" sqref="B90"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H50" sqref="D50:H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9614,7 +9770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A7F4833-88F1-44B1-8A75-76AFCBB7BC62}">
   <dimension ref="A1:J281"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A221" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A236" sqref="A236"/>
     </sheetView>

</xml_diff>

<commit_message>
Changes in variables in tables
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
+++ b/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F13492-002F-4311-AFC3-03ED3421B9EE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1C83B7-2338-4023-8F00-7828A7E45385}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2593" uniqueCount="822">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2595" uniqueCount="823">
   <si>
     <t>setting_name</t>
   </si>
@@ -2513,6 +2513,9 @@
   </si>
   <si>
     <t>fogau</t>
+  </si>
+  <si>
+    <t>ESTADO</t>
   </si>
 </sst>
 </file>
@@ -4576,11 +4579,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
-  <dimension ref="A1:C222"/>
+  <dimension ref="A1:C214"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A204" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C221" sqref="C221"/>
+      <pane ySplit="1" topLeftCell="A198" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C214" sqref="C214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4603,10 +4606,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>630</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
@@ -4614,10 +4617,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
+        <v>633</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
@@ -4625,10 +4628,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>715</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -4636,10 +4639,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>720</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -4647,10 +4650,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
+        <v>718</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -4658,7 +4661,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
@@ -4669,10 +4672,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>621</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
@@ -4680,10 +4683,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>70</v>
+        <v>171</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -4691,43 +4694,54 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>89</v>
+        <v>393</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>120</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>256</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
+      <c r="A11" t="s">
+        <v>389</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="C11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>401</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B13" t="s">
-        <v>72</v>
+        <v>397</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>343</v>
       </c>
       <c r="C13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>704</v>
       </c>
       <c r="B14" t="s">
-        <v>120</v>
+        <v>22</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -4735,9 +4749,9 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" t="s">
+        <v>702</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>72</v>
       </c>
       <c r="C15" t="b">
@@ -4746,32 +4760,54 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>120</v>
+        <v>706</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
       </c>
       <c r="C16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>322</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>118</v>
+        <v>600</v>
       </c>
       <c r="B18" t="s">
-        <v>119</v>
+        <v>22</v>
       </c>
       <c r="C18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>349</v>
+      </c>
+      <c r="B19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>171</v>
+        <v>372</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>120</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
@@ -4779,10 +4815,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>142</v>
+        <v>356</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
@@ -4790,10 +4826,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>156</v>
+        <v>377</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="C22" t="b">
         <v>0</v>
@@ -4801,10 +4837,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>152</v>
+        <v>353</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C23" t="b">
         <v>0</v>
@@ -4812,10 +4848,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>161</v>
+        <v>375</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C24" t="b">
         <v>0</v>
@@ -4823,10 +4859,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>160</v>
+        <v>346</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C25" t="b">
         <v>0</v>
@@ -4834,7 +4870,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>139</v>
+        <v>369</v>
       </c>
       <c r="B26" t="s">
         <v>22</v>
@@ -4845,10 +4881,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>136</v>
+        <v>359</v>
       </c>
       <c r="B27" t="s">
-        <v>126</v>
+        <v>22</v>
       </c>
       <c r="C27" t="b">
         <v>0</v>
@@ -4856,7 +4892,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>144</v>
+        <v>379</v>
       </c>
       <c r="B28" t="s">
         <v>22</v>
@@ -4867,32 +4903,32 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>128</v>
+        <v>362</v>
       </c>
       <c r="B29" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="C29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>132</v>
+        <v>381</v>
       </c>
       <c r="B30" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="C30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>174</v>
+        <v>340</v>
       </c>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C31" t="b">
         <v>0</v>
@@ -4900,7 +4936,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>168</v>
+        <v>357</v>
       </c>
       <c r="B32" t="s">
         <v>22</v>
@@ -4911,10 +4947,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>164</v>
+        <v>378</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C33" t="b">
         <v>0</v>
@@ -4922,10 +4958,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>163</v>
+        <v>345</v>
       </c>
       <c r="B34" t="s">
-        <v>25</v>
+        <v>343</v>
       </c>
       <c r="C34" t="b">
         <v>0</v>
@@ -4933,7 +4969,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>165</v>
+        <v>364</v>
       </c>
       <c r="B35" t="s">
         <v>22</v>
@@ -4944,21 +4980,32 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>147</v>
+        <v>382</v>
       </c>
       <c r="B36" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>367</v>
+      </c>
+      <c r="B37" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>265</v>
+        <v>384</v>
       </c>
       <c r="B38" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="C38" t="b">
         <v>0</v>
@@ -4966,10 +5013,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>269</v>
+        <v>351</v>
       </c>
       <c r="B39" t="s">
-        <v>120</v>
+        <v>22</v>
       </c>
       <c r="C39" t="b">
         <v>0</v>
@@ -4977,7 +5024,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>109</v>
+        <v>373</v>
       </c>
       <c r="B40" t="s">
         <v>22</v>
@@ -4988,10 +5035,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>273</v>
+        <v>142</v>
       </c>
       <c r="B41" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
       <c r="C41" t="b">
         <v>0</v>
@@ -5010,10 +5057,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>295</v>
+        <v>68</v>
       </c>
       <c r="B43" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C43" t="b">
         <v>0</v>
@@ -5021,21 +5068,21 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>299</v>
+        <v>820</v>
       </c>
       <c r="B44" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>304</v>
+        <v>116</v>
       </c>
       <c r="B45" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="C45" t="b">
         <v>0</v>
@@ -5043,10 +5090,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>110</v>
+        <v>156</v>
       </c>
       <c r="B46" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C46" t="b">
         <v>0</v>
@@ -5054,10 +5101,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>111</v>
+        <v>152</v>
       </c>
       <c r="B47" t="s">
-        <v>120</v>
+        <v>25</v>
       </c>
       <c r="C47" t="b">
         <v>0</v>
@@ -5065,10 +5112,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>112</v>
+        <v>700</v>
       </c>
       <c r="B48" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C48" t="b">
         <v>0</v>
@@ -5076,10 +5123,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>123</v>
+        <v>331</v>
       </c>
       <c r="B49" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C49" t="b">
         <v>0</v>
@@ -5087,10 +5134,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>125</v>
+        <v>326</v>
       </c>
       <c r="B50" t="s">
-        <v>120</v>
+        <v>22</v>
       </c>
       <c r="C50" t="b">
         <v>0</v>
@@ -5098,7 +5145,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>124</v>
+        <v>329</v>
       </c>
       <c r="B51" t="s">
         <v>25</v>
@@ -5109,7 +5156,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>307</v>
+        <v>110</v>
       </c>
       <c r="B52" t="s">
         <v>22</v>
@@ -5120,21 +5167,21 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>309</v>
+        <v>768</v>
       </c>
       <c r="B53" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>113</v>
-      </c>
-      <c r="B54" t="s">
-        <v>22</v>
+        <v>277</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>108</v>
       </c>
       <c r="C54" t="b">
         <v>0</v>
@@ -5142,10 +5189,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>114</v>
+        <v>771</v>
       </c>
       <c r="B55" t="s">
-        <v>120</v>
+        <v>25</v>
       </c>
       <c r="C55" t="b">
         <v>0</v>
@@ -5153,10 +5200,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>115</v>
+        <v>665</v>
       </c>
       <c r="B56" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C56" t="b">
         <v>0</v>
@@ -5164,9 +5211,9 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>116</v>
-      </c>
-      <c r="B57" t="s">
+        <v>668</v>
+      </c>
+      <c r="B57" s="6" t="s">
         <v>72</v>
       </c>
       <c r="C57" t="b">
@@ -5175,7 +5222,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>317</v>
+        <v>708</v>
       </c>
       <c r="B58" t="s">
         <v>22</v>
@@ -5186,10 +5233,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>322</v>
+        <v>635</v>
       </c>
       <c r="B59" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C59" t="b">
         <v>0</v>
@@ -5197,10 +5244,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>326</v>
-      </c>
-      <c r="B60" t="s">
-        <v>22</v>
+        <v>638</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="C60" t="b">
         <v>0</v>
@@ -5208,10 +5255,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>329</v>
+        <v>111</v>
       </c>
       <c r="B61" t="s">
-        <v>25</v>
+        <v>120</v>
       </c>
       <c r="C61" t="b">
         <v>0</v>
@@ -5219,10 +5266,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>331</v>
+        <v>125</v>
       </c>
       <c r="B62" t="s">
-        <v>25</v>
+        <v>120</v>
       </c>
       <c r="C62" t="b">
         <v>0</v>
@@ -5230,10 +5277,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>333</v>
+        <v>114</v>
       </c>
       <c r="B63" t="s">
-        <v>22</v>
+        <v>120</v>
       </c>
       <c r="C63" t="b">
         <v>0</v>
@@ -5241,7 +5288,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>336</v>
+        <v>710</v>
       </c>
       <c r="B64" t="s">
         <v>22</v>
@@ -5252,10 +5299,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>385</v>
+        <v>713</v>
       </c>
       <c r="B65" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="C65" t="b">
         <v>0</v>
@@ -5263,7 +5310,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>340</v>
+        <v>675</v>
       </c>
       <c r="B66" t="s">
         <v>22</v>
@@ -5274,10 +5321,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>345</v>
-      </c>
-      <c r="B67" t="s">
-        <v>343</v>
+        <v>686</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="C67" t="b">
         <v>0</v>
@@ -5285,7 +5332,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>346</v>
+        <v>682</v>
       </c>
       <c r="B68" t="s">
         <v>22</v>
@@ -5296,10 +5343,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>349</v>
+        <v>646</v>
       </c>
       <c r="B69" t="s">
-        <v>120</v>
+        <v>22</v>
       </c>
       <c r="C69" t="b">
         <v>0</v>
@@ -5307,10 +5354,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>351</v>
-      </c>
-      <c r="B70" t="s">
-        <v>22</v>
+        <v>650</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="C70" t="b">
         <v>0</v>
@@ -5318,10 +5365,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>353</v>
-      </c>
-      <c r="B71" t="s">
-        <v>22</v>
+        <v>652</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="C71" t="b">
         <v>0</v>
@@ -5329,10 +5376,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>356</v>
+        <v>697</v>
       </c>
       <c r="B72" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="C72" t="b">
         <v>0</v>
@@ -5340,7 +5387,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>357</v>
+        <v>623</v>
       </c>
       <c r="B73" t="s">
         <v>22</v>
@@ -5351,7 +5398,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>359</v>
+        <v>626</v>
       </c>
       <c r="B74" t="s">
         <v>22</v>
@@ -5362,10 +5409,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>362</v>
+        <v>269</v>
       </c>
       <c r="B75" t="s">
-        <v>72</v>
+        <v>120</v>
       </c>
       <c r="C75" t="b">
         <v>0</v>
@@ -5373,10 +5420,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>364</v>
+        <v>273</v>
       </c>
       <c r="B76" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="C76" t="b">
         <v>0</v>
@@ -5384,10 +5431,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>367</v>
+        <v>109</v>
       </c>
       <c r="B77" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
       <c r="C77" t="b">
         <v>0</v>
@@ -5395,7 +5442,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>369</v>
+        <v>609</v>
       </c>
       <c r="B78" t="s">
         <v>22</v>
@@ -5406,7 +5453,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>372</v>
+        <v>580</v>
       </c>
       <c r="B79" t="s">
         <v>120</v>
@@ -5417,18 +5464,18 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>373</v>
-      </c>
-      <c r="B80" t="s">
-        <v>22</v>
+        <v>567</v>
+      </c>
+      <c r="B80" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="C80" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>375</v>
+        <v>585</v>
       </c>
       <c r="B81" t="s">
         <v>22</v>
@@ -5439,18 +5486,18 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>377</v>
-      </c>
-      <c r="B82" t="s">
-        <v>72</v>
+        <v>583</v>
+      </c>
+      <c r="B82" s="11" t="s">
+        <v>343</v>
       </c>
       <c r="C82" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>378</v>
+        <v>640</v>
       </c>
       <c r="B83" t="s">
         <v>22</v>
@@ -5461,10 +5508,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>379</v>
-      </c>
-      <c r="B84" t="s">
-        <v>22</v>
+        <v>644</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="C84" t="b">
         <v>0</v>
@@ -5472,10 +5519,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>381</v>
+        <v>161</v>
       </c>
       <c r="B85" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="C85" t="b">
         <v>0</v>
@@ -5483,10 +5530,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>382</v>
+        <v>160</v>
       </c>
       <c r="B86" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C86" t="b">
         <v>0</v>
@@ -5494,21 +5541,32 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>384</v>
+        <v>70</v>
       </c>
       <c r="B87" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="C87" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>821</v>
+      </c>
+      <c r="B88" t="s">
+        <v>25</v>
+      </c>
+      <c r="C88" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>277</v>
-      </c>
-      <c r="B89" s="13" t="s">
-        <v>108</v>
+        <v>139</v>
+      </c>
+      <c r="B89" t="s">
+        <v>22</v>
       </c>
       <c r="C89" t="b">
         <v>0</v>
@@ -5516,54 +5574,76 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>768</v>
+        <v>136</v>
       </c>
       <c r="B90" t="s">
-        <v>25</v>
+        <v>126</v>
       </c>
       <c r="C90" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>769</v>
+        <v>144</v>
       </c>
       <c r="B91" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C91" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>770</v>
-      </c>
-      <c r="B92" t="s">
-        <v>25</v>
+        <v>688</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="C92" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>690</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C93" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>771</v>
+        <v>317</v>
       </c>
       <c r="B94" t="s">
+        <v>22</v>
+      </c>
+      <c r="C94" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>112</v>
+      </c>
+      <c r="B95" t="s">
         <v>25</v>
       </c>
-      <c r="C94" t="b">
+      <c r="C95" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>393</v>
+        <v>124</v>
       </c>
       <c r="B96" t="s">
-        <v>120</v>
+        <v>25</v>
       </c>
       <c r="C96" t="b">
         <v>0</v>
@@ -5571,32 +5651,32 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>389</v>
-      </c>
-      <c r="B97" s="11" t="s">
-        <v>108</v>
+        <v>115</v>
+      </c>
+      <c r="B97" t="s">
+        <v>25</v>
       </c>
       <c r="C97" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>401</v>
+        <v>128</v>
       </c>
       <c r="B98" t="s">
         <v>22</v>
       </c>
       <c r="C98" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>397</v>
-      </c>
-      <c r="B99" s="11" t="s">
-        <v>343</v>
+        <v>132</v>
+      </c>
+      <c r="B99" t="s">
+        <v>22</v>
       </c>
       <c r="C99" t="b">
         <v>1</v>
@@ -5604,10 +5684,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>580</v>
+        <v>333</v>
       </c>
       <c r="B100" t="s">
-        <v>120</v>
+        <v>22</v>
       </c>
       <c r="C100" t="b">
         <v>0</v>
@@ -5615,21 +5695,21 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>567</v>
-      </c>
-      <c r="B101" s="11" t="s">
-        <v>108</v>
+        <v>336</v>
+      </c>
+      <c r="B101" t="s">
+        <v>22</v>
       </c>
       <c r="C101" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>585</v>
+        <v>174</v>
       </c>
       <c r="B102" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C102" t="b">
         <v>0</v>
@@ -5637,21 +5717,21 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>583</v>
-      </c>
-      <c r="B103" s="11" t="s">
-        <v>343</v>
+        <v>168</v>
+      </c>
+      <c r="B103" t="s">
+        <v>22</v>
       </c>
       <c r="C103" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>447</v>
+        <v>628</v>
       </c>
       <c r="B104" t="s">
-        <v>120</v>
+        <v>22</v>
       </c>
       <c r="C104" t="b">
         <v>0</v>
@@ -5659,65 +5739,65 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>422</v>
-      </c>
-      <c r="B105" s="11" t="s">
-        <v>108</v>
+        <v>113</v>
+      </c>
+      <c r="B105" t="s">
+        <v>22</v>
       </c>
       <c r="C105" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>451</v>
+        <v>770</v>
       </c>
       <c r="B106" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C106" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>450</v>
-      </c>
-      <c r="B107" s="11" t="s">
-        <v>343</v>
+        <v>66</v>
+      </c>
+      <c r="B107" t="s">
+        <v>25</v>
       </c>
       <c r="C107" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>496</v>
+        <v>819</v>
       </c>
       <c r="B108" t="s">
-        <v>120</v>
+        <v>25</v>
       </c>
       <c r="C108" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>471</v>
-      </c>
-      <c r="B109" s="11" t="s">
-        <v>108</v>
+        <v>694</v>
+      </c>
+      <c r="B109" t="s">
+        <v>22</v>
       </c>
       <c r="C109" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>500</v>
+        <v>73</v>
       </c>
       <c r="B110" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="C110" t="b">
         <v>0</v>
@@ -5725,21 +5805,21 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>499</v>
-      </c>
-      <c r="B111" s="11" t="s">
-        <v>343</v>
+        <v>691</v>
+      </c>
+      <c r="B111" t="s">
+        <v>22</v>
       </c>
       <c r="C111" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>545</v>
+      <c r="A112" s="17" t="s">
+        <v>256</v>
       </c>
       <c r="B112" t="s">
-        <v>120</v>
+        <v>22</v>
       </c>
       <c r="C112" t="b">
         <v>0</v>
@@ -5747,20 +5827,20 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>520</v>
-      </c>
-      <c r="B113" s="11" t="s">
-        <v>108</v>
+        <v>118</v>
+      </c>
+      <c r="B113" t="s">
+        <v>119</v>
       </c>
       <c r="C113" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>549</v>
-      </c>
-      <c r="B114" t="s">
+        <v>593</v>
+      </c>
+      <c r="B114" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C114" t="b">
@@ -5769,18 +5849,18 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>548</v>
-      </c>
-      <c r="B115" s="11" t="s">
-        <v>343</v>
+        <v>597</v>
+      </c>
+      <c r="B115" t="s">
+        <v>72</v>
       </c>
       <c r="C115" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>426</v>
+        <v>41</v>
       </c>
       <c r="B116" t="s">
         <v>120</v>
@@ -5791,21 +5871,21 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>418</v>
-      </c>
-      <c r="B117" s="11" t="s">
-        <v>108</v>
+        <v>617</v>
+      </c>
+      <c r="B117" t="s">
+        <v>120</v>
       </c>
       <c r="C117" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>431</v>
-      </c>
-      <c r="B118" t="s">
-        <v>22</v>
+        <v>615</v>
+      </c>
+      <c r="B118" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="C118" t="b">
         <v>0</v>
@@ -5813,21 +5893,21 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>429</v>
-      </c>
-      <c r="B119" s="11" t="s">
-        <v>343</v>
+        <v>620</v>
+      </c>
+      <c r="B119" t="s">
+        <v>120</v>
       </c>
       <c r="C119" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>475</v>
-      </c>
-      <c r="B120" t="s">
-        <v>120</v>
+        <v>619</v>
+      </c>
+      <c r="B120" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="C120" t="b">
         <v>0</v>
@@ -5835,21 +5915,21 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>467</v>
-      </c>
-      <c r="B121" s="11" t="s">
-        <v>108</v>
+        <v>654</v>
+      </c>
+      <c r="B121" t="s">
+        <v>22</v>
       </c>
       <c r="C121" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>480</v>
-      </c>
-      <c r="B122" t="s">
-        <v>22</v>
+        <v>657</v>
+      </c>
+      <c r="B122" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="C122" t="b">
         <v>0</v>
@@ -5857,43 +5937,43 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>478</v>
-      </c>
-      <c r="B123" s="11" t="s">
-        <v>343</v>
+        <v>123</v>
+      </c>
+      <c r="B123" t="s">
+        <v>22</v>
       </c>
       <c r="C123" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>524</v>
+        <v>769</v>
       </c>
       <c r="B124" t="s">
-        <v>120</v>
+        <v>25</v>
       </c>
       <c r="C124" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>516</v>
-      </c>
-      <c r="B125" s="11" t="s">
-        <v>108</v>
+        <v>385</v>
+      </c>
+      <c r="B125" t="s">
+        <v>22</v>
       </c>
       <c r="C125" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>529</v>
+        <v>447</v>
       </c>
       <c r="B126" t="s">
-        <v>22</v>
+        <v>120</v>
       </c>
       <c r="C126" t="b">
         <v>0</v>
@@ -5901,10 +5981,10 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>527</v>
+        <v>422</v>
       </c>
       <c r="B127" s="11" t="s">
-        <v>343</v>
+        <v>108</v>
       </c>
       <c r="C127" t="b">
         <v>1</v>
@@ -5912,10 +5992,10 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>437</v>
+        <v>451</v>
       </c>
       <c r="B128" t="s">
-        <v>120</v>
+        <v>22</v>
       </c>
       <c r="C128" t="b">
         <v>0</v>
@@ -5923,10 +6003,10 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>420</v>
+        <v>450</v>
       </c>
       <c r="B129" s="11" t="s">
-        <v>108</v>
+        <v>343</v>
       </c>
       <c r="C129" t="b">
         <v>1</v>
@@ -5934,10 +6014,10 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>441</v>
+        <v>496</v>
       </c>
       <c r="B130" t="s">
-        <v>22</v>
+        <v>120</v>
       </c>
       <c r="C130" t="b">
         <v>0</v>
@@ -5945,10 +6025,10 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>440</v>
+        <v>471</v>
       </c>
       <c r="B131" s="11" t="s">
-        <v>343</v>
+        <v>108</v>
       </c>
       <c r="C131" t="b">
         <v>1</v>
@@ -5956,10 +6036,10 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>486</v>
+        <v>500</v>
       </c>
       <c r="B132" t="s">
-        <v>120</v>
+        <v>22</v>
       </c>
       <c r="C132" t="b">
         <v>0</v>
@@ -5967,10 +6047,10 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>469</v>
+        <v>499</v>
       </c>
       <c r="B133" s="11" t="s">
-        <v>108</v>
+        <v>343</v>
       </c>
       <c r="C133" t="b">
         <v>1</v>
@@ -5978,10 +6058,10 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>490</v>
+        <v>545</v>
       </c>
       <c r="B134" t="s">
-        <v>22</v>
+        <v>120</v>
       </c>
       <c r="C134" t="b">
         <v>0</v>
@@ -5989,10 +6069,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>489</v>
+        <v>520</v>
       </c>
       <c r="B135" s="11" t="s">
-        <v>343</v>
+        <v>108</v>
       </c>
       <c r="C135" t="b">
         <v>1</v>
@@ -6000,10 +6080,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>535</v>
+        <v>549</v>
       </c>
       <c r="B136" t="s">
-        <v>120</v>
+        <v>22</v>
       </c>
       <c r="C136" t="b">
         <v>0</v>
@@ -6011,10 +6091,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>518</v>
+        <v>548</v>
       </c>
       <c r="B137" s="11" t="s">
-        <v>108</v>
+        <v>343</v>
       </c>
       <c r="C137" t="b">
         <v>1</v>
@@ -6022,10 +6102,10 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>539</v>
+        <v>607</v>
       </c>
       <c r="B138" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C138" t="b">
         <v>0</v>
@@ -6033,18 +6113,18 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>538</v>
-      </c>
-      <c r="B139" s="11" t="s">
-        <v>343</v>
+        <v>605</v>
+      </c>
+      <c r="B139" t="s">
+        <v>22</v>
       </c>
       <c r="C139" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>407</v>
+        <v>426</v>
       </c>
       <c r="B140" t="s">
         <v>120</v>
@@ -6055,7 +6135,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>391</v>
+        <v>418</v>
       </c>
       <c r="B141" s="11" t="s">
         <v>108</v>
@@ -6066,7 +6146,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>412</v>
+        <v>431</v>
       </c>
       <c r="B142" t="s">
         <v>22</v>
@@ -6077,7 +6157,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>410</v>
+        <v>429</v>
       </c>
       <c r="B143" s="11" t="s">
         <v>343</v>
@@ -6088,7 +6168,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>457</v>
+        <v>475</v>
       </c>
       <c r="B144" t="s">
         <v>120</v>
@@ -6099,7 +6179,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>424</v>
+        <v>467</v>
       </c>
       <c r="B145" s="11" t="s">
         <v>108</v>
@@ -6110,7 +6190,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>461</v>
+        <v>480</v>
       </c>
       <c r="B146" t="s">
         <v>22</v>
@@ -6121,7 +6201,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>460</v>
+        <v>478</v>
       </c>
       <c r="B147" s="11" t="s">
         <v>343</v>
@@ -6132,7 +6212,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>506</v>
+        <v>524</v>
       </c>
       <c r="B148" t="s">
         <v>120</v>
@@ -6143,7 +6223,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>473</v>
+        <v>516</v>
       </c>
       <c r="B149" s="11" t="s">
         <v>108</v>
@@ -6154,7 +6234,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>510</v>
+        <v>529</v>
       </c>
       <c r="B150" t="s">
         <v>22</v>
@@ -6165,7 +6245,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>509</v>
+        <v>527</v>
       </c>
       <c r="B151" s="11" t="s">
         <v>343</v>
@@ -6176,10 +6256,10 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>569</v>
+        <v>602</v>
       </c>
       <c r="B152" t="s">
-        <v>120</v>
+        <v>22</v>
       </c>
       <c r="C152" t="b">
         <v>0</v>
@@ -6187,87 +6267,98 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>565</v>
-      </c>
-      <c r="B153" s="11" t="s">
-        <v>108</v>
+        <v>437</v>
+      </c>
+      <c r="B153" t="s">
+        <v>120</v>
       </c>
       <c r="C153" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>574</v>
-      </c>
-      <c r="B154" t="s">
-        <v>22</v>
+        <v>420</v>
+      </c>
+      <c r="B154" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="C154" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>572</v>
-      </c>
-      <c r="B155" s="11" t="s">
-        <v>343</v>
+        <v>441</v>
+      </c>
+      <c r="B155" t="s">
+        <v>22</v>
       </c>
       <c r="C155" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>555</v>
-      </c>
-      <c r="B156" t="s">
-        <v>120</v>
+        <v>440</v>
+      </c>
+      <c r="B156" s="11" t="s">
+        <v>343</v>
       </c>
       <c r="C156" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>522</v>
-      </c>
-      <c r="B157" s="11" t="s">
-        <v>108</v>
+        <v>486</v>
+      </c>
+      <c r="B157" t="s">
+        <v>120</v>
       </c>
       <c r="C157" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>559</v>
-      </c>
-      <c r="B158" t="s">
-        <v>22</v>
+        <v>469</v>
+      </c>
+      <c r="B158" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="C158" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>558</v>
-      </c>
-      <c r="B159" s="11" t="s">
+        <v>490</v>
+      </c>
+      <c r="B159" t="s">
+        <v>22</v>
+      </c>
+      <c r="C159" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>489</v>
+      </c>
+      <c r="B160" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="C159" t="b">
+      <c r="C160" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>630</v>
+        <v>535</v>
       </c>
       <c r="B161" t="s">
-        <v>22</v>
+        <v>120</v>
       </c>
       <c r="C161" t="b">
         <v>0</v>
@@ -6275,18 +6366,18 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>633</v>
-      </c>
-      <c r="B162" s="6" t="s">
-        <v>72</v>
+        <v>518</v>
+      </c>
+      <c r="B162" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="C162" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>715</v>
+        <v>539</v>
       </c>
       <c r="B163" t="s">
         <v>22</v>
@@ -6297,21 +6388,21 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>720</v>
-      </c>
-      <c r="B164" t="s">
-        <v>25</v>
+        <v>538</v>
+      </c>
+      <c r="B164" s="11" t="s">
+        <v>343</v>
       </c>
       <c r="C164" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>718</v>
-      </c>
-      <c r="B165" s="6" t="s">
-        <v>72</v>
+        <v>407</v>
+      </c>
+      <c r="B165" t="s">
+        <v>120</v>
       </c>
       <c r="C165" t="b">
         <v>0</v>
@@ -6319,18 +6410,18 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>621</v>
-      </c>
-      <c r="B166" t="s">
-        <v>22</v>
+        <v>391</v>
+      </c>
+      <c r="B166" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="C166" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>704</v>
+        <v>782</v>
       </c>
       <c r="B167" t="s">
         <v>22</v>
@@ -6341,10 +6432,10 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>702</v>
-      </c>
-      <c r="B168" s="6" t="s">
-        <v>72</v>
+        <v>412</v>
+      </c>
+      <c r="B168" t="s">
+        <v>22</v>
       </c>
       <c r="C168" t="b">
         <v>0</v>
@@ -6352,21 +6443,21 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>706</v>
-      </c>
-      <c r="B169" t="s">
-        <v>22</v>
+        <v>410</v>
+      </c>
+      <c r="B169" s="11" t="s">
+        <v>343</v>
       </c>
       <c r="C169" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="B170" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C170" t="b">
         <v>0</v>
@@ -6374,7 +6465,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>700</v>
+        <v>307</v>
       </c>
       <c r="B171" t="s">
         <v>22</v>
@@ -6385,7 +6476,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>665</v>
+        <v>309</v>
       </c>
       <c r="B172" t="s">
         <v>22</v>
@@ -6396,9 +6487,9 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>668</v>
-      </c>
-      <c r="B173" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B173" t="s">
         <v>72</v>
       </c>
       <c r="C173" t="b">
@@ -6407,7 +6498,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>708</v>
+        <v>265</v>
       </c>
       <c r="B174" t="s">
         <v>22</v>
@@ -6418,10 +6509,10 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>635</v>
-      </c>
-      <c r="B175" t="s">
-        <v>22</v>
+        <v>679</v>
+      </c>
+      <c r="B175" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="C175" t="b">
         <v>0</v>
@@ -6429,10 +6520,10 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>638</v>
-      </c>
-      <c r="B176" s="6" t="s">
-        <v>72</v>
+        <v>164</v>
+      </c>
+      <c r="B176" t="s">
+        <v>25</v>
       </c>
       <c r="C176" t="b">
         <v>0</v>
@@ -6440,10 +6531,10 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>710</v>
+        <v>163</v>
       </c>
       <c r="B177" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C177" t="b">
         <v>0</v>
@@ -6451,10 +6542,10 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>713</v>
+        <v>52</v>
       </c>
       <c r="B178" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="C178" t="b">
         <v>0</v>
@@ -6462,10 +6553,10 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>675</v>
-      </c>
-      <c r="B179" t="s">
-        <v>22</v>
+        <v>48</v>
+      </c>
+      <c r="B179" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="C179" t="b">
         <v>0</v>
@@ -6473,9 +6564,9 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>686</v>
-      </c>
-      <c r="B180" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B180" t="s">
         <v>72</v>
       </c>
       <c r="C180" t="b">
@@ -6484,10 +6575,10 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>682</v>
+        <v>89</v>
       </c>
       <c r="B181" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="C181" t="b">
         <v>0</v>
@@ -6495,7 +6586,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>646</v>
+        <v>659</v>
       </c>
       <c r="B182" t="s">
         <v>22</v>
@@ -6506,7 +6597,7 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>650</v>
+        <v>663</v>
       </c>
       <c r="B183" s="6" t="s">
         <v>72</v>
@@ -6517,10 +6608,10 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>652</v>
-      </c>
-      <c r="B184" s="6" t="s">
-        <v>72</v>
+        <v>457</v>
+      </c>
+      <c r="B184" t="s">
+        <v>120</v>
       </c>
       <c r="C184" t="b">
         <v>0</v>
@@ -6528,18 +6619,18 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>697</v>
-      </c>
-      <c r="B185" t="s">
-        <v>25</v>
+        <v>424</v>
+      </c>
+      <c r="B185" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="C185" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>623</v>
+        <v>461</v>
       </c>
       <c r="B186" t="s">
         <v>22</v>
@@ -6550,21 +6641,21 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>626</v>
-      </c>
-      <c r="B187" t="s">
-        <v>22</v>
+        <v>460</v>
+      </c>
+      <c r="B187" s="11" t="s">
+        <v>343</v>
       </c>
       <c r="C187" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>609</v>
+        <v>506</v>
       </c>
       <c r="B188" t="s">
-        <v>22</v>
+        <v>120</v>
       </c>
       <c r="C188" t="b">
         <v>0</v>
@@ -6572,21 +6663,21 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>640</v>
-      </c>
-      <c r="B189" t="s">
-        <v>22</v>
+        <v>473</v>
+      </c>
+      <c r="B189" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="C189" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>644</v>
-      </c>
-      <c r="B190" s="6" t="s">
-        <v>72</v>
+        <v>510</v>
+      </c>
+      <c r="B190" t="s">
+        <v>22</v>
       </c>
       <c r="C190" t="b">
         <v>0</v>
@@ -6594,21 +6685,21 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>688</v>
-      </c>
-      <c r="B191" s="6" t="s">
-        <v>72</v>
+        <v>509</v>
+      </c>
+      <c r="B191" s="11" t="s">
+        <v>343</v>
       </c>
       <c r="C191" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>690</v>
-      </c>
-      <c r="B192" s="6" t="s">
-        <v>72</v>
+        <v>611</v>
+      </c>
+      <c r="B192" t="s">
+        <v>22</v>
       </c>
       <c r="C192" t="b">
         <v>0</v>
@@ -6616,10 +6707,10 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>628</v>
+        <v>569</v>
       </c>
       <c r="B193" t="s">
-        <v>22</v>
+        <v>120</v>
       </c>
       <c r="C193" t="b">
         <v>0</v>
@@ -6627,18 +6718,18 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>694</v>
-      </c>
-      <c r="B194" t="s">
-        <v>22</v>
+        <v>565</v>
+      </c>
+      <c r="B194" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="C194" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>691</v>
+        <v>574</v>
       </c>
       <c r="B195" t="s">
         <v>22</v>
@@ -6649,21 +6740,21 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>593</v>
-      </c>
-      <c r="B196" s="6" t="s">
-        <v>22</v>
+        <v>572</v>
+      </c>
+      <c r="B196" s="11" t="s">
+        <v>343</v>
       </c>
       <c r="C196" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>597</v>
+        <v>613</v>
       </c>
       <c r="B197" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="C197" t="b">
         <v>0</v>
@@ -6671,10 +6762,10 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>617</v>
+        <v>77</v>
       </c>
       <c r="B198" t="s">
-        <v>120</v>
+        <v>22</v>
       </c>
       <c r="C198" t="b">
         <v>0</v>
@@ -6682,10 +6773,10 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>615</v>
-      </c>
-      <c r="B199" s="6" t="s">
-        <v>72</v>
+        <v>55</v>
+      </c>
+      <c r="B199" t="s">
+        <v>50</v>
       </c>
       <c r="C199" t="b">
         <v>0</v>
@@ -6693,10 +6784,10 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>620</v>
+        <v>165</v>
       </c>
       <c r="B200" t="s">
-        <v>120</v>
+        <v>22</v>
       </c>
       <c r="C200" t="b">
         <v>0</v>
@@ -6704,10 +6795,10 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>619</v>
-      </c>
-      <c r="B201" s="6" t="s">
-        <v>72</v>
+        <v>299</v>
+      </c>
+      <c r="B201" t="s">
+        <v>22</v>
       </c>
       <c r="C201" t="b">
         <v>0</v>
@@ -6715,7 +6806,7 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>654</v>
+        <v>304</v>
       </c>
       <c r="B202" t="s">
         <v>22</v>
@@ -6726,10 +6817,10 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>657</v>
-      </c>
-      <c r="B203" s="6" t="s">
-        <v>72</v>
+        <v>295</v>
+      </c>
+      <c r="B203" t="s">
+        <v>22</v>
       </c>
       <c r="C203" t="b">
         <v>0</v>
@@ -6737,10 +6828,10 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>607</v>
+        <v>670</v>
       </c>
       <c r="B204" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C204" t="b">
         <v>0</v>
@@ -6748,10 +6839,10 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>605</v>
-      </c>
-      <c r="B205" t="s">
-        <v>22</v>
+        <v>673</v>
+      </c>
+      <c r="B205" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="C205" t="b">
         <v>0</v>
@@ -6759,10 +6850,10 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>602</v>
+        <v>147</v>
       </c>
       <c r="B206" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C206" t="b">
         <v>0</v>
@@ -6770,10 +6861,10 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>782</v>
+        <v>772</v>
       </c>
       <c r="B207" t="s">
-        <v>22</v>
+        <v>120</v>
       </c>
       <c r="C207" t="b">
         <v>0</v>
@@ -6781,10 +6872,10 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>603</v>
+        <v>773</v>
       </c>
       <c r="B208" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="C208" t="b">
         <v>0</v>
@@ -6792,10 +6883,10 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>679</v>
-      </c>
-      <c r="B209" s="6" t="s">
-        <v>72</v>
+        <v>555</v>
+      </c>
+      <c r="B209" t="s">
+        <v>120</v>
       </c>
       <c r="C209" t="b">
         <v>0</v>
@@ -6803,21 +6894,21 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>659</v>
-      </c>
-      <c r="B210" t="s">
-        <v>22</v>
+        <v>522</v>
+      </c>
+      <c r="B210" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="C210" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>663</v>
-      </c>
-      <c r="B211" s="6" t="s">
-        <v>72</v>
+        <v>559</v>
+      </c>
+      <c r="B211" t="s">
+        <v>22</v>
       </c>
       <c r="C211" t="b">
         <v>0</v>
@@ -6825,106 +6916,29 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>611</v>
-      </c>
-      <c r="B212" t="s">
-        <v>22</v>
+        <v>558</v>
+      </c>
+      <c r="B212" s="11" t="s">
+        <v>343</v>
       </c>
       <c r="C212" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
-        <v>613</v>
-      </c>
-      <c r="B213" t="s">
-        <v>25</v>
-      </c>
-      <c r="C213" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>670</v>
+        <v>822</v>
       </c>
       <c r="B214" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C214" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
-        <v>673</v>
-      </c>
-      <c r="B215" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C215" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
-        <v>772</v>
-      </c>
-      <c r="B217" t="s">
-        <v>120</v>
-      </c>
-      <c r="C217" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
-        <v>773</v>
-      </c>
-      <c r="B218" t="s">
-        <v>72</v>
-      </c>
-      <c r="C218" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
-        <v>819</v>
-      </c>
-      <c r="B220" t="s">
-        <v>25</v>
-      </c>
-      <c r="C220" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
-        <v>820</v>
-      </c>
-      <c r="B221" t="s">
-        <v>25</v>
-      </c>
-      <c r="C221" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
-        <v>821</v>
-      </c>
-      <c r="B222" t="s">
-        <v>25</v>
-      </c>
-      <c r="C222" t="b">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A20:C36">
-    <sortCondition ref="A20"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C222">
+    <sortCondition ref="A90"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7023,7 +7037,7 @@
   <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
@@ -8065,7 +8079,7 @@
   <dimension ref="A1:M169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H50" sqref="D50:H50"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
NAME -> NOME CRI
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
+++ b/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1C83B7-2338-4023-8F00-7828A7E45385}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0316E5-D6F1-44D5-9FAF-2E59597B0A30}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2595" uniqueCount="823">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2595" uniqueCount="824">
   <si>
     <t>setting_name</t>
   </si>
@@ -2516,6 +2516,9 @@
   </si>
   <si>
     <t>ESTADO</t>
+  </si>
+  <si>
+    <t>NOME</t>
   </si>
 </sst>
 </file>
@@ -4581,9 +4584,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
   <dimension ref="A1:C214"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A198" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C214" sqref="C214"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5794,7 +5797,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>73</v>
+        <v>823</v>
       </c>
       <c r="B110" t="s">
         <v>72</v>
@@ -7036,9 +7039,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7151,7 +7154,7 @@
         <v>72</v>
       </c>
       <c r="F8" t="s">
-        <v>73</v>
+        <v>823</v>
       </c>
       <c r="G8" t="s">
         <v>74</v>

</xml_diff>

<commit_message>
Added Assistant to CRIANCA + assistant: int -> string
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
+++ b/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2FCAC3-6234-4DBA-B4BC-E1E13B8EB526}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7ABD0F-6198-4F7E-B849-8A11E7B36DE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2715" uniqueCount="872">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2720" uniqueCount="875">
   <si>
     <t>setting_name</t>
   </si>
@@ -2665,6 +2665,15 @@
   </si>
   <si>
     <t>integer_dropdown</t>
+  </si>
+  <si>
+    <t>ASSISTENTE</t>
+  </si>
+  <si>
+    <t>Name: {{data.ASSISTENTE}}</t>
+  </si>
+  <si>
+    <t>Nome: {{data.ASSISTENTE}}</t>
   </si>
 </sst>
 </file>
@@ -5441,11 +5450,11 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
-  <dimension ref="A1:C218"/>
+  <dimension ref="A1:C220"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A198" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G211" sqref="G211"/>
+      <selection pane="bottomLeft" activeCell="C221" sqref="A221:C221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7840,6 +7849,17 @@
       </c>
       <c r="C218" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>872</v>
+      </c>
+      <c r="B220" t="s">
+        <v>72</v>
+      </c>
+      <c r="C220" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -7940,10 +7960,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31E2D9B7-AFA3-430F-905F-12902E548477}">
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8016,93 +8036,93 @@
         <v>149</v>
       </c>
       <c r="G4" t="s">
+        <v>873</v>
+      </c>
+      <c r="H4" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>149</v>
+      </c>
+      <c r="G5" t="s">
         <v>826</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H5" t="s">
         <v>827</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>88</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>830</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
         <v>149</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G7" t="s">
         <v>833</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H7" t="s">
         <v>834</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>88</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>831</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
         <v>149</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G10" t="s">
         <v>836</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H10" t="s">
         <v>837</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>88</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>832</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
         <v>149</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G13" t="s">
         <v>838</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H13" t="s">
         <v>839</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
-        <v>149</v>
-      </c>
-      <c r="G14" t="s">
-        <v>849</v>
-      </c>
-      <c r="H14" t="s">
-        <v>851</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -8110,10 +8130,10 @@
         <v>149</v>
       </c>
       <c r="G15" t="s">
-        <v>835</v>
+        <v>849</v>
       </c>
       <c r="H15" t="s">
-        <v>835</v>
+        <v>851</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -8121,10 +8141,10 @@
         <v>149</v>
       </c>
       <c r="G16" t="s">
-        <v>828</v>
+        <v>835</v>
       </c>
       <c r="H16" t="s">
-        <v>828</v>
+        <v>835</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -8132,119 +8152,116 @@
         <v>149</v>
       </c>
       <c r="G17" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="H17" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
+        <v>149</v>
+      </c>
+      <c r="G18" t="s">
+        <v>829</v>
+      </c>
+      <c r="H18" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
         <v>22</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E19" t="s">
         <v>752</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F19" t="s">
         <v>818</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G19" t="s">
         <v>870</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H19" t="s">
         <v>870</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" t="s">
         <v>88</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>820</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F22" t="s">
-        <v>817</v>
-      </c>
-      <c r="G22" t="s">
-        <v>74</v>
-      </c>
-      <c r="H22" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>120</v>
+        <v>72</v>
       </c>
       <c r="F23" t="s">
-        <v>41</v>
+        <v>817</v>
       </c>
       <c r="G23" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="H23" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" t="s">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="F24" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="G24" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="H24" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>72</v>
+        <v>22</v>
+      </c>
+      <c r="E25" t="s">
+        <v>76</v>
       </c>
       <c r="F25" t="s">
-        <v>118</v>
+        <v>77</v>
       </c>
       <c r="G25" t="s">
-        <v>848</v>
+        <v>84</v>
       </c>
       <c r="H25" t="s">
-        <v>850</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="F26" t="s">
-        <v>66</v>
+        <v>118</v>
       </c>
       <c r="G26" t="s">
-        <v>67</v>
+        <v>848</v>
       </c>
       <c r="H26" t="s">
-        <v>67</v>
+        <v>850</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -8252,13 +8269,13 @@
         <v>25</v>
       </c>
       <c r="F27" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -8266,34 +8283,37 @@
         <v>25</v>
       </c>
       <c r="F28" t="s">
+        <v>68</v>
+      </c>
+      <c r="G28" t="s">
+        <v>69</v>
+      </c>
+      <c r="H28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" t="s">
         <v>70</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G29" t="s">
         <v>71</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H29" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D31" t="s">
-        <v>149</v>
-      </c>
-      <c r="G31" t="s">
-        <v>824</v>
-      </c>
-      <c r="H31" t="s">
-        <v>825</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -8301,10 +8321,10 @@
         <v>149</v>
       </c>
       <c r="G32" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="H32" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -8312,10 +8332,10 @@
         <v>149</v>
       </c>
       <c r="G33" t="s">
-        <v>822</v>
+        <v>826</v>
       </c>
       <c r="H33" t="s">
-        <v>823</v>
+        <v>827</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -8323,10 +8343,10 @@
         <v>149</v>
       </c>
       <c r="G34" t="s">
-        <v>849</v>
+        <v>822</v>
       </c>
       <c r="H34" t="s">
-        <v>851</v>
+        <v>823</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -8334,10 +8354,10 @@
         <v>149</v>
       </c>
       <c r="G35" t="s">
-        <v>835</v>
+        <v>849</v>
       </c>
       <c r="H35" t="s">
-        <v>835</v>
+        <v>851</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -8345,10 +8365,10 @@
         <v>149</v>
       </c>
       <c r="G36" t="s">
-        <v>828</v>
+        <v>835</v>
       </c>
       <c r="H36" t="s">
-        <v>828</v>
+        <v>835</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -8356,25 +8376,36 @@
         <v>149</v>
       </c>
       <c r="G37" t="s">
+        <v>828</v>
+      </c>
+      <c r="H37" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>149</v>
+      </c>
+      <c r="G38" t="s">
         <v>829</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H38" t="s">
         <v>829</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
         <v>260</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Assistant to GRAVIDA_VISIT
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
+++ b/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB188F39-6828-47A2-A548-43C912E134BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486FDD33-FAA9-4B8C-9748-D6A52D442779}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2471" uniqueCount="823">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2468" uniqueCount="821">
   <si>
     <t>setting_name</t>
   </si>
@@ -2368,12 +2368,6 @@
   </si>
   <si>
     <t>ASSISTENTE</t>
-  </si>
-  <si>
-    <t>Name: {{data.ASSISTENTE}}</t>
-  </si>
-  <si>
-    <t>Nome: {{data.ASSISTENTE}}</t>
   </si>
   <si>
     <t>data('BCG') == null</t>
@@ -3248,9 +3242,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB23FD29-3338-4879-B1BD-848935333D8A}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8:XFD24"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7135,10 +7129,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31E2D9B7-AFA3-430F-905F-12902E548477}">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7211,93 +7205,93 @@
         <v>149</v>
       </c>
       <c r="G4" t="s">
-        <v>773</v>
+        <v>726</v>
       </c>
       <c r="H4" t="s">
-        <v>774</v>
+        <v>727</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
+      <c r="B5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
         <v>149</v>
       </c>
-      <c r="G5" t="s">
-        <v>726</v>
-      </c>
-      <c r="H5" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" t="s">
-        <v>730</v>
+      <c r="G6" t="s">
+        <v>733</v>
+      </c>
+      <c r="H6" t="s">
+        <v>734</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
-        <v>149</v>
-      </c>
-      <c r="G7" t="s">
-        <v>733</v>
-      </c>
-      <c r="H7" t="s">
-        <v>734</v>
+      <c r="B7" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>149</v>
+      </c>
+      <c r="G9" t="s">
+        <v>736</v>
+      </c>
+      <c r="H9" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>88</v>
-      </c>
-      <c r="C9" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
-        <v>149</v>
-      </c>
-      <c r="G10" t="s">
-        <v>736</v>
-      </c>
-      <c r="H10" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>149</v>
+      </c>
+      <c r="G12" t="s">
+        <v>738</v>
+      </c>
+      <c r="H12" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>88</v>
-      </c>
-      <c r="C12" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
         <v>149</v>
       </c>
-      <c r="G13" t="s">
-        <v>738</v>
-      </c>
-      <c r="H13" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>103</v>
+      <c r="G14" t="s">
+        <v>749</v>
+      </c>
+      <c r="H14" t="s">
+        <v>751</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -7305,10 +7299,10 @@
         <v>149</v>
       </c>
       <c r="G15" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="H15" t="s">
-        <v>751</v>
+        <v>735</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -7316,10 +7310,10 @@
         <v>149</v>
       </c>
       <c r="G16" t="s">
-        <v>735</v>
+        <v>728</v>
       </c>
       <c r="H16" t="s">
-        <v>735</v>
+        <v>728</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -7327,116 +7321,119 @@
         <v>149</v>
       </c>
       <c r="G17" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="H17" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>149</v>
+        <v>22</v>
+      </c>
+      <c r="E18" t="s">
+        <v>655</v>
+      </c>
+      <c r="F18" t="s">
+        <v>718</v>
       </c>
       <c r="G18" t="s">
-        <v>729</v>
+        <v>770</v>
       </c>
       <c r="H18" t="s">
-        <v>729</v>
+        <v>770</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" t="s">
-        <v>655</v>
-      </c>
-      <c r="F19" t="s">
-        <v>718</v>
-      </c>
-      <c r="G19" t="s">
-        <v>770</v>
-      </c>
-      <c r="H19" t="s">
-        <v>770</v>
+      <c r="B19" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>88</v>
+      </c>
+      <c r="C20" t="s">
+        <v>720</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
       <c r="B21" t="s">
-        <v>88</v>
-      </c>
-      <c r="C21" t="s">
-        <v>720</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>46</v>
+      <c r="D22" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" t="s">
+        <v>717</v>
+      </c>
+      <c r="G22" t="s">
+        <v>74</v>
+      </c>
+      <c r="H22" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>72</v>
+        <v>120</v>
       </c>
       <c r="F23" t="s">
-        <v>717</v>
+        <v>41</v>
       </c>
       <c r="G23" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="H23" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>120</v>
+        <v>22</v>
+      </c>
+      <c r="E24" t="s">
+        <v>76</v>
       </c>
       <c r="F24" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="G24" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>22</v>
-      </c>
-      <c r="E25" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F25" t="s">
-        <v>77</v>
+        <v>118</v>
       </c>
       <c r="G25" t="s">
-        <v>84</v>
+        <v>748</v>
       </c>
       <c r="H25" t="s">
-        <v>85</v>
+        <v>750</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="F26" t="s">
-        <v>118</v>
+        <v>66</v>
       </c>
       <c r="G26" t="s">
-        <v>748</v>
+        <v>67</v>
       </c>
       <c r="H26" t="s">
-        <v>750</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -7444,13 +7441,13 @@
         <v>25</v>
       </c>
       <c r="F27" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G27" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H27" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -7458,37 +7455,34 @@
         <v>25</v>
       </c>
       <c r="F28" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G28" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H28" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D29" t="s">
-        <v>25</v>
-      </c>
-      <c r="F29" t="s">
-        <v>70</v>
-      </c>
-      <c r="G29" t="s">
-        <v>71</v>
-      </c>
-      <c r="H29" t="s">
-        <v>71</v>
+      <c r="B29" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>46</v>
+      <c r="D31" t="s">
+        <v>149</v>
+      </c>
+      <c r="G31" t="s">
+        <v>724</v>
+      </c>
+      <c r="H31" t="s">
+        <v>725</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -7496,10 +7490,10 @@
         <v>149</v>
       </c>
       <c r="G32" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="H32" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -7507,10 +7501,10 @@
         <v>149</v>
       </c>
       <c r="G33" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="H33" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -7518,10 +7512,10 @@
         <v>149</v>
       </c>
       <c r="G34" t="s">
-        <v>722</v>
+        <v>749</v>
       </c>
       <c r="H34" t="s">
-        <v>723</v>
+        <v>751</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -7529,10 +7523,10 @@
         <v>149</v>
       </c>
       <c r="G35" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="H35" t="s">
-        <v>751</v>
+        <v>735</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -7540,10 +7534,10 @@
         <v>149</v>
       </c>
       <c r="G36" t="s">
-        <v>735</v>
+        <v>728</v>
       </c>
       <c r="H36" t="s">
-        <v>735</v>
+        <v>728</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -7551,36 +7545,25 @@
         <v>149</v>
       </c>
       <c r="G37" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="H37" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D38" t="s">
-        <v>149</v>
-      </c>
-      <c r="G38" t="s">
-        <v>729</v>
-      </c>
-      <c r="H38" t="s">
-        <v>729</v>
+      <c r="B38" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
       <c r="B39" t="s">
-        <v>47</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
       <c r="B40" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
         <v>260</v>
       </c>
     </row>
@@ -11039,7 +11022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A7F4833-88F1-44B1-8A75-76AFCBB7BC62}">
   <dimension ref="A1:J230"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
     </sheetView>
@@ -11100,7 +11083,7 @@
         <v>88</v>
       </c>
       <c r="C3" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -11168,10 +11151,10 @@
         <v>390</v>
       </c>
       <c r="G10" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="H10" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -11205,7 +11188,7 @@
         <v>88</v>
       </c>
       <c r="C15" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -11273,10 +11256,10 @@
         <v>397</v>
       </c>
       <c r="G22" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="H22" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
@@ -11320,7 +11303,7 @@
         <v>88</v>
       </c>
       <c r="C29" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
@@ -11388,10 +11371,10 @@
         <v>404</v>
       </c>
       <c r="G36" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="H36" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
@@ -11425,7 +11408,7 @@
         <v>88</v>
       </c>
       <c r="C41" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
@@ -11517,10 +11500,10 @@
         <v>410</v>
       </c>
       <c r="G51" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="H51" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
@@ -11554,7 +11537,7 @@
         <v>88</v>
       </c>
       <c r="C56" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
@@ -11646,10 +11629,10 @@
         <v>416</v>
       </c>
       <c r="G66" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="H66" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.25">
@@ -11683,7 +11666,7 @@
         <v>88</v>
       </c>
       <c r="C71" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.25">
@@ -11775,10 +11758,10 @@
         <v>422</v>
       </c>
       <c r="G81" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="H81" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.25">
@@ -11822,7 +11805,7 @@
         <v>88</v>
       </c>
       <c r="C88" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
@@ -11890,10 +11873,10 @@
         <v>429</v>
       </c>
       <c r="G95" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="H95" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
@@ -11927,7 +11910,7 @@
         <v>88</v>
       </c>
       <c r="C100" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.25">
@@ -12019,10 +12002,10 @@
         <v>435</v>
       </c>
       <c r="G110" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="H110" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
     </row>
     <row r="111" spans="2:9" x14ac:dyDescent="0.25">
@@ -12056,7 +12039,7 @@
         <v>88</v>
       </c>
       <c r="C115" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.25">
@@ -12148,10 +12131,10 @@
         <v>441</v>
       </c>
       <c r="G125" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="H125" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
     </row>
     <row r="126" spans="2:9" x14ac:dyDescent="0.25">
@@ -12185,7 +12168,7 @@
         <v>88</v>
       </c>
       <c r="C130" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
     </row>
     <row r="131" spans="2:9" x14ac:dyDescent="0.25">
@@ -12277,10 +12260,10 @@
         <v>447</v>
       </c>
       <c r="G140" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="H140" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
     </row>
     <row r="141" spans="2:9" x14ac:dyDescent="0.25">
@@ -12324,7 +12307,7 @@
         <v>88</v>
       </c>
       <c r="C147" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
     </row>
     <row r="148" spans="2:9" x14ac:dyDescent="0.25">
@@ -12392,10 +12375,10 @@
         <v>454</v>
       </c>
       <c r="G154" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="H154" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
     </row>
     <row r="155" spans="2:9" x14ac:dyDescent="0.25">
@@ -12429,7 +12412,7 @@
         <v>88</v>
       </c>
       <c r="C159" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
     </row>
     <row r="160" spans="2:9" x14ac:dyDescent="0.25">
@@ -12521,10 +12504,10 @@
         <v>460</v>
       </c>
       <c r="G169" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="H169" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
     </row>
     <row r="170" spans="2:9" x14ac:dyDescent="0.25">
@@ -12558,7 +12541,7 @@
         <v>88</v>
       </c>
       <c r="C174" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
     </row>
     <row r="175" spans="2:9" x14ac:dyDescent="0.25">
@@ -12650,10 +12633,10 @@
         <v>466</v>
       </c>
       <c r="G184" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="H184" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
     </row>
     <row r="185" spans="2:9" x14ac:dyDescent="0.25">
@@ -12687,7 +12670,7 @@
         <v>88</v>
       </c>
       <c r="C189" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="190" spans="2:9" x14ac:dyDescent="0.25">
@@ -12779,10 +12762,10 @@
         <v>472</v>
       </c>
       <c r="G199" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="H199" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
     </row>
     <row r="200" spans="2:9" x14ac:dyDescent="0.25">
@@ -12826,7 +12809,7 @@
         <v>88</v>
       </c>
       <c r="C206" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
     </row>
     <row r="207" spans="2:9" x14ac:dyDescent="0.25">
@@ -12894,10 +12877,10 @@
         <v>479</v>
       </c>
       <c r="G213" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="H213" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
     </row>
     <row r="214" spans="2:9" x14ac:dyDescent="0.25">
@@ -12931,7 +12914,7 @@
         <v>88</v>
       </c>
       <c r="C218" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
     </row>
     <row r="219" spans="2:9" x14ac:dyDescent="0.25">
@@ -12999,10 +12982,10 @@
         <v>486</v>
       </c>
       <c r="G225" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="H225" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
     </row>
     <row r="226" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update to skip pattern when reg. new child/mif
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
+++ b/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5E7ED8-23D6-4A8E-A9CB-9F31FFF64285}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51690BB-04CF-418D-95CC-16FA69A140EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="674" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="674" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2787" uniqueCount="1133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2788" uniqueCount="1132">
   <si>
     <t>setting_name</t>
   </si>
@@ -2149,9 +2149,6 @@
     <t>data('vping') == '2'</t>
   </si>
   <si>
-    <t>data('REGID') != null</t>
-  </si>
-  <si>
     <t>data('MOMA') == '1'</t>
   </si>
   <si>
@@ -2188,9 +2185,6 @@
     <t>data('change') == '1'</t>
   </si>
   <si>
-    <t>data('NOME') == null</t>
-  </si>
-  <si>
     <t>Sex: {{data.SEX}}</t>
   </si>
   <si>
@@ -2845,9 +2839,6 @@
     <t>Sexo: Feminino</t>
   </si>
   <si>
-    <t>Quer mudar?</t>
-  </si>
-  <si>
     <t>Fogão</t>
   </si>
   <si>
@@ -3449,6 +3440,12 @@
   </si>
   <si>
     <t>freebase.echo('&lt;b&gt;Date of the BCG vaccination is before the date of birth&lt;b&gt;')</t>
+  </si>
+  <si>
+    <t>data('lastvisitdate') == null</t>
+  </si>
+  <si>
+    <t>Mudar as informações?</t>
   </si>
 </sst>
 </file>
@@ -4228,7 +4225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A6BCC52-34B1-45EC-BAB5-A647CE434BBE}">
   <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
@@ -4240,7 +4237,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="B1" s="53" t="s">
         <v>23</v>
@@ -4248,450 +4245,450 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="B2" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="B3" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="B4" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="B5" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="B6" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="B7" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="B8" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="B9" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="B10" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="B11" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="B12" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="B13" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="B14" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="B15" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>856</v>
+      </c>
+      <c r="B16" t="s">
         <v>858</v>
-      </c>
-      <c r="B16" t="s">
-        <v>860</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>857</v>
+      </c>
+      <c r="B17" t="s">
         <v>859</v>
-      </c>
-      <c r="B17" t="s">
-        <v>861</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="B18" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="B19" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="B20" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="B21" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="B22" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="B23" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="B24" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="B25" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="B26" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="B27" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1041</v>
+        <v>1038</v>
       </c>
       <c r="B28" t="s">
-        <v>1045</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
       <c r="B29" t="s">
-        <v>1046</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="B30" t="s">
-        <v>1132</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1050</v>
+        <v>1047</v>
       </c>
       <c r="B31" t="s">
-        <v>1131</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1051</v>
+        <v>1048</v>
       </c>
       <c r="B32" t="s">
-        <v>1130</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="B33" t="s">
-        <v>1129</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
       <c r="B34" t="s">
-        <v>1128</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1054</v>
+        <v>1051</v>
       </c>
       <c r="B35" t="s">
-        <v>1127</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>1055</v>
+        <v>1052</v>
       </c>
       <c r="B36" t="s">
-        <v>1126</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
       <c r="B37" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1057</v>
+        <v>1054</v>
       </c>
       <c r="B38" t="s">
-        <v>1124</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>1058</v>
+        <v>1055</v>
       </c>
       <c r="B39" t="s">
-        <v>1123</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1059</v>
+        <v>1056</v>
       </c>
       <c r="B40" t="s">
-        <v>1122</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1060</v>
+        <v>1057</v>
       </c>
       <c r="B41" t="s">
-        <v>1121</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="B42" t="s">
-        <v>1120</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="B43" t="s">
-        <v>1119</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>1063</v>
+        <v>1060</v>
       </c>
       <c r="B44" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="B45" t="s">
-        <v>1117</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>1065</v>
+        <v>1062</v>
       </c>
       <c r="B46" t="s">
-        <v>1116</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>1066</v>
+        <v>1063</v>
       </c>
       <c r="B47" t="s">
-        <v>1115</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>1067</v>
+        <v>1064</v>
       </c>
       <c r="B48" t="s">
-        <v>1114</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>1068</v>
+        <v>1065</v>
       </c>
       <c r="B49" t="s">
-        <v>1113</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>1069</v>
+        <v>1066</v>
       </c>
       <c r="B50" t="s">
-        <v>1112</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>1070</v>
+        <v>1067</v>
       </c>
       <c r="B51" t="s">
-        <v>1111</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>1071</v>
+        <v>1068</v>
       </c>
       <c r="B52" t="s">
-        <v>1110</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>1072</v>
+        <v>1069</v>
       </c>
       <c r="B53" t="s">
-        <v>1109</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>1073</v>
+        <v>1070</v>
       </c>
       <c r="B54" t="s">
-        <v>1108</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>1074</v>
+        <v>1071</v>
       </c>
       <c r="B55" t="s">
-        <v>1107</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>1075</v>
+        <v>1072</v>
       </c>
       <c r="B56" t="s">
-        <v>1106</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>1076</v>
+        <v>1073</v>
       </c>
       <c r="B57" t="s">
-        <v>1105</v>
+        <v>1102</v>
       </c>
     </row>
   </sheetData>
@@ -5508,7 +5505,7 @@
         <v>254</v>
       </c>
       <c r="D38" s="57" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
       <c r="E38" s="57"/>
     </row>
@@ -5524,7 +5521,7 @@
         <v>252</v>
       </c>
       <c r="D39" s="57" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
       <c r="E39" s="57"/>
     </row>
@@ -5540,7 +5537,7 @@
         <v>253</v>
       </c>
       <c r="D40" s="57" t="s">
-        <v>1030</v>
+        <v>1027</v>
       </c>
       <c r="E40" s="57"/>
     </row>
@@ -5681,7 +5678,7 @@
         <v>628</v>
       </c>
       <c r="D49" s="57" t="s">
-        <v>1031</v>
+        <v>1028</v>
       </c>
       <c r="E49" s="57"/>
     </row>
@@ -5840,7 +5837,7 @@
         <v>643</v>
       </c>
       <c r="D59" s="60" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="E59" s="60"/>
     </row>
@@ -5888,7 +5885,7 @@
         <v>534</v>
       </c>
       <c r="D62" s="57" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="E62" s="57"/>
     </row>
@@ -5920,7 +5917,7 @@
         <v>548</v>
       </c>
       <c r="D64" s="57" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="E64" s="57"/>
     </row>
@@ -5936,7 +5933,7 @@
         <v>553</v>
       </c>
       <c r="D65" s="57" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="E65" s="57"/>
     </row>
@@ -5952,7 +5949,7 @@
         <v>558</v>
       </c>
       <c r="D66" s="57" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="E66" s="57"/>
     </row>
@@ -5968,7 +5965,7 @@
         <v>645</v>
       </c>
       <c r="D67" s="57" t="s">
-        <v>1035</v>
+        <v>1032</v>
       </c>
       <c r="E67" s="57"/>
     </row>
@@ -6080,7 +6077,7 @@
         <v>651</v>
       </c>
       <c r="D74" s="57" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
       <c r="E74" s="57"/>
     </row>
@@ -6096,7 +6093,7 @@
         <v>682</v>
       </c>
       <c r="D75" s="57" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
       <c r="E75" s="57"/>
     </row>
@@ -6112,7 +6109,7 @@
         <v>651</v>
       </c>
       <c r="D76" s="57" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
       <c r="E76" s="57"/>
     </row>
@@ -6128,7 +6125,7 @@
         <v>683</v>
       </c>
       <c r="D77" s="57" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
       <c r="E77" s="57"/>
     </row>
@@ -6144,7 +6141,7 @@
         <v>651</v>
       </c>
       <c r="D78" s="57" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
       <c r="E78" s="57"/>
     </row>
@@ -6160,7 +6157,7 @@
         <v>684</v>
       </c>
       <c r="D79" s="57" t="s">
-        <v>1039</v>
+        <v>1036</v>
       </c>
       <c r="E79" s="57"/>
     </row>
@@ -6176,7 +6173,7 @@
         <v>651</v>
       </c>
       <c r="D80" s="57" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
       <c r="E80" s="57"/>
     </row>
@@ -6826,7 +6823,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B43" t="s">
         <v>25</v>
@@ -7299,7 +7296,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B86" t="s">
         <v>25</v>
@@ -7519,7 +7516,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B106" t="s">
         <v>25</v>
@@ -7541,7 +7538,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B108" t="s">
         <v>72</v>
@@ -8182,7 +8179,7 @@
         <v>52</v>
       </c>
       <c r="B166" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="C166" t="b">
         <v>0</v>
@@ -8380,7 +8377,7 @@
         <v>55</v>
       </c>
       <c r="B184" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="C184" t="b">
         <v>0</v>
@@ -8616,7 +8613,7 @@
     </row>
     <row r="197" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="B197" s="49" t="s">
         <v>72</v>
@@ -8645,7 +8642,7 @@
     </row>
     <row r="199" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B199" t="s">
         <v>25</v>
@@ -8664,7 +8661,7 @@
     </row>
     <row r="200" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B200" t="s">
         <v>25</v>
@@ -8683,7 +8680,7 @@
     </row>
     <row r="201" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="B201" t="s">
         <v>25</v>
@@ -8702,7 +8699,7 @@
     </row>
     <row r="202" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="B202" t="s">
         <v>120</v>
@@ -8721,7 +8718,7 @@
     </row>
     <row r="204" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="B204" t="s">
         <v>72</v>
@@ -8745,7 +8742,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8799,7 +8796,7 @@
         <v>88</v>
       </c>
       <c r="C2" t="s">
-        <v>712</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -8814,7 +8811,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -8831,8 +8828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31E2D9B7-AFA3-430F-905F-12902E548477}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8895,10 +8892,10 @@
         <v>149</v>
       </c>
       <c r="G3" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="H3" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="I3" s="55"/>
     </row>
@@ -8907,10 +8904,10 @@
         <v>149</v>
       </c>
       <c r="G4" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="H4" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
       <c r="I4" s="55"/>
     </row>
@@ -8919,7 +8916,7 @@
         <v>88</v>
       </c>
       <c r="C5" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="I5" s="55"/>
     </row>
@@ -8928,10 +8925,10 @@
         <v>149</v>
       </c>
       <c r="G6" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="H6" s="55" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="I6" s="55"/>
     </row>
@@ -8946,7 +8943,7 @@
         <v>88</v>
       </c>
       <c r="C8" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="I8" s="55"/>
     </row>
@@ -8955,10 +8952,10 @@
         <v>149</v>
       </c>
       <c r="G9" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="H9" s="55" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="I9" s="55"/>
     </row>
@@ -8973,7 +8970,7 @@
         <v>88</v>
       </c>
       <c r="C11" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="I11" s="55"/>
     </row>
@@ -8982,10 +8979,10 @@
         <v>149</v>
       </c>
       <c r="G12" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H12" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="I12" s="55"/>
     </row>
@@ -9000,10 +8997,10 @@
         <v>149</v>
       </c>
       <c r="G14" t="s">
+        <v>734</v>
+      </c>
+      <c r="H14" t="s">
         <v>736</v>
-      </c>
-      <c r="H14" t="s">
-        <v>738</v>
       </c>
       <c r="I14" s="55"/>
     </row>
@@ -9012,10 +9009,10 @@
         <v>149</v>
       </c>
       <c r="G15" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="H15" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="I15" s="55"/>
     </row>
@@ -9024,10 +9021,10 @@
         <v>149</v>
       </c>
       <c r="G16" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="H16" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="I16" s="55"/>
     </row>
@@ -9036,10 +9033,10 @@
         <v>149</v>
       </c>
       <c r="G17" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="H17" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
       <c r="I17" s="55"/>
     </row>
@@ -9051,13 +9048,13 @@
         <v>646</v>
       </c>
       <c r="F18" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="G18" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="H18" s="55" t="s">
-        <v>931</v>
+        <v>1131</v>
       </c>
       <c r="I18" s="55"/>
     </row>
@@ -9069,10 +9066,10 @@
         <v>275</v>
       </c>
       <c r="G19" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="H19" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="I19" s="55"/>
     </row>
@@ -9088,7 +9085,7 @@
         <v>88</v>
       </c>
       <c r="C21" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="I21" s="55"/>
     </row>
@@ -9103,7 +9100,7 @@
         <v>72</v>
       </c>
       <c r="F23" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="G23" t="s">
         <v>74</v>
@@ -9154,10 +9151,10 @@
         <v>118</v>
       </c>
       <c r="G26" t="s">
+        <v>733</v>
+      </c>
+      <c r="H26" t="s">
         <v>735</v>
-      </c>
-      <c r="H26" t="s">
-        <v>737</v>
       </c>
       <c r="I26" s="55"/>
     </row>
@@ -9223,10 +9220,10 @@
         <v>149</v>
       </c>
       <c r="G32" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="H32" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="I32" s="55"/>
     </row>
@@ -9235,10 +9232,10 @@
         <v>149</v>
       </c>
       <c r="G33" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="H33" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
       <c r="I33" s="55"/>
     </row>
@@ -9247,10 +9244,10 @@
         <v>149</v>
       </c>
       <c r="G34" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="H34" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="I34" s="55"/>
     </row>
@@ -9259,10 +9256,10 @@
         <v>149</v>
       </c>
       <c r="G35" t="s">
+        <v>734</v>
+      </c>
+      <c r="H35" t="s">
         <v>736</v>
-      </c>
-      <c r="H35" t="s">
-        <v>738</v>
       </c>
       <c r="I35" s="55"/>
     </row>
@@ -9271,10 +9268,10 @@
         <v>149</v>
       </c>
       <c r="G36" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="H36" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="I36" s="55"/>
     </row>
@@ -9283,10 +9280,10 @@
         <v>149</v>
       </c>
       <c r="G37" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="H37" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="I37" s="55"/>
     </row>
@@ -9295,10 +9292,10 @@
         <v>149</v>
       </c>
       <c r="G38" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="H38" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
       <c r="I38" s="55"/>
     </row>
@@ -9328,9 +9325,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
   <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9456,7 +9453,7 @@
         <v>72</v>
       </c>
       <c r="F8" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="G8" t="s">
         <v>74</v>
@@ -9502,13 +9499,13 @@
       <c r="I10" s="55"/>
       <c r="J10" s="55"/>
       <c r="L10" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="M10" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -9616,7 +9613,7 @@
         <v>88</v>
       </c>
       <c r="C19" t="s">
-        <v>699</v>
+        <v>249</v>
       </c>
       <c r="H19" s="55"/>
       <c r="I19" s="55"/>
@@ -9644,7 +9641,7 @@
         <v>307</v>
       </c>
       <c r="H21" s="55" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="I21" s="55"/>
       <c r="J21" s="55"/>
@@ -9654,7 +9651,7 @@
         <v>88</v>
       </c>
       <c r="C22" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="H22" s="55"/>
       <c r="I22" s="55"/>
@@ -9674,7 +9671,7 @@
         <v>67</v>
       </c>
       <c r="I23" s="55" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="J23" s="55"/>
     </row>
@@ -9692,7 +9689,7 @@
         <v>69</v>
       </c>
       <c r="I24" s="55" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="J24" s="55"/>
     </row>
@@ -9707,10 +9704,10 @@
         <v>71</v>
       </c>
       <c r="H25" s="55" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
       <c r="I25" s="55" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="J25" s="55"/>
     </row>
@@ -9789,7 +9786,7 @@
         <v>71</v>
       </c>
       <c r="H32" s="55" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
       <c r="I32" s="55"/>
       <c r="J32" s="55"/>
@@ -9856,7 +9853,7 @@
         <v>95</v>
       </c>
       <c r="H38" s="55" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
       <c r="I38" s="55"/>
       <c r="J38" s="55"/>
@@ -9883,7 +9880,7 @@
         <v>104</v>
       </c>
       <c r="H40" s="55" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
       <c r="I40" s="55"/>
       <c r="J40" s="55"/>
@@ -9920,7 +9917,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>259</v>
+        <v>709</v>
       </c>
     </row>
   </sheetData>
@@ -9932,10 +9929,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB22453C-0017-476B-BA31-56D5A3D2A587}">
-  <dimension ref="A1:K57"/>
+  <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8:J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10121,7 +10119,7 @@
         <v>174</v>
       </c>
       <c r="H14" s="55" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
       <c r="I14" s="55"/>
       <c r="J14" s="55"/>
@@ -10154,7 +10152,7 @@
         <v>140</v>
       </c>
       <c r="H17" s="55" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
       <c r="I17" s="55"/>
       <c r="J17" s="55"/>
@@ -10427,10 +10425,10 @@
         <v>149</v>
       </c>
       <c r="G43" s="54" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
       <c r="H43" s="55" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
       <c r="I43" s="55"/>
       <c r="J43" s="55"/>
@@ -10512,7 +10510,7 @@
         <v>165</v>
       </c>
       <c r="H50" s="55" t="s">
-        <v>941</v>
+        <v>938</v>
       </c>
       <c r="I50" s="55"/>
       <c r="J50" s="55"/>
@@ -10545,7 +10543,7 @@
         <v>168</v>
       </c>
       <c r="H53" s="55" t="s">
-        <v>942</v>
+        <v>939</v>
       </c>
       <c r="I53" s="55"/>
       <c r="J53" s="55"/>
@@ -10578,7 +10576,7 @@
         <v>171</v>
       </c>
       <c r="H56" s="55" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
       <c r="I56" s="55"/>
       <c r="J56" s="55"/>
@@ -10586,6 +10584,11 @@
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>709</v>
       </c>
     </row>
   </sheetData>
@@ -10673,7 +10676,7 @@
         <v>88</v>
       </c>
       <c r="C3" s="55" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -10681,10 +10684,10 @@
         <v>149</v>
       </c>
       <c r="G4" s="55" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="H4" s="55" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -10698,7 +10701,7 @@
         <v>88</v>
       </c>
       <c r="C6" s="55" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -10706,10 +10709,10 @@
         <v>149</v>
       </c>
       <c r="G7" s="55" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="H7" s="55" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -10723,7 +10726,7 @@
         <v>88</v>
       </c>
       <c r="C9" s="55" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -10731,10 +10734,10 @@
         <v>149</v>
       </c>
       <c r="G10" s="55" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="H10" s="55" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -10748,7 +10751,7 @@
         <v>88</v>
       </c>
       <c r="C12" s="55" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -10756,10 +10759,10 @@
         <v>149</v>
       </c>
       <c r="G13" s="55" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="H13" s="55" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -10773,7 +10776,7 @@
         <v>88</v>
       </c>
       <c r="C15" s="55" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -10781,10 +10784,10 @@
         <v>149</v>
       </c>
       <c r="G16" s="55" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="H16" s="55" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -10798,7 +10801,7 @@
         <v>88</v>
       </c>
       <c r="C18" s="55" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -10806,10 +10809,10 @@
         <v>149</v>
       </c>
       <c r="G19" s="55" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="H19" s="55" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -10823,10 +10826,10 @@
         <v>149</v>
       </c>
       <c r="G21" s="55" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="H21" s="62" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -10834,10 +10837,10 @@
         <v>149</v>
       </c>
       <c r="G22" s="55" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="H22" s="55" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -10882,13 +10885,13 @@
         <v>270</v>
       </c>
       <c r="K25" s="55" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="L25" s="55" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="M25" s="55" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -11024,7 +11027,7 @@
         <v>284</v>
       </c>
       <c r="H40" s="55" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -11048,16 +11051,16 @@
         <v>286</v>
       </c>
       <c r="H42" s="55" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
       <c r="K42" s="55" t="s">
-        <v>1040</v>
+        <v>1037</v>
       </c>
       <c r="L42" s="55" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="M42" s="55" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -11072,7 +11075,7 @@
         <v>287</v>
       </c>
       <c r="H43" s="55" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -11121,7 +11124,7 @@
         <v>289</v>
       </c>
       <c r="H49" s="55" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
@@ -11145,16 +11148,16 @@
         <v>291</v>
       </c>
       <c r="H51" s="55" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
       <c r="K51" s="55" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="L51" s="55" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="M51" s="55" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
@@ -11169,7 +11172,7 @@
         <v>292</v>
       </c>
       <c r="H52" s="55" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
@@ -11210,7 +11213,7 @@
         <v>294</v>
       </c>
       <c r="H57" s="55" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -11228,7 +11231,7 @@
         <v>297</v>
       </c>
       <c r="H58" s="55" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
@@ -11255,7 +11258,7 @@
         <v>301</v>
       </c>
       <c r="H60" s="55" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
@@ -11291,7 +11294,7 @@
         <v>303</v>
       </c>
       <c r="H64" s="55" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
@@ -11309,7 +11312,7 @@
         <v>305</v>
       </c>
       <c r="H65" s="55" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
@@ -11347,7 +11350,7 @@
         <v>307</v>
       </c>
       <c r="H69" s="55" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
@@ -11371,16 +11374,16 @@
         <v>309</v>
       </c>
       <c r="H71" s="55" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
       <c r="K71" s="55" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="L71" s="55" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="M71" s="55" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
@@ -11395,7 +11398,7 @@
         <v>310</v>
       </c>
       <c r="H72" s="55" t="s">
-        <v>957</v>
+        <v>954</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
@@ -11410,7 +11413,7 @@
         <v>311</v>
       </c>
       <c r="H73" s="55" t="s">
-        <v>958</v>
+        <v>955</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
@@ -11456,7 +11459,7 @@
         <v>313</v>
       </c>
       <c r="H79" s="55" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
@@ -11538,16 +11541,16 @@
         <v>318</v>
       </c>
       <c r="H89" s="55" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
       <c r="K89" s="55" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="L89" s="55" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="M89" s="62" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
@@ -11577,7 +11580,7 @@
         <v>321</v>
       </c>
       <c r="H92" s="55" t="s">
-        <v>961</v>
+        <v>958</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
@@ -11613,7 +11616,7 @@
         <v>324</v>
       </c>
       <c r="H96" s="55" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -11628,7 +11631,7 @@
         <v>326</v>
       </c>
       <c r="H97" s="55" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -11664,7 +11667,7 @@
         <v>328</v>
       </c>
       <c r="H101" s="55" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -11691,7 +11694,7 @@
         <v>331</v>
       </c>
       <c r="H103" s="55" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -11737,13 +11740,13 @@
         <v>88</v>
       </c>
       <c r="C110" s="75" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="57"/>
       <c r="B111" s="57" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="C111" s="57"/>
       <c r="D111" s="57"/>
@@ -11793,7 +11796,7 @@
         <v>376</v>
       </c>
       <c r="H115" s="55" t="s">
-        <v>981</v>
+        <v>978</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -12343,7 +12346,7 @@
         <v>334</v>
       </c>
       <c r="H4" s="55" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -12385,7 +12388,7 @@
         <v>337</v>
       </c>
       <c r="H8" s="55" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -12417,7 +12420,7 @@
         <v>340</v>
       </c>
       <c r="H11" s="55" t="s">
-        <v>968</v>
+        <v>965</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -12442,7 +12445,7 @@
         <v>343</v>
       </c>
       <c r="H13" s="55" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -12460,7 +12463,7 @@
         <v>345</v>
       </c>
       <c r="H14" s="55" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -12509,7 +12512,7 @@
         <v>347</v>
       </c>
       <c r="H19" s="55" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -12518,7 +12521,7 @@
         <v>88</v>
       </c>
       <c r="C20" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="H20" s="55"/>
     </row>
@@ -12534,7 +12537,7 @@
         <v>347</v>
       </c>
       <c r="H21" s="55" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -12573,7 +12576,7 @@
         <v>350</v>
       </c>
       <c r="H25" s="55" t="s">
-        <v>972</v>
+        <v>969</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -12605,7 +12608,7 @@
         <v>352</v>
       </c>
       <c r="H28" s="55" t="s">
-        <v>973</v>
+        <v>970</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -12630,7 +12633,7 @@
         <v>355</v>
       </c>
       <c r="H30" s="55" t="s">
-        <v>974</v>
+        <v>971</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -12679,7 +12682,7 @@
         <v>357</v>
       </c>
       <c r="H35" s="55" t="s">
-        <v>975</v>
+        <v>972</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -12704,7 +12707,7 @@
         <v>360</v>
       </c>
       <c r="H37" s="55" t="s">
-        <v>976</v>
+        <v>973</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -12750,7 +12753,7 @@
         <v>362</v>
       </c>
       <c r="H42" s="55" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -12759,7 +12762,7 @@
         <v>88</v>
       </c>
       <c r="C43" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="H43" s="55"/>
     </row>
@@ -12775,7 +12778,7 @@
         <v>343</v>
       </c>
       <c r="H44" s="55" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -12793,7 +12796,7 @@
         <v>345</v>
       </c>
       <c r="H45" s="55" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -12842,7 +12845,7 @@
         <v>347</v>
       </c>
       <c r="H50" s="55" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -12851,7 +12854,7 @@
         <v>88</v>
       </c>
       <c r="C51" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="H51" s="55"/>
     </row>
@@ -12867,7 +12870,7 @@
         <v>347</v>
       </c>
       <c r="H52" s="55" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -12906,7 +12909,7 @@
         <v>350</v>
       </c>
       <c r="H56" s="55" t="s">
-        <v>972</v>
+        <v>969</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -12938,7 +12941,7 @@
         <v>352</v>
       </c>
       <c r="H59" s="55" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -12963,7 +12966,7 @@
         <v>355</v>
       </c>
       <c r="H61" s="55" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -13012,7 +13015,7 @@
         <v>357</v>
       </c>
       <c r="H66" s="55" t="s">
-        <v>975</v>
+        <v>972</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -13037,7 +13040,7 @@
         <v>360</v>
       </c>
       <c r="H68" s="55" t="s">
-        <v>976</v>
+        <v>973</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -13096,7 +13099,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H77" s="55" t="s">
-        <v>981</v>
+        <v>978</v>
       </c>
     </row>
   </sheetData>
@@ -13180,7 +13183,7 @@
         <v>88</v>
       </c>
       <c r="C3" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -13248,10 +13251,10 @@
         <v>385</v>
       </c>
       <c r="G10" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="H10" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -13285,7 +13288,7 @@
         <v>88</v>
       </c>
       <c r="C15" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -13353,10 +13356,10 @@
         <v>392</v>
       </c>
       <c r="G22" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="H22" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -13401,7 +13404,7 @@
         <v>88</v>
       </c>
       <c r="C29" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -13410,10 +13413,10 @@
         <v>149</v>
       </c>
       <c r="G30" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="H30" t="s">
-        <v>1077</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -13428,7 +13431,7 @@
         <v>88</v>
       </c>
       <c r="C32" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -13437,10 +13440,10 @@
         <v>149</v>
       </c>
       <c r="G33" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="H33" t="s">
-        <v>1078</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -13451,10 +13454,10 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="C35" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -13522,10 +13525,10 @@
         <v>399</v>
       </c>
       <c r="G42" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="H42" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -13559,7 +13562,7 @@
         <v>88</v>
       </c>
       <c r="C47" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -13651,10 +13654,10 @@
         <v>405</v>
       </c>
       <c r="G57" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="H57" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
@@ -13688,7 +13691,7 @@
         <v>88</v>
       </c>
       <c r="C62" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
@@ -13780,10 +13783,10 @@
         <v>411</v>
       </c>
       <c r="G72" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="H72" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.25">
@@ -13817,7 +13820,7 @@
         <v>88</v>
       </c>
       <c r="C77" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
@@ -13909,10 +13912,10 @@
         <v>417</v>
       </c>
       <c r="G87" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="H87" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -13957,7 +13960,7 @@
         <v>88</v>
       </c>
       <c r="C94" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -13966,10 +13969,10 @@
         <v>149</v>
       </c>
       <c r="G95" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="H95" t="s">
-        <v>1079</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -13984,7 +13987,7 @@
         <v>88</v>
       </c>
       <c r="C97" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -13993,10 +13996,10 @@
         <v>149</v>
       </c>
       <c r="G98" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="H98" t="s">
-        <v>1080</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -14011,7 +14014,7 @@
         <v>88</v>
       </c>
       <c r="C100" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -14020,10 +14023,10 @@
         <v>149</v>
       </c>
       <c r="G101" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="H101" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -14038,7 +14041,7 @@
         <v>88</v>
       </c>
       <c r="C103" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
@@ -14047,10 +14050,10 @@
         <v>149</v>
       </c>
       <c r="G104" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="H104" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
@@ -14064,7 +14067,7 @@
         <v>88</v>
       </c>
       <c r="C106" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
@@ -14132,10 +14135,10 @@
         <v>424</v>
       </c>
       <c r="G113" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="H113" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.25">
@@ -14169,7 +14172,7 @@
         <v>88</v>
       </c>
       <c r="C118" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.25">
@@ -14261,10 +14264,10 @@
         <v>430</v>
       </c>
       <c r="G128" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="H128" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="129" spans="2:9" x14ac:dyDescent="0.25">
@@ -14298,7 +14301,7 @@
         <v>88</v>
       </c>
       <c r="C133" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="134" spans="2:9" x14ac:dyDescent="0.25">
@@ -14390,10 +14393,10 @@
         <v>436</v>
       </c>
       <c r="G143" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="H143" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
     </row>
     <row r="144" spans="2:9" x14ac:dyDescent="0.25">
@@ -14427,7 +14430,7 @@
         <v>88</v>
       </c>
       <c r="C148" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="149" spans="2:9" x14ac:dyDescent="0.25">
@@ -14519,10 +14522,10 @@
         <v>442</v>
       </c>
       <c r="G158" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="H158" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
     </row>
     <row r="159" spans="2:9" x14ac:dyDescent="0.25">
@@ -14567,7 +14570,7 @@
         <v>88</v>
       </c>
       <c r="C165" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
@@ -14576,10 +14579,10 @@
         <v>149</v>
       </c>
       <c r="G166" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="H166" t="s">
-        <v>1083</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
@@ -14594,7 +14597,7 @@
         <v>88</v>
       </c>
       <c r="C168" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
@@ -14603,10 +14606,10 @@
         <v>149</v>
       </c>
       <c r="G169" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="H169" t="s">
-        <v>1084</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
@@ -14621,7 +14624,7 @@
         <v>88</v>
       </c>
       <c r="C171" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
@@ -14630,10 +14633,10 @@
         <v>149</v>
       </c>
       <c r="G172" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="H172" t="s">
-        <v>1085</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
@@ -14648,7 +14651,7 @@
         <v>88</v>
       </c>
       <c r="C174" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
@@ -14657,10 +14660,10 @@
         <v>149</v>
       </c>
       <c r="G175" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="H175" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
@@ -14675,7 +14678,7 @@
         <v>88</v>
       </c>
       <c r="C177" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
@@ -14684,10 +14687,10 @@
         <v>149</v>
       </c>
       <c r="G178" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="H178" t="s">
-        <v>1087</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
@@ -14702,7 +14705,7 @@
         <v>88</v>
       </c>
       <c r="C180" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
@@ -14711,10 +14714,10 @@
         <v>149</v>
       </c>
       <c r="G181" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="H181" t="s">
-        <v>1088</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
@@ -14729,7 +14732,7 @@
         <v>88</v>
       </c>
       <c r="C183" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">
@@ -14738,10 +14741,10 @@
         <v>149</v>
       </c>
       <c r="G184" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="H184" t="s">
-        <v>1089</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
@@ -14756,7 +14759,7 @@
         <v>88</v>
       </c>
       <c r="C186" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.25">
@@ -14765,10 +14768,10 @@
         <v>149</v>
       </c>
       <c r="G187" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="H187" t="s">
-        <v>1090</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.25">
@@ -14782,7 +14785,7 @@
         <v>88</v>
       </c>
       <c r="C189" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.25">
@@ -14850,10 +14853,10 @@
         <v>449</v>
       </c>
       <c r="G196" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="H196" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
     </row>
     <row r="197" spans="2:9" x14ac:dyDescent="0.25">
@@ -14887,7 +14890,7 @@
         <v>88</v>
       </c>
       <c r="C201" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
     </row>
     <row r="202" spans="2:9" x14ac:dyDescent="0.25">
@@ -14979,10 +14982,10 @@
         <v>455</v>
       </c>
       <c r="G211" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="H211" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
     </row>
     <row r="212" spans="2:9" x14ac:dyDescent="0.25">
@@ -15016,7 +15019,7 @@
         <v>88</v>
       </c>
       <c r="C216" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
     </row>
     <row r="217" spans="2:9" x14ac:dyDescent="0.25">
@@ -15108,10 +15111,10 @@
         <v>461</v>
       </c>
       <c r="G226" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="H226" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
     </row>
     <row r="227" spans="2:9" x14ac:dyDescent="0.25">
@@ -15145,7 +15148,7 @@
         <v>88</v>
       </c>
       <c r="C231" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
     </row>
     <row r="232" spans="2:9" x14ac:dyDescent="0.25">
@@ -15237,10 +15240,10 @@
         <v>467</v>
       </c>
       <c r="G241" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H241" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.25">
@@ -15285,7 +15288,7 @@
         <v>88</v>
       </c>
       <c r="C248" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
     </row>
     <row r="249" spans="1:8" x14ac:dyDescent="0.25">
@@ -15294,10 +15297,10 @@
         <v>149</v>
       </c>
       <c r="G249" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="H249" t="s">
-        <v>1091</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="250" spans="1:8" x14ac:dyDescent="0.25">
@@ -15312,7 +15315,7 @@
         <v>88</v>
       </c>
       <c r="C251" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.25">
@@ -15321,10 +15324,10 @@
         <v>149</v>
       </c>
       <c r="G252" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="H252" t="s">
-        <v>1092</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="253" spans="1:8" x14ac:dyDescent="0.25">
@@ -15339,7 +15342,7 @@
         <v>88</v>
       </c>
       <c r="C254" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
     </row>
     <row r="255" spans="1:8" x14ac:dyDescent="0.25">
@@ -15348,10 +15351,10 @@
         <v>149</v>
       </c>
       <c r="G255" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="H255" t="s">
-        <v>1093</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="256" spans="1:8" x14ac:dyDescent="0.25">
@@ -15366,7 +15369,7 @@
         <v>88</v>
       </c>
       <c r="C257" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.25">
@@ -15375,10 +15378,10 @@
         <v>149</v>
       </c>
       <c r="G258" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="H258" t="s">
-        <v>1094</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.25">
@@ -15393,7 +15396,7 @@
         <v>88</v>
       </c>
       <c r="C260" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
     </row>
     <row r="261" spans="1:8" x14ac:dyDescent="0.25">
@@ -15402,10 +15405,10 @@
         <v>149</v>
       </c>
       <c r="G261" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="H261" t="s">
-        <v>1095</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="262" spans="1:8" x14ac:dyDescent="0.25">
@@ -15420,7 +15423,7 @@
         <v>88</v>
       </c>
       <c r="C263" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
     </row>
     <row r="264" spans="1:8" x14ac:dyDescent="0.25">
@@ -15429,10 +15432,10 @@
         <v>149</v>
       </c>
       <c r="G264" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="H264" t="s">
-        <v>1096</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="265" spans="1:8" x14ac:dyDescent="0.25">
@@ -15447,7 +15450,7 @@
         <v>88</v>
       </c>
       <c r="C266" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
     </row>
     <row r="267" spans="1:8" x14ac:dyDescent="0.25">
@@ -15456,10 +15459,10 @@
         <v>149</v>
       </c>
       <c r="G267" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="H267" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="268" spans="1:8" x14ac:dyDescent="0.25">
@@ -15474,7 +15477,7 @@
         <v>88</v>
       </c>
       <c r="C269" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
     </row>
     <row r="270" spans="1:8" x14ac:dyDescent="0.25">
@@ -15483,10 +15486,10 @@
         <v>149</v>
       </c>
       <c r="G270" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="H270" t="s">
-        <v>1098</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="271" spans="1:8" x14ac:dyDescent="0.25">
@@ -15501,7 +15504,7 @@
         <v>88</v>
       </c>
       <c r="C272" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
     </row>
     <row r="273" spans="1:9" x14ac:dyDescent="0.25">
@@ -15510,10 +15513,10 @@
         <v>149</v>
       </c>
       <c r="G273" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="H273" t="s">
-        <v>1099</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="274" spans="1:9" x14ac:dyDescent="0.25">
@@ -15528,7 +15531,7 @@
         <v>88</v>
       </c>
       <c r="C275" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
     </row>
     <row r="276" spans="1:9" x14ac:dyDescent="0.25">
@@ -15537,10 +15540,10 @@
         <v>149</v>
       </c>
       <c r="G276" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="H276" t="s">
-        <v>1100</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="277" spans="1:9" x14ac:dyDescent="0.25">
@@ -15554,7 +15557,7 @@
         <v>88</v>
       </c>
       <c r="C278" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
     </row>
     <row r="279" spans="1:9" x14ac:dyDescent="0.25">
@@ -15622,10 +15625,10 @@
         <v>474</v>
       </c>
       <c r="G285" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="H285" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
     </row>
     <row r="286" spans="1:9" x14ac:dyDescent="0.25">
@@ -15659,7 +15662,7 @@
         <v>88</v>
       </c>
       <c r="C290" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
     </row>
     <row r="291" spans="1:9" x14ac:dyDescent="0.25">
@@ -15727,10 +15730,10 @@
         <v>481</v>
       </c>
       <c r="G297" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="H297" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
     </row>
     <row r="298" spans="1:9" x14ac:dyDescent="0.25">
@@ -15775,7 +15778,7 @@
         <v>88</v>
       </c>
       <c r="C304" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
     </row>
     <row r="305" spans="1:8" x14ac:dyDescent="0.25">
@@ -15784,10 +15787,10 @@
         <v>149</v>
       </c>
       <c r="G305" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="H305" t="s">
-        <v>1101</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="306" spans="1:8" x14ac:dyDescent="0.25">
@@ -15802,7 +15805,7 @@
         <v>88</v>
       </c>
       <c r="C307" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
     </row>
     <row r="308" spans="1:8" x14ac:dyDescent="0.25">
@@ -15811,10 +15814,10 @@
         <v>149</v>
       </c>
       <c r="G308" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="H308" t="s">
-        <v>1102</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="309" spans="1:8" x14ac:dyDescent="0.25">
@@ -15829,7 +15832,7 @@
         <v>88</v>
       </c>
       <c r="C310" s="6" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
       <c r="D310" s="50"/>
       <c r="E310" s="50"/>
@@ -15843,10 +15846,10 @@
         <v>149</v>
       </c>
       <c r="G311" s="50" t="s">
-        <v>1043</v>
+        <v>1040</v>
       </c>
       <c r="H311" s="50" t="s">
-        <v>1103</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="312" spans="1:8" x14ac:dyDescent="0.25">
@@ -15861,13 +15864,13 @@
         <v>88</v>
       </c>
       <c r="C313" s="6" t="s">
-        <v>1047</v>
+        <v>1044</v>
       </c>
       <c r="G313" t="s">
-        <v>1044</v>
+        <v>1041</v>
       </c>
       <c r="H313" t="s">
-        <v>1104</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="314" spans="1:8" x14ac:dyDescent="0.25">
@@ -16054,7 +16057,7 @@
         <v>378</v>
       </c>
       <c r="H10" s="55" t="s">
-        <v>982</v>
+        <v>979</v>
       </c>
       <c r="J10" s="12"/>
     </row>
@@ -16091,7 +16094,7 @@
         <v>388</v>
       </c>
       <c r="H12" s="55" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -16106,7 +16109,7 @@
         <v>497</v>
       </c>
       <c r="H13" s="55" t="s">
-        <v>984</v>
+        <v>981</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -16138,7 +16141,7 @@
         <v>499</v>
       </c>
       <c r="H16" s="55" t="s">
-        <v>985</v>
+        <v>982</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -16153,7 +16156,7 @@
         <v>501</v>
       </c>
       <c r="H17" s="55" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -16171,7 +16174,7 @@
         <v>503</v>
       </c>
       <c r="H18" s="55" t="s">
-        <v>987</v>
+        <v>984</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -16189,7 +16192,7 @@
         <v>505</v>
       </c>
       <c r="H19" s="55" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -16204,7 +16207,7 @@
         <v>507</v>
       </c>
       <c r="H20" s="55" t="s">
-        <v>989</v>
+        <v>986</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -16241,7 +16244,7 @@
         <v>509</v>
       </c>
       <c r="H24" s="55" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -16256,7 +16259,7 @@
         <v>511</v>
       </c>
       <c r="H25" s="55" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -16285,7 +16288,7 @@
         <v>509</v>
       </c>
       <c r="H28" s="55" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -16300,7 +16303,7 @@
         <v>511</v>
       </c>
       <c r="H29" s="55" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -16332,7 +16335,7 @@
         <v>515</v>
       </c>
       <c r="H32" s="55" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -16364,7 +16367,7 @@
         <v>517</v>
       </c>
       <c r="H35" s="55" t="s">
-        <v>993</v>
+        <v>990</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -16392,7 +16395,7 @@
         <v>520</v>
       </c>
       <c r="H37" s="55" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -16431,7 +16434,7 @@
         <v>522</v>
       </c>
       <c r="H41" s="55" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -16463,7 +16466,7 @@
         <v>524</v>
       </c>
       <c r="H44" s="55" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -16488,7 +16491,7 @@
         <v>527</v>
       </c>
       <c r="H46" s="55" t="s">
-        <v>997</v>
+        <v>994</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -16527,7 +16530,7 @@
         <v>529</v>
       </c>
       <c r="H50" s="55" t="s">
-        <v>998</v>
+        <v>995</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -16556,7 +16559,7 @@
         <v>532</v>
       </c>
       <c r="H53" s="55" t="s">
-        <v>999</v>
+        <v>996</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -16620,7 +16623,7 @@
         <v>538</v>
       </c>
       <c r="H59" s="55" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -16684,7 +16687,7 @@
         <v>544</v>
       </c>
       <c r="H65" s="55" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -16699,7 +16702,7 @@
         <v>546</v>
       </c>
       <c r="H66" s="55" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -16738,7 +16741,7 @@
         <v>548</v>
       </c>
       <c r="H70" s="55" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -16763,7 +16766,7 @@
         <v>551</v>
       </c>
       <c r="H72" s="55" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -16802,7 +16805,7 @@
         <v>553</v>
       </c>
       <c r="H76" s="55" t="s">
-        <v>1005</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -16827,7 +16830,7 @@
         <v>556</v>
       </c>
       <c r="H78" s="55" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -16866,7 +16869,7 @@
         <v>558</v>
       </c>
       <c r="H82" s="55" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -16891,7 +16894,7 @@
         <v>561</v>
       </c>
       <c r="H84" s="55" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -16930,7 +16933,7 @@
         <v>563</v>
       </c>
       <c r="H88" s="55" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -16955,7 +16958,7 @@
         <v>566</v>
       </c>
       <c r="H90" s="55" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -17019,7 +17022,7 @@
         <v>572</v>
       </c>
       <c r="H96" s="55" t="s">
-        <v>1011</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -17068,7 +17071,7 @@
         <v>574</v>
       </c>
       <c r="H101" s="55" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -17093,7 +17096,7 @@
         <v>577</v>
       </c>
       <c r="H103" s="55" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -17136,7 +17139,7 @@
         <v>579</v>
       </c>
       <c r="H108" s="55" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -17151,7 +17154,7 @@
         <v>579</v>
       </c>
       <c r="H109" s="55" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -17183,7 +17186,7 @@
         <v>582</v>
       </c>
       <c r="H112" s="55" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -17227,7 +17230,7 @@
         <v>585</v>
       </c>
       <c r="H116" s="55" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -17273,7 +17276,7 @@
         <v>588</v>
       </c>
       <c r="H121" s="55" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -17301,7 +17304,7 @@
         <v>591</v>
       </c>
       <c r="H123" s="55" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -17337,7 +17340,7 @@
         <v>593</v>
       </c>
       <c r="H127" s="55" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -17355,7 +17358,7 @@
         <v>595</v>
       </c>
       <c r="H128" s="55" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -17387,7 +17390,7 @@
         <v>597</v>
       </c>
       <c r="H131" s="55" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -17405,7 +17408,7 @@
         <v>599</v>
       </c>
       <c r="H132" s="55" t="s">
-        <v>1022</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
@@ -17444,7 +17447,7 @@
         <v>601</v>
       </c>
       <c r="H136" s="55" t="s">
-        <v>1023</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
@@ -17469,7 +17472,7 @@
         <v>604</v>
       </c>
       <c r="H138" s="55" t="s">
-        <v>1024</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
@@ -17508,7 +17511,7 @@
         <v>606</v>
       </c>
       <c r="H142" s="55" t="s">
-        <v>1025</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
@@ -17533,7 +17536,7 @@
         <v>609</v>
       </c>
       <c r="H144" s="55" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
@@ -17548,7 +17551,7 @@
         <v>611</v>
       </c>
       <c r="H145" s="55" t="s">
-        <v>1027</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Only show cildren we should visit + changes to constrins in CRIANCA
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
+++ b/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51690BB-04CF-418D-95CC-16FA69A140EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7C7FE0-5377-4CA7-B50D-4733F6B55236}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="674" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="674" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2788" uniqueCount="1132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2784" uniqueCount="1131">
   <si>
     <t>setting_name</t>
   </si>
@@ -2635,84 +2635,6 @@
     <t xml:space="preserve">if </t>
   </si>
   <si>
-    <t>adate.diffInYears(data('OUTDATE'), data('POLIONAS'))&lt;0 &amp;&amp; data('POLIONAS') != null</t>
-  </si>
-  <si>
-    <t>adate.diffInYears(data('OUTDATE'), data('BCG'))&lt;0 &amp;&amp; data('BCG') != null</t>
-  </si>
-  <si>
-    <t>adate.diffInYears(data('OUTDATE'), data('PENTA1'))&lt;0  &amp;&amp; data('PENTA1') != null</t>
-  </si>
-  <si>
-    <t>adate.diffInYears(data('OUTDATE'), data('POLIO1'))&lt;0  &amp;&amp; data('POLIO1') != null</t>
-  </si>
-  <si>
-    <t>adate.diffInYears(data('OUTDATE'), data('PCV1'))&lt;0 &amp;&amp; data('PCV1') != null</t>
-  </si>
-  <si>
-    <t>adate.diffInYears(data('OUTDATE'), data('ROX1'))&lt;0  &amp;&amp; data('ROX1') != null</t>
-  </si>
-  <si>
-    <t>adate.diffInYears(data('OUTDATE'), data('PENTA2'))&lt;0 &amp;&amp; data('PENTA2') != null</t>
-  </si>
-  <si>
-    <t>adate.diffInYears(data('OUTDATE'), data('POLIO2'))&lt;0 &amp;&amp; data('POLIO2') != null</t>
-  </si>
-  <si>
-    <t>adate.diffInYears(data('OUTDATE'), data('PCV2'))&lt;0 &amp;&amp; data('PCV2') != null</t>
-  </si>
-  <si>
-    <t>adate.diffInYears(data('OUTDATE'), data('ROX2'))&lt;0 &amp;&amp; data('ROX2') != null</t>
-  </si>
-  <si>
-    <t>adate.diffInYears(data('PENTA1'), data('PENTA2'))&lt;0 &amp;&amp; data('PENTA2') != null</t>
-  </si>
-  <si>
-    <t>adate.diffInYears(data('POLIO1'), data('POLIO2'))&lt;0  &amp;&amp; data('POLIO2') != null</t>
-  </si>
-  <si>
-    <t>adate.diffInYears(data('PCV1'), data('PCV2'))&lt;0  &amp;&amp; data('PCV2') != null</t>
-  </si>
-  <si>
-    <t>adate.diffInYears(data('ROX1'), data('ROX2'))&lt;0  &amp;&amp; data('ROX2') != null</t>
-  </si>
-  <si>
-    <t>adate.diffInYears(data('OUTDATE'), data('PENTA3'))&lt;0  &amp;&amp; data('PENTA3') != null</t>
-  </si>
-  <si>
-    <t>adate.diffInYears(data('OUTDATE'), data('POLIO3'))&lt;0 &amp;&amp; data('POLIO3') != null</t>
-  </si>
-  <si>
-    <t>adate.diffInYears(data('OUTDATE'), data('PCV3'))&lt;0 &amp;&amp; data('PCV3') != null</t>
-  </si>
-  <si>
-    <t>adate.diffInYears(data('OUTDATE'), data('VPI'))&lt;0 &amp;&amp; data('VPI') != null</t>
-  </si>
-  <si>
-    <t>adate.diffInYears(data('PENTA2'), data('PENTA3'))&lt;0  &amp;&amp; data('PENTA3') != null</t>
-  </si>
-  <si>
-    <t>adate.diffInYears(data('POLIO2'), data('POLIO3'))&lt;0  &amp;&amp; data('POLIO3') != null</t>
-  </si>
-  <si>
-    <t>adate.diffInYears(data('PCV2'), data('PCV3'))&lt;0  &amp;&amp; data('PCV3') != null</t>
-  </si>
-  <si>
-    <t>adate.diffInYears(data('PENTA1'), data('PENTA3'))&lt;0  &amp;&amp; data('PENTA3') != null</t>
-  </si>
-  <si>
-    <t>adate.diffInYears(data('POLIO1'), data('POLIO3'))&lt;0  &amp;&amp; data('POLIO3') != null</t>
-  </si>
-  <si>
-    <t>adate.diffInYears(data('PCV1'), data('PCV3'))&lt;0  &amp;&amp; data('PCV3') != null</t>
-  </si>
-  <si>
-    <t>adate.diffInYears(data('OUTDATE'), data('FEBAMAREL'))&lt;0 &amp;&amp; data('FEBAMAREL') != null</t>
-  </si>
-  <si>
-    <t>adate.diffInYears(data('OUTDATE'), data('SARAMPO1'))&lt;0 &amp;&amp; data('SARAMPO') != null</t>
-  </si>
-  <si>
     <t>1penta2pu</t>
   </si>
   <si>
@@ -2809,15 +2731,9 @@
     <t>Today's date: {{data.CONT}}</t>
   </si>
   <si>
-    <t>Today</t>
-  </si>
-  <si>
     <t>Exitdate cannot be before before last vist and cannot be in the future</t>
   </si>
   <si>
-    <t>((adate.diffInYears(data('CONT'), data('EXITDATA'))&lt;1) &amp;&amp; (adate.diffInYears(data('EXITDATA'), data('lastvisitdate'))&lt;0) &amp;&amp; (data('PRES') == '2' || data('PRES') == '3'))</t>
-  </si>
-  <si>
     <t>adate.diffInYears(data('CONT'), data('DAPAMA'))&lt;1</t>
   </si>
   <si>
@@ -2923,9 +2839,6 @@
     <t>A criança foi internada no Hostpital desde a última visita?</t>
   </si>
   <si>
-    <t>Quais são as medidas de MUAC na crianca em MM</t>
-  </si>
-  <si>
     <t>A criança tem uma cicatriz de BSG?</t>
   </si>
   <si>
@@ -3446,6 +3359,90 @@
   </si>
   <si>
     <t>Mudar as informações?</t>
+  </si>
+  <si>
+    <t>adate.diffInYears(data('CONT'), data('EXITDATA'))&lt;1 &amp;&amp; adate.diffInYears(data('EXITDATA'), data('lastvisitdate'))&lt;0 || (data('PRES') != '2' &amp;&amp; data('PRES') != '3')</t>
+  </si>
+  <si>
+    <t>Quais são as medidas de braco na crianca em MM</t>
+  </si>
+  <si>
+    <t>adate.diffInYears(data('OUTDATE'), data('BCG'))&lt;0 &amp;&amp; data('BCG') != null &amp;&amp; data('BCG') != 'D:2,M:2,Y:1922'</t>
+  </si>
+  <si>
+    <t>adate.diffInYears(data('OUTDATE'), data('POLIONAS'))&lt;0 &amp;&amp; data('POLIONAS') != null &amp;&amp; data('POLIONAS') != 'D:2,M:2,Y:1922'</t>
+  </si>
+  <si>
+    <t>adate.diffInYears(data('OUTDATE'), data('PENTA1'))&lt;0  &amp;&amp; data('PENTA1') != null &amp;&amp; data('PENTA1') != 'D:2,M:2,Y:1922'</t>
+  </si>
+  <si>
+    <t>adate.diffInYears(data('OUTDATE'), data('POLIO1'))&lt;0  &amp;&amp; data('POLIO1') != null &amp;&amp; data('POLIO1') != 'D:2,M:2,Y:1922'</t>
+  </si>
+  <si>
+    <t>adate.diffInYears(data('OUTDATE'), data('PCV1'))&lt;0 &amp;&amp; data('PCV1') != null &amp;&amp; data('PCV1') != 'D:2,M:2,Y:1922'</t>
+  </si>
+  <si>
+    <t>adate.diffInYears(data('OUTDATE'), data('ROX1'))&lt;0  &amp;&amp; data('ROX1') != null &amp;&amp; data('ROX1') != 'D:2,M:2,Y:1922'</t>
+  </si>
+  <si>
+    <t>adate.diffInYears(data('OUTDATE'), data('PENTA2'))&lt;0 &amp;&amp; data('PENTA2') != null &amp;&amp; data('PENTA2') != 'D:2,M:2,Y:1922'</t>
+  </si>
+  <si>
+    <t>adate.diffInYears(data('PENTA1'), data('PENTA2'))&lt;0 &amp;&amp; data('PENTA2') != null &amp;&amp; data('PENTA2') != 'D:2,M:2,Y:1922'</t>
+  </si>
+  <si>
+    <t>adate.diffInYears(data('OUTDATE'), data('POLIO2'))&lt;0 &amp;&amp; data('POLIO2') != null &amp;&amp; data('POLIO2') != 'D:2,M:2,Y:1922'</t>
+  </si>
+  <si>
+    <t>adate.diffInYears(data('POLIO1'), data('POLIO2'))&lt;0  &amp;&amp; data('POLIO2') != null &amp;&amp; data('POLIO2') != 'D:2,M:2,Y:1922'</t>
+  </si>
+  <si>
+    <t>adate.diffInYears(data('OUTDATE'), data('PCV2'))&lt;0 &amp;&amp; data('PCV2') != null &amp;&amp; data('PCV2') != 'D:2,M:2,Y:1922'</t>
+  </si>
+  <si>
+    <t>adate.diffInYears(data('PCV1'), data('PCV2'))&lt;0  &amp;&amp; data('PCV2') != null &amp;&amp; data('PCV2') != 'D:2,M:2,Y:1922'</t>
+  </si>
+  <si>
+    <t>adate.diffInYears(data('OUTDATE'), data('ROX2'))&lt;0 &amp;&amp; data('ROX2') != null &amp;&amp; data('ROX2') != 'D:2,M:2,Y:1922'</t>
+  </si>
+  <si>
+    <t>adate.diffInYears(data('ROX1'), data('ROX2'))&lt;0  &amp;&amp; data('ROX2') != null &amp;&amp; data('ROX2') != 'D:2,M:2,Y:1922'</t>
+  </si>
+  <si>
+    <t>adate.diffInYears(data('OUTDATE'), data('PENTA3'))&lt;0  &amp;&amp; data('PENTA3') != null &amp;&amp; data('PENTA3') != 'D:2,M:2,Y:1922'</t>
+  </si>
+  <si>
+    <t>adate.diffInYears(data('PENTA2'), data('PENTA3'))&lt;0  &amp;&amp; data('PENTA3') != null &amp;&amp; data('PENTA3') != 'D:2,M:2,Y:1922'</t>
+  </si>
+  <si>
+    <t>adate.diffInYears(data('PENTA1'), data('PENTA3'))&lt;0  &amp;&amp; data('PENTA3') != null &amp;&amp; data('PENTA3') != 'D:2,M:2,Y:1922'</t>
+  </si>
+  <si>
+    <t>adate.diffInYears(data('OUTDATE'), data('POLIO3'))&lt;0 &amp;&amp; data('POLIO3') != null &amp;&amp; data('POLIO3') != 'D:2,M:2,Y:1922'</t>
+  </si>
+  <si>
+    <t>adate.diffInYears(data('POLIO2'), data('POLIO3'))&lt;0  &amp;&amp; data('POLIO3') != null &amp;&amp; data('POLIO3') != 'D:2,M:2,Y:1922'</t>
+  </si>
+  <si>
+    <t>adate.diffInYears(data('POLIO1'), data('POLIO3'))&lt;0  &amp;&amp; data('POLIO3') != null &amp;&amp; data('POLIO3') != 'D:2,M:2,Y:1922'</t>
+  </si>
+  <si>
+    <t>adate.diffInYears(data('OUTDATE'), data('PCV3'))&lt;0 &amp;&amp; data('PCV3') != null &amp;&amp; data('PCV3') != 'D:2,M:2,Y:1922'</t>
+  </si>
+  <si>
+    <t>adate.diffInYears(data('PCV2'), data('PCV3'))&lt;0  &amp;&amp; data('PCV3') != null &amp;&amp; data('PCV3') != 'D:2,M:2,Y:1922'</t>
+  </si>
+  <si>
+    <t>adate.diffInYears(data('PCV1'), data('PCV3'))&lt;0  &amp;&amp; data('PCV3') != null &amp;&amp; data('PCV3') != 'D:2,M:2,Y:1922'</t>
+  </si>
+  <si>
+    <t>adate.diffInYears(data('OUTDATE'), data('VPI'))&lt;0 &amp;&amp; data('VPI') != null &amp;&amp; data('VPI') != 'D:2,M:2,Y:1922'</t>
+  </si>
+  <si>
+    <t>adate.diffInYears(data('OUTDATE'), data('SARAMPO1'))&lt;0 &amp;&amp; data('SARAMPO') != null &amp;&amp; data('SARAMPO') != 'D:2,M:2,Y:1922'</t>
+  </si>
+  <si>
+    <t>adate.diffInYears(data('OUTDATE'), data('FEBAMAREL'))&lt;0 &amp;&amp; data('FEBAMAREL') != null &amp;&amp; data('FEBAMAREL') != 'D:2,M:2,Y:1922'</t>
   </si>
 </sst>
 </file>
@@ -4373,322 +4370,322 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>887</v>
+        <v>861</v>
       </c>
       <c r="B18" t="s">
-        <v>908</v>
+        <v>882</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>892</v>
+        <v>866</v>
       </c>
       <c r="B19" t="s">
-        <v>910</v>
+        <v>884</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>893</v>
+        <v>867</v>
       </c>
       <c r="B20" t="s">
-        <v>909</v>
+        <v>883</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>894</v>
+        <v>868</v>
       </c>
       <c r="B21" t="s">
-        <v>911</v>
+        <v>885</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>902</v>
+        <v>876</v>
       </c>
       <c r="B22" t="s">
-        <v>912</v>
+        <v>886</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>903</v>
+        <v>877</v>
       </c>
       <c r="B23" t="s">
-        <v>913</v>
+        <v>887</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>904</v>
+        <v>878</v>
       </c>
       <c r="B24" t="s">
-        <v>914</v>
+        <v>888</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>905</v>
+        <v>879</v>
       </c>
       <c r="B25" t="s">
-        <v>915</v>
+        <v>889</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>906</v>
+        <v>880</v>
       </c>
       <c r="B26" t="s">
-        <v>916</v>
+        <v>890</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>907</v>
+        <v>881</v>
       </c>
       <c r="B27" t="s">
-        <v>917</v>
+        <v>891</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1038</v>
+        <v>1009</v>
       </c>
       <c r="B28" t="s">
-        <v>1042</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1039</v>
+        <v>1010</v>
       </c>
       <c r="B29" t="s">
-        <v>1043</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1046</v>
+        <v>1017</v>
       </c>
       <c r="B30" t="s">
-        <v>1129</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1047</v>
+        <v>1018</v>
       </c>
       <c r="B31" t="s">
-        <v>1128</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1048</v>
+        <v>1019</v>
       </c>
       <c r="B32" t="s">
-        <v>1127</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1049</v>
+        <v>1020</v>
       </c>
       <c r="B33" t="s">
-        <v>1126</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1050</v>
+        <v>1021</v>
       </c>
       <c r="B34" t="s">
-        <v>1125</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1051</v>
+        <v>1022</v>
       </c>
       <c r="B35" t="s">
-        <v>1124</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>1052</v>
+        <v>1023</v>
       </c>
       <c r="B36" t="s">
-        <v>1123</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>1053</v>
+        <v>1024</v>
       </c>
       <c r="B37" t="s">
-        <v>1122</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1054</v>
+        <v>1025</v>
       </c>
       <c r="B38" t="s">
-        <v>1121</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>1055</v>
+        <v>1026</v>
       </c>
       <c r="B39" t="s">
-        <v>1120</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1056</v>
+        <v>1027</v>
       </c>
       <c r="B40" t="s">
-        <v>1119</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1057</v>
+        <v>1028</v>
       </c>
       <c r="B41" t="s">
-        <v>1118</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>1058</v>
+        <v>1029</v>
       </c>
       <c r="B42" t="s">
-        <v>1117</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>1059</v>
+        <v>1030</v>
       </c>
       <c r="B43" t="s">
-        <v>1116</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>1060</v>
+        <v>1031</v>
       </c>
       <c r="B44" t="s">
-        <v>1115</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>1061</v>
+        <v>1032</v>
       </c>
       <c r="B45" t="s">
-        <v>1114</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>1062</v>
+        <v>1033</v>
       </c>
       <c r="B46" t="s">
-        <v>1113</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>1063</v>
+        <v>1034</v>
       </c>
       <c r="B47" t="s">
-        <v>1112</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>1064</v>
+        <v>1035</v>
       </c>
       <c r="B48" t="s">
-        <v>1111</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>1065</v>
+        <v>1036</v>
       </c>
       <c r="B49" t="s">
-        <v>1110</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>1066</v>
+        <v>1037</v>
       </c>
       <c r="B50" t="s">
-        <v>1109</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>1067</v>
+        <v>1038</v>
       </c>
       <c r="B51" t="s">
-        <v>1108</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>1068</v>
+        <v>1039</v>
       </c>
       <c r="B52" t="s">
-        <v>1107</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>1069</v>
+        <v>1040</v>
       </c>
       <c r="B53" t="s">
-        <v>1106</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>1070</v>
+        <v>1041</v>
       </c>
       <c r="B54" t="s">
-        <v>1105</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>1071</v>
+        <v>1042</v>
       </c>
       <c r="B55" t="s">
-        <v>1104</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>1072</v>
+        <v>1043</v>
       </c>
       <c r="B56" t="s">
-        <v>1103</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B57" t="s">
         <v>1073</v>
-      </c>
-      <c r="B57" t="s">
-        <v>1102</v>
       </c>
     </row>
   </sheetData>
@@ -5505,7 +5502,7 @@
         <v>254</v>
       </c>
       <c r="D38" s="57" t="s">
-        <v>1025</v>
+        <v>996</v>
       </c>
       <c r="E38" s="57"/>
     </row>
@@ -5521,7 +5518,7 @@
         <v>252</v>
       </c>
       <c r="D39" s="57" t="s">
-        <v>1026</v>
+        <v>997</v>
       </c>
       <c r="E39" s="57"/>
     </row>
@@ -5537,7 +5534,7 @@
         <v>253</v>
       </c>
       <c r="D40" s="57" t="s">
-        <v>1027</v>
+        <v>998</v>
       </c>
       <c r="E40" s="57"/>
     </row>
@@ -5678,7 +5675,7 @@
         <v>628</v>
       </c>
       <c r="D49" s="57" t="s">
-        <v>1028</v>
+        <v>999</v>
       </c>
       <c r="E49" s="57"/>
     </row>
@@ -5837,7 +5834,7 @@
         <v>643</v>
       </c>
       <c r="D59" s="60" t="s">
-        <v>1029</v>
+        <v>1000</v>
       </c>
       <c r="E59" s="60"/>
     </row>
@@ -5885,7 +5882,7 @@
         <v>534</v>
       </c>
       <c r="D62" s="57" t="s">
-        <v>1030</v>
+        <v>1001</v>
       </c>
       <c r="E62" s="57"/>
     </row>
@@ -5917,7 +5914,7 @@
         <v>548</v>
       </c>
       <c r="D64" s="57" t="s">
-        <v>1000</v>
+        <v>971</v>
       </c>
       <c r="E64" s="57"/>
     </row>
@@ -5933,7 +5930,7 @@
         <v>553</v>
       </c>
       <c r="D65" s="57" t="s">
-        <v>1031</v>
+        <v>1002</v>
       </c>
       <c r="E65" s="57"/>
     </row>
@@ -5949,7 +5946,7 @@
         <v>558</v>
       </c>
       <c r="D66" s="57" t="s">
-        <v>1004</v>
+        <v>975</v>
       </c>
       <c r="E66" s="57"/>
     </row>
@@ -5965,7 +5962,7 @@
         <v>645</v>
       </c>
       <c r="D67" s="57" t="s">
-        <v>1032</v>
+        <v>1003</v>
       </c>
       <c r="E67" s="57"/>
     </row>
@@ -6077,7 +6074,7 @@
         <v>651</v>
       </c>
       <c r="D74" s="57" t="s">
-        <v>1033</v>
+        <v>1004</v>
       </c>
       <c r="E74" s="57"/>
     </row>
@@ -6093,7 +6090,7 @@
         <v>682</v>
       </c>
       <c r="D75" s="57" t="s">
-        <v>1034</v>
+        <v>1005</v>
       </c>
       <c r="E75" s="57"/>
     </row>
@@ -6109,7 +6106,7 @@
         <v>651</v>
       </c>
       <c r="D76" s="57" t="s">
-        <v>1033</v>
+        <v>1004</v>
       </c>
       <c r="E76" s="57"/>
     </row>
@@ -6125,7 +6122,7 @@
         <v>683</v>
       </c>
       <c r="D77" s="57" t="s">
-        <v>1035</v>
+        <v>1006</v>
       </c>
       <c r="E77" s="57"/>
     </row>
@@ -6141,7 +6138,7 @@
         <v>651</v>
       </c>
       <c r="D78" s="57" t="s">
-        <v>1033</v>
+        <v>1004</v>
       </c>
       <c r="E78" s="57"/>
     </row>
@@ -6157,7 +6154,7 @@
         <v>684</v>
       </c>
       <c r="D79" s="57" t="s">
-        <v>1036</v>
+        <v>1007</v>
       </c>
       <c r="E79" s="57"/>
     </row>
@@ -6173,7 +6170,7 @@
         <v>651</v>
       </c>
       <c r="D80" s="57" t="s">
-        <v>1033</v>
+        <v>1004</v>
       </c>
       <c r="E80" s="57"/>
     </row>
@@ -8796,7 +8793,7 @@
         <v>88</v>
       </c>
       <c r="C2" t="s">
-        <v>1130</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -8826,10 +8823,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31E2D9B7-AFA3-430F-905F-12902E548477}">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8907,7 +8904,7 @@
         <v>715</v>
       </c>
       <c r="H4" t="s">
-        <v>931</v>
+        <v>903</v>
       </c>
       <c r="I4" s="55"/>
     </row>
@@ -8928,7 +8925,7 @@
         <v>721</v>
       </c>
       <c r="H6" s="55" t="s">
-        <v>927</v>
+        <v>899</v>
       </c>
       <c r="I6" s="55"/>
     </row>
@@ -8955,7 +8952,7 @@
         <v>723</v>
       </c>
       <c r="H9" s="55" t="s">
-        <v>928</v>
+        <v>900</v>
       </c>
       <c r="I9" s="55"/>
     </row>
@@ -9036,7 +9033,7 @@
         <v>717</v>
       </c>
       <c r="H17" t="s">
-        <v>930</v>
+        <v>902</v>
       </c>
       <c r="I17" s="55"/>
     </row>
@@ -9054,107 +9051,107 @@
         <v>755</v>
       </c>
       <c r="H18" s="55" t="s">
-        <v>1131</v>
+        <v>1102</v>
       </c>
       <c r="I18" s="55"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
-        <v>120</v>
-      </c>
-      <c r="F19" t="s">
-        <v>275</v>
-      </c>
-      <c r="G19" t="s">
-        <v>919</v>
-      </c>
-      <c r="H19" t="s">
-        <v>919</v>
+      <c r="B19" t="s">
+        <v>47</v>
       </c>
       <c r="I19" s="55"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>88</v>
+      </c>
+      <c r="C20" t="s">
+        <v>710</v>
       </c>
       <c r="I20" s="55"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
       <c r="B21" t="s">
-        <v>88</v>
-      </c>
-      <c r="C21" t="s">
-        <v>710</v>
+        <v>46</v>
       </c>
       <c r="I21" s="55"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>46</v>
+      <c r="D22" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" t="s">
+        <v>707</v>
+      </c>
+      <c r="G22" t="s">
+        <v>74</v>
+      </c>
+      <c r="H22" t="s">
+        <v>75</v>
       </c>
       <c r="I22" s="55"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>72</v>
+        <v>120</v>
       </c>
       <c r="F23" t="s">
-        <v>707</v>
+        <v>41</v>
       </c>
       <c r="G23" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="H23" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="I23" s="55"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>120</v>
+        <v>22</v>
+      </c>
+      <c r="E24" t="s">
+        <v>76</v>
       </c>
       <c r="F24" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="G24" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I24" s="55"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>22</v>
-      </c>
-      <c r="E25" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F25" t="s">
-        <v>77</v>
+        <v>118</v>
       </c>
       <c r="G25" t="s">
-        <v>84</v>
+        <v>733</v>
       </c>
       <c r="H25" t="s">
-        <v>85</v>
+        <v>735</v>
       </c>
       <c r="I25" s="55"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="F26" t="s">
-        <v>118</v>
+        <v>66</v>
       </c>
       <c r="G26" t="s">
-        <v>733</v>
+        <v>67</v>
       </c>
       <c r="H26" t="s">
-        <v>735</v>
+        <v>67</v>
       </c>
       <c r="I26" s="55"/>
     </row>
@@ -9163,13 +9160,13 @@
         <v>25</v>
       </c>
       <c r="F27" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G27" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H27" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I27" s="55"/>
     </row>
@@ -9178,40 +9175,37 @@
         <v>25</v>
       </c>
       <c r="F28" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G28" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H28" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="I28" s="55"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D29" t="s">
-        <v>25</v>
-      </c>
-      <c r="F29" t="s">
-        <v>70</v>
-      </c>
-      <c r="G29" t="s">
-        <v>71</v>
-      </c>
-      <c r="H29" t="s">
-        <v>71</v>
+      <c r="B29" t="s">
+        <v>47</v>
       </c>
       <c r="I29" s="55"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I30" s="55"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>46</v>
+      <c r="D31" t="s">
+        <v>149</v>
+      </c>
+      <c r="G31" t="s">
+        <v>713</v>
+      </c>
+      <c r="H31" t="s">
+        <v>714</v>
       </c>
       <c r="I31" s="55"/>
     </row>
@@ -9220,10 +9214,10 @@
         <v>149</v>
       </c>
       <c r="G32" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="H32" t="s">
-        <v>714</v>
+        <v>903</v>
       </c>
       <c r="I32" s="55"/>
     </row>
@@ -9232,10 +9226,10 @@
         <v>149</v>
       </c>
       <c r="G33" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="H33" t="s">
-        <v>931</v>
+        <v>712</v>
       </c>
       <c r="I33" s="55"/>
     </row>
@@ -9244,10 +9238,10 @@
         <v>149</v>
       </c>
       <c r="G34" t="s">
-        <v>711</v>
+        <v>734</v>
       </c>
       <c r="H34" t="s">
-        <v>712</v>
+        <v>736</v>
       </c>
       <c r="I34" s="55"/>
     </row>
@@ -9256,10 +9250,10 @@
         <v>149</v>
       </c>
       <c r="G35" t="s">
-        <v>734</v>
+        <v>722</v>
       </c>
       <c r="H35" t="s">
-        <v>736</v>
+        <v>722</v>
       </c>
       <c r="I35" s="55"/>
     </row>
@@ -9268,10 +9262,10 @@
         <v>149</v>
       </c>
       <c r="G36" t="s">
-        <v>722</v>
+        <v>716</v>
       </c>
       <c r="H36" t="s">
-        <v>722</v>
+        <v>716</v>
       </c>
       <c r="I36" s="55"/>
     </row>
@@ -9280,39 +9274,27 @@
         <v>149</v>
       </c>
       <c r="G37" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="H37" t="s">
-        <v>716</v>
+        <v>902</v>
       </c>
       <c r="I37" s="55"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D38" t="s">
-        <v>149</v>
-      </c>
-      <c r="G38" t="s">
-        <v>717</v>
-      </c>
-      <c r="H38" t="s">
-        <v>930</v>
+      <c r="B38" t="s">
+        <v>47</v>
       </c>
       <c r="I38" s="55"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
       <c r="B39" t="s">
-        <v>47</v>
-      </c>
-      <c r="I39" s="55"/>
+        <v>103</v>
+      </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
       <c r="B40" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
         <v>259</v>
       </c>
     </row>
@@ -9326,8 +9308,8 @@
   <dimension ref="A1:N46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9641,7 +9623,7 @@
         <v>307</v>
       </c>
       <c r="H21" s="55" t="s">
-        <v>932</v>
+        <v>904</v>
       </c>
       <c r="I21" s="55"/>
       <c r="J21" s="55"/>
@@ -9704,7 +9686,7 @@
         <v>71</v>
       </c>
       <c r="H25" s="55" t="s">
-        <v>929</v>
+        <v>901</v>
       </c>
       <c r="I25" s="55" t="s">
         <v>702</v>
@@ -9786,7 +9768,7 @@
         <v>71</v>
       </c>
       <c r="H32" s="55" t="s">
-        <v>929</v>
+        <v>901</v>
       </c>
       <c r="I32" s="55"/>
       <c r="J32" s="55"/>
@@ -9853,7 +9835,7 @@
         <v>95</v>
       </c>
       <c r="H38" s="55" t="s">
-        <v>933</v>
+        <v>905</v>
       </c>
       <c r="I38" s="55"/>
       <c r="J38" s="55"/>
@@ -9880,7 +9862,7 @@
         <v>104</v>
       </c>
       <c r="H40" s="55" t="s">
-        <v>934</v>
+        <v>906</v>
       </c>
       <c r="I40" s="55"/>
       <c r="J40" s="55"/>
@@ -9931,7 +9913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB22453C-0017-476B-BA31-56D5A3D2A587}">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B58" sqref="B58"/>
     </sheetView>
@@ -10119,7 +10101,7 @@
         <v>174</v>
       </c>
       <c r="H14" s="55" t="s">
-        <v>935</v>
+        <v>907</v>
       </c>
       <c r="I14" s="55"/>
       <c r="J14" s="55"/>
@@ -10152,7 +10134,7 @@
         <v>140</v>
       </c>
       <c r="H17" s="55" t="s">
-        <v>936</v>
+        <v>908</v>
       </c>
       <c r="I17" s="55"/>
       <c r="J17" s="55"/>
@@ -10425,10 +10407,10 @@
         <v>149</v>
       </c>
       <c r="G43" s="54" t="s">
-        <v>937</v>
+        <v>909</v>
       </c>
       <c r="H43" s="55" t="s">
-        <v>937</v>
+        <v>909</v>
       </c>
       <c r="I43" s="55"/>
       <c r="J43" s="55"/>
@@ -10510,7 +10492,7 @@
         <v>165</v>
       </c>
       <c r="H50" s="55" t="s">
-        <v>938</v>
+        <v>910</v>
       </c>
       <c r="I50" s="55"/>
       <c r="J50" s="55"/>
@@ -10543,7 +10525,7 @@
         <v>168</v>
       </c>
       <c r="H53" s="55" t="s">
-        <v>939</v>
+        <v>911</v>
       </c>
       <c r="I53" s="55"/>
       <c r="J53" s="55"/>
@@ -10576,7 +10558,7 @@
         <v>171</v>
       </c>
       <c r="H56" s="55" t="s">
-        <v>940</v>
+        <v>912</v>
       </c>
       <c r="I56" s="55"/>
       <c r="J56" s="55"/>
@@ -10600,9 +10582,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35657444-F5E1-4936-AB00-D82A0F63E5F4}">
   <dimension ref="A1:M166"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J44" sqref="J44"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10837,10 +10819,10 @@
         <v>149</v>
       </c>
       <c r="G22" s="55" t="s">
-        <v>918</v>
+        <v>892</v>
       </c>
       <c r="H22" s="55" t="s">
-        <v>918</v>
+        <v>892</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -10885,13 +10867,13 @@
         <v>270</v>
       </c>
       <c r="K25" s="55" t="s">
-        <v>921</v>
+        <v>1103</v>
       </c>
       <c r="L25" s="55" t="s">
-        <v>920</v>
+        <v>893</v>
       </c>
       <c r="M25" s="55" t="s">
-        <v>920</v>
+        <v>893</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -11027,7 +11009,7 @@
         <v>284</v>
       </c>
       <c r="H40" s="55" t="s">
-        <v>941</v>
+        <v>913</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -11051,16 +11033,16 @@
         <v>286</v>
       </c>
       <c r="H42" s="55" t="s">
-        <v>942</v>
+        <v>914</v>
       </c>
       <c r="K42" s="55" t="s">
-        <v>1037</v>
+        <v>1008</v>
       </c>
       <c r="L42" s="55" t="s">
-        <v>924</v>
+        <v>896</v>
       </c>
       <c r="M42" s="55" t="s">
-        <v>924</v>
+        <v>896</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -11075,7 +11057,7 @@
         <v>287</v>
       </c>
       <c r="H43" s="55" t="s">
-        <v>943</v>
+        <v>915</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -11124,7 +11106,7 @@
         <v>289</v>
       </c>
       <c r="H49" s="55" t="s">
-        <v>944</v>
+        <v>916</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
@@ -11148,16 +11130,16 @@
         <v>291</v>
       </c>
       <c r="H51" s="55" t="s">
-        <v>945</v>
+        <v>917</v>
       </c>
       <c r="K51" s="55" t="s">
-        <v>922</v>
+        <v>894</v>
       </c>
       <c r="L51" s="55" t="s">
-        <v>925</v>
+        <v>897</v>
       </c>
       <c r="M51" s="55" t="s">
-        <v>925</v>
+        <v>897</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
@@ -11172,7 +11154,7 @@
         <v>292</v>
       </c>
       <c r="H52" s="55" t="s">
-        <v>946</v>
+        <v>918</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
@@ -11213,7 +11195,7 @@
         <v>294</v>
       </c>
       <c r="H57" s="55" t="s">
-        <v>947</v>
+        <v>919</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -11231,7 +11213,7 @@
         <v>297</v>
       </c>
       <c r="H58" s="55" t="s">
-        <v>948</v>
+        <v>920</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
@@ -11258,7 +11240,7 @@
         <v>301</v>
       </c>
       <c r="H60" s="55" t="s">
-        <v>949</v>
+        <v>921</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
@@ -11294,7 +11276,7 @@
         <v>303</v>
       </c>
       <c r="H64" s="55" t="s">
-        <v>950</v>
+        <v>922</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
@@ -11312,7 +11294,7 @@
         <v>305</v>
       </c>
       <c r="H65" s="55" t="s">
-        <v>951</v>
+        <v>923</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
@@ -11350,7 +11332,7 @@
         <v>307</v>
       </c>
       <c r="H69" s="55" t="s">
-        <v>952</v>
+        <v>924</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
@@ -11374,16 +11356,16 @@
         <v>309</v>
       </c>
       <c r="H71" s="55" t="s">
-        <v>953</v>
+        <v>925</v>
       </c>
       <c r="K71" s="55" t="s">
-        <v>923</v>
+        <v>895</v>
       </c>
       <c r="L71" s="55" t="s">
-        <v>926</v>
+        <v>898</v>
       </c>
       <c r="M71" s="55" t="s">
-        <v>926</v>
+        <v>898</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
@@ -11398,7 +11380,7 @@
         <v>310</v>
       </c>
       <c r="H72" s="55" t="s">
-        <v>954</v>
+        <v>926</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
@@ -11413,7 +11395,7 @@
         <v>311</v>
       </c>
       <c r="H73" s="55" t="s">
-        <v>955</v>
+        <v>927</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
@@ -11459,7 +11441,7 @@
         <v>313</v>
       </c>
       <c r="H79" s="55" t="s">
-        <v>956</v>
+        <v>928</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
@@ -11541,7 +11523,7 @@
         <v>318</v>
       </c>
       <c r="H89" s="55" t="s">
-        <v>957</v>
+        <v>1104</v>
       </c>
       <c r="K89" s="55" t="s">
         <v>810</v>
@@ -11580,7 +11562,7 @@
         <v>321</v>
       </c>
       <c r="H92" s="55" t="s">
-        <v>958</v>
+        <v>929</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
@@ -11616,7 +11598,7 @@
         <v>324</v>
       </c>
       <c r="H96" s="55" t="s">
-        <v>959</v>
+        <v>930</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -11631,7 +11613,7 @@
         <v>326</v>
       </c>
       <c r="H97" s="55" t="s">
-        <v>960</v>
+        <v>931</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -11667,7 +11649,7 @@
         <v>328</v>
       </c>
       <c r="H101" s="55" t="s">
-        <v>961</v>
+        <v>932</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -11694,7 +11676,7 @@
         <v>331</v>
       </c>
       <c r="H103" s="55" t="s">
-        <v>962</v>
+        <v>933</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -11796,7 +11778,7 @@
         <v>376</v>
       </c>
       <c r="H115" s="55" t="s">
-        <v>978</v>
+        <v>949</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -12257,9 +12239,9 @@
   <dimension ref="A1:M77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomLeft" activeCell="F35" sqref="F35:G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12346,7 +12328,7 @@
         <v>334</v>
       </c>
       <c r="H4" s="55" t="s">
-        <v>963</v>
+        <v>934</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -12388,7 +12370,7 @@
         <v>337</v>
       </c>
       <c r="H8" s="55" t="s">
-        <v>964</v>
+        <v>935</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -12420,7 +12402,7 @@
         <v>340</v>
       </c>
       <c r="H11" s="55" t="s">
-        <v>965</v>
+        <v>936</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -12445,7 +12427,7 @@
         <v>343</v>
       </c>
       <c r="H13" s="55" t="s">
-        <v>966</v>
+        <v>937</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -12463,7 +12445,7 @@
         <v>345</v>
       </c>
       <c r="H14" s="55" t="s">
-        <v>967</v>
+        <v>938</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -12512,7 +12494,7 @@
         <v>347</v>
       </c>
       <c r="H19" s="55" t="s">
-        <v>968</v>
+        <v>939</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -12537,7 +12519,7 @@
         <v>347</v>
       </c>
       <c r="H21" s="55" t="s">
-        <v>968</v>
+        <v>939</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -12576,7 +12558,7 @@
         <v>350</v>
       </c>
       <c r="H25" s="55" t="s">
-        <v>969</v>
+        <v>940</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -12608,7 +12590,7 @@
         <v>352</v>
       </c>
       <c r="H28" s="55" t="s">
-        <v>970</v>
+        <v>941</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -12633,7 +12615,7 @@
         <v>355</v>
       </c>
       <c r="H30" s="55" t="s">
-        <v>971</v>
+        <v>942</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -12682,7 +12664,7 @@
         <v>357</v>
       </c>
       <c r="H35" s="55" t="s">
-        <v>972</v>
+        <v>943</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -12707,7 +12689,7 @@
         <v>360</v>
       </c>
       <c r="H37" s="55" t="s">
-        <v>973</v>
+        <v>944</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -12753,7 +12735,7 @@
         <v>362</v>
       </c>
       <c r="H42" s="55" t="s">
-        <v>974</v>
+        <v>945</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -12778,7 +12760,7 @@
         <v>343</v>
       </c>
       <c r="H44" s="55" t="s">
-        <v>975</v>
+        <v>946</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -12796,7 +12778,7 @@
         <v>345</v>
       </c>
       <c r="H45" s="55" t="s">
-        <v>967</v>
+        <v>938</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -12845,7 +12827,7 @@
         <v>347</v>
       </c>
       <c r="H50" s="55" t="s">
-        <v>968</v>
+        <v>939</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -12870,7 +12852,7 @@
         <v>347</v>
       </c>
       <c r="H52" s="55" t="s">
-        <v>968</v>
+        <v>939</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -12909,7 +12891,7 @@
         <v>350</v>
       </c>
       <c r="H56" s="55" t="s">
-        <v>969</v>
+        <v>940</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -12941,7 +12923,7 @@
         <v>352</v>
       </c>
       <c r="H59" s="55" t="s">
-        <v>976</v>
+        <v>947</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -12966,7 +12948,7 @@
         <v>355</v>
       </c>
       <c r="H61" s="55" t="s">
-        <v>977</v>
+        <v>948</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -13015,7 +12997,7 @@
         <v>357</v>
       </c>
       <c r="H66" s="55" t="s">
-        <v>972</v>
+        <v>943</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -13040,7 +13022,7 @@
         <v>360</v>
       </c>
       <c r="H68" s="55" t="s">
-        <v>973</v>
+        <v>944</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -13099,7 +13081,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H77" s="55" t="s">
-        <v>978</v>
+        <v>949</v>
       </c>
     </row>
   </sheetData>
@@ -13111,9 +13093,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A7F4833-88F1-44B1-8A75-76AFCBB7BC62}">
   <dimension ref="A1:M316"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A300" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H317" sqref="H317"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D306" sqref="D306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13404,7 +13386,7 @@
         <v>88</v>
       </c>
       <c r="C29" t="s">
-        <v>862</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -13416,7 +13398,7 @@
         <v>815</v>
       </c>
       <c r="H30" t="s">
-        <v>1074</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -13431,7 +13413,7 @@
         <v>88</v>
       </c>
       <c r="C32" t="s">
-        <v>861</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -13443,7 +13425,7 @@
         <v>816</v>
       </c>
       <c r="H33" t="s">
-        <v>1075</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -13960,7 +13942,7 @@
         <v>88</v>
       </c>
       <c r="C94" t="s">
-        <v>863</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -13972,7 +13954,7 @@
         <v>819</v>
       </c>
       <c r="H95" t="s">
-        <v>1076</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -13987,7 +13969,7 @@
         <v>88</v>
       </c>
       <c r="C97" t="s">
-        <v>864</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -13999,7 +13981,7 @@
         <v>820</v>
       </c>
       <c r="H98" t="s">
-        <v>1077</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -14014,7 +13996,7 @@
         <v>88</v>
       </c>
       <c r="C100" t="s">
-        <v>865</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -14026,7 +14008,7 @@
         <v>826</v>
       </c>
       <c r="H101" t="s">
-        <v>1078</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -14041,7 +14023,7 @@
         <v>88</v>
       </c>
       <c r="C103" t="s">
-        <v>866</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
@@ -14053,7 +14035,7 @@
         <v>821</v>
       </c>
       <c r="H104" t="s">
-        <v>1079</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
@@ -14570,7 +14552,7 @@
         <v>88</v>
       </c>
       <c r="C165" t="s">
-        <v>867</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
@@ -14582,7 +14564,7 @@
         <v>831</v>
       </c>
       <c r="H166" t="s">
-        <v>1080</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
@@ -14597,7 +14579,7 @@
         <v>88</v>
       </c>
       <c r="C168" t="s">
-        <v>868</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
@@ -14609,7 +14591,7 @@
         <v>832</v>
       </c>
       <c r="H169" t="s">
-        <v>1081</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
@@ -14624,7 +14606,7 @@
         <v>88</v>
       </c>
       <c r="C171" t="s">
-        <v>869</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
@@ -14636,7 +14618,7 @@
         <v>833</v>
       </c>
       <c r="H172" t="s">
-        <v>1082</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
@@ -14651,7 +14633,7 @@
         <v>88</v>
       </c>
       <c r="C174" t="s">
-        <v>870</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
@@ -14663,7 +14645,7 @@
         <v>834</v>
       </c>
       <c r="H175" t="s">
-        <v>1083</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
@@ -14678,7 +14660,7 @@
         <v>88</v>
       </c>
       <c r="C177" t="s">
-        <v>871</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
@@ -14687,10 +14669,10 @@
         <v>149</v>
       </c>
       <c r="G178" t="s">
-        <v>888</v>
+        <v>862</v>
       </c>
       <c r="H178" t="s">
-        <v>1084</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
@@ -14705,7 +14687,7 @@
         <v>88</v>
       </c>
       <c r="C180" t="s">
-        <v>872</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
@@ -14714,10 +14696,10 @@
         <v>149</v>
       </c>
       <c r="G181" t="s">
-        <v>889</v>
+        <v>863</v>
       </c>
       <c r="H181" t="s">
-        <v>1085</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
@@ -14732,7 +14714,7 @@
         <v>88</v>
       </c>
       <c r="C183" t="s">
-        <v>873</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">
@@ -14741,10 +14723,10 @@
         <v>149</v>
       </c>
       <c r="G184" t="s">
-        <v>890</v>
+        <v>864</v>
       </c>
       <c r="H184" t="s">
-        <v>1086</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
@@ -14759,7 +14741,7 @@
         <v>88</v>
       </c>
       <c r="C186" t="s">
-        <v>874</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.25">
@@ -14768,10 +14750,10 @@
         <v>149</v>
       </c>
       <c r="G187" t="s">
-        <v>891</v>
+        <v>865</v>
       </c>
       <c r="H187" t="s">
-        <v>1087</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.25">
@@ -15288,7 +15270,7 @@
         <v>88</v>
       </c>
       <c r="C248" t="s">
-        <v>875</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="249" spans="1:8" x14ac:dyDescent="0.25">
@@ -15300,7 +15282,7 @@
         <v>843</v>
       </c>
       <c r="H249" t="s">
-        <v>1088</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="250" spans="1:8" x14ac:dyDescent="0.25">
@@ -15315,7 +15297,7 @@
         <v>88</v>
       </c>
       <c r="C251" t="s">
-        <v>876</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.25">
@@ -15327,7 +15309,7 @@
         <v>844</v>
       </c>
       <c r="H252" t="s">
-        <v>1089</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="253" spans="1:8" x14ac:dyDescent="0.25">
@@ -15342,7 +15324,7 @@
         <v>88</v>
       </c>
       <c r="C254" t="s">
-        <v>877</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="255" spans="1:8" x14ac:dyDescent="0.25">
@@ -15354,7 +15336,7 @@
         <v>845</v>
       </c>
       <c r="H255" t="s">
-        <v>1090</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="256" spans="1:8" x14ac:dyDescent="0.25">
@@ -15369,7 +15351,7 @@
         <v>88</v>
       </c>
       <c r="C257" t="s">
-        <v>878</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.25">
@@ -15378,10 +15360,10 @@
         <v>149</v>
       </c>
       <c r="G258" t="s">
-        <v>895</v>
+        <v>869</v>
       </c>
       <c r="H258" t="s">
-        <v>1091</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.25">
@@ -15396,7 +15378,7 @@
         <v>88</v>
       </c>
       <c r="C260" t="s">
-        <v>879</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="261" spans="1:8" x14ac:dyDescent="0.25">
@@ -15405,10 +15387,10 @@
         <v>149</v>
       </c>
       <c r="G261" t="s">
-        <v>896</v>
+        <v>870</v>
       </c>
       <c r="H261" t="s">
-        <v>1092</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="262" spans="1:8" x14ac:dyDescent="0.25">
@@ -15423,7 +15405,7 @@
         <v>88</v>
       </c>
       <c r="C263" t="s">
-        <v>880</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="264" spans="1:8" x14ac:dyDescent="0.25">
@@ -15432,10 +15414,10 @@
         <v>149</v>
       </c>
       <c r="G264" t="s">
-        <v>897</v>
+        <v>871</v>
       </c>
       <c r="H264" t="s">
-        <v>1093</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="265" spans="1:8" x14ac:dyDescent="0.25">
@@ -15450,7 +15432,7 @@
         <v>88</v>
       </c>
       <c r="C266" t="s">
-        <v>881</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="267" spans="1:8" x14ac:dyDescent="0.25">
@@ -15459,10 +15441,10 @@
         <v>149</v>
       </c>
       <c r="G267" t="s">
-        <v>898</v>
+        <v>872</v>
       </c>
       <c r="H267" t="s">
-        <v>1094</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="268" spans="1:8" x14ac:dyDescent="0.25">
@@ -15477,7 +15459,7 @@
         <v>88</v>
       </c>
       <c r="C269" t="s">
-        <v>882</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="270" spans="1:8" x14ac:dyDescent="0.25">
@@ -15486,10 +15468,10 @@
         <v>149</v>
       </c>
       <c r="G270" t="s">
-        <v>899</v>
+        <v>873</v>
       </c>
       <c r="H270" t="s">
-        <v>1095</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="271" spans="1:8" x14ac:dyDescent="0.25">
@@ -15504,7 +15486,7 @@
         <v>88</v>
       </c>
       <c r="C272" t="s">
-        <v>883</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="273" spans="1:9" x14ac:dyDescent="0.25">
@@ -15513,10 +15495,10 @@
         <v>149</v>
       </c>
       <c r="G273" t="s">
-        <v>900</v>
+        <v>874</v>
       </c>
       <c r="H273" t="s">
-        <v>1096</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="274" spans="1:9" x14ac:dyDescent="0.25">
@@ -15531,7 +15513,7 @@
         <v>88</v>
       </c>
       <c r="C275" t="s">
-        <v>884</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="276" spans="1:9" x14ac:dyDescent="0.25">
@@ -15540,10 +15522,10 @@
         <v>149</v>
       </c>
       <c r="G276" t="s">
-        <v>901</v>
+        <v>875</v>
       </c>
       <c r="H276" t="s">
-        <v>1097</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="277" spans="1:9" x14ac:dyDescent="0.25">
@@ -15778,7 +15760,7 @@
         <v>88</v>
       </c>
       <c r="C304" t="s">
-        <v>886</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="305" spans="1:8" x14ac:dyDescent="0.25">
@@ -15790,7 +15772,7 @@
         <v>855</v>
       </c>
       <c r="H305" t="s">
-        <v>1098</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="306" spans="1:8" x14ac:dyDescent="0.25">
@@ -15805,7 +15787,7 @@
         <v>88</v>
       </c>
       <c r="C307" t="s">
-        <v>885</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="308" spans="1:8" x14ac:dyDescent="0.25">
@@ -15817,7 +15799,7 @@
         <v>854</v>
       </c>
       <c r="H308" t="s">
-        <v>1099</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="309" spans="1:8" x14ac:dyDescent="0.25">
@@ -15832,7 +15814,7 @@
         <v>88</v>
       </c>
       <c r="C310" s="6" t="s">
-        <v>1045</v>
+        <v>1016</v>
       </c>
       <c r="D310" s="50"/>
       <c r="E310" s="50"/>
@@ -15846,10 +15828,10 @@
         <v>149</v>
       </c>
       <c r="G311" s="50" t="s">
-        <v>1040</v>
+        <v>1011</v>
       </c>
       <c r="H311" s="50" t="s">
-        <v>1100</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="312" spans="1:8" x14ac:dyDescent="0.25">
@@ -15864,13 +15846,13 @@
         <v>88</v>
       </c>
       <c r="C313" s="6" t="s">
-        <v>1044</v>
+        <v>1015</v>
       </c>
       <c r="G313" t="s">
-        <v>1041</v>
+        <v>1012</v>
       </c>
       <c r="H313" t="s">
-        <v>1101</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="314" spans="1:8" x14ac:dyDescent="0.25">
@@ -15900,8 +15882,8 @@
   <dimension ref="A1:M147"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I135" sqref="I135"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16057,7 +16039,7 @@
         <v>378</v>
       </c>
       <c r="H10" s="55" t="s">
-        <v>979</v>
+        <v>950</v>
       </c>
       <c r="J10" s="12"/>
     </row>
@@ -16094,7 +16076,7 @@
         <v>388</v>
       </c>
       <c r="H12" s="55" t="s">
-        <v>980</v>
+        <v>951</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -16109,7 +16091,7 @@
         <v>497</v>
       </c>
       <c r="H13" s="55" t="s">
-        <v>981</v>
+        <v>952</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -16141,7 +16123,7 @@
         <v>499</v>
       </c>
       <c r="H16" s="55" t="s">
-        <v>982</v>
+        <v>953</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -16156,7 +16138,7 @@
         <v>501</v>
       </c>
       <c r="H17" s="55" t="s">
-        <v>983</v>
+        <v>954</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -16174,7 +16156,7 @@
         <v>503</v>
       </c>
       <c r="H18" s="55" t="s">
-        <v>984</v>
+        <v>955</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -16192,7 +16174,7 @@
         <v>505</v>
       </c>
       <c r="H19" s="55" t="s">
-        <v>985</v>
+        <v>956</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -16207,7 +16189,7 @@
         <v>507</v>
       </c>
       <c r="H20" s="55" t="s">
-        <v>986</v>
+        <v>957</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -16244,7 +16226,7 @@
         <v>509</v>
       </c>
       <c r="H24" s="55" t="s">
-        <v>987</v>
+        <v>958</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -16259,7 +16241,7 @@
         <v>511</v>
       </c>
       <c r="H25" s="55" t="s">
-        <v>988</v>
+        <v>959</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -16288,7 +16270,7 @@
         <v>509</v>
       </c>
       <c r="H28" s="55" t="s">
-        <v>987</v>
+        <v>958</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -16303,7 +16285,7 @@
         <v>511</v>
       </c>
       <c r="H29" s="55" t="s">
-        <v>988</v>
+        <v>959</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -16335,7 +16317,7 @@
         <v>515</v>
       </c>
       <c r="H32" s="55" t="s">
-        <v>989</v>
+        <v>960</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -16367,7 +16349,7 @@
         <v>517</v>
       </c>
       <c r="H35" s="55" t="s">
-        <v>990</v>
+        <v>961</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -16395,7 +16377,7 @@
         <v>520</v>
       </c>
       <c r="H37" s="55" t="s">
-        <v>991</v>
+        <v>962</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -16434,7 +16416,7 @@
         <v>522</v>
       </c>
       <c r="H41" s="55" t="s">
-        <v>992</v>
+        <v>963</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -16466,7 +16448,7 @@
         <v>524</v>
       </c>
       <c r="H44" s="55" t="s">
-        <v>993</v>
+        <v>964</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -16491,7 +16473,7 @@
         <v>527</v>
       </c>
       <c r="H46" s="55" t="s">
-        <v>994</v>
+        <v>965</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -16530,7 +16512,7 @@
         <v>529</v>
       </c>
       <c r="H50" s="55" t="s">
-        <v>995</v>
+        <v>966</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -16559,7 +16541,7 @@
         <v>532</v>
       </c>
       <c r="H53" s="55" t="s">
-        <v>996</v>
+        <v>967</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -16623,7 +16605,7 @@
         <v>538</v>
       </c>
       <c r="H59" s="55" t="s">
-        <v>997</v>
+        <v>968</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -16687,7 +16669,7 @@
         <v>544</v>
       </c>
       <c r="H65" s="55" t="s">
-        <v>998</v>
+        <v>969</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -16702,7 +16684,7 @@
         <v>546</v>
       </c>
       <c r="H66" s="55" t="s">
-        <v>999</v>
+        <v>970</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -16741,7 +16723,7 @@
         <v>548</v>
       </c>
       <c r="H70" s="55" t="s">
-        <v>1000</v>
+        <v>971</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -16766,7 +16748,7 @@
         <v>551</v>
       </c>
       <c r="H72" s="55" t="s">
-        <v>1001</v>
+        <v>972</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -16805,7 +16787,7 @@
         <v>553</v>
       </c>
       <c r="H76" s="55" t="s">
-        <v>1002</v>
+        <v>973</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -16830,7 +16812,7 @@
         <v>556</v>
       </c>
       <c r="H78" s="55" t="s">
-        <v>1003</v>
+        <v>974</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -16869,7 +16851,7 @@
         <v>558</v>
       </c>
       <c r="H82" s="55" t="s">
-        <v>1004</v>
+        <v>975</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -16894,7 +16876,7 @@
         <v>561</v>
       </c>
       <c r="H84" s="55" t="s">
-        <v>1005</v>
+        <v>976</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -16933,7 +16915,7 @@
         <v>563</v>
       </c>
       <c r="H88" s="55" t="s">
-        <v>1006</v>
+        <v>977</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -16958,7 +16940,7 @@
         <v>566</v>
       </c>
       <c r="H90" s="55" t="s">
-        <v>1007</v>
+        <v>978</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -17022,7 +17004,7 @@
         <v>572</v>
       </c>
       <c r="H96" s="55" t="s">
-        <v>1008</v>
+        <v>979</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -17071,7 +17053,7 @@
         <v>574</v>
       </c>
       <c r="H101" s="55" t="s">
-        <v>1009</v>
+        <v>980</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -17096,7 +17078,7 @@
         <v>577</v>
       </c>
       <c r="H103" s="55" t="s">
-        <v>1010</v>
+        <v>981</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -17139,7 +17121,7 @@
         <v>579</v>
       </c>
       <c r="H108" s="55" t="s">
-        <v>1011</v>
+        <v>982</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -17154,7 +17136,7 @@
         <v>579</v>
       </c>
       <c r="H109" s="55" t="s">
-        <v>1011</v>
+        <v>982</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -17186,7 +17168,7 @@
         <v>582</v>
       </c>
       <c r="H112" s="55" t="s">
-        <v>1012</v>
+        <v>983</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -17230,7 +17212,7 @@
         <v>585</v>
       </c>
       <c r="H116" s="55" t="s">
-        <v>1013</v>
+        <v>984</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -17276,7 +17258,7 @@
         <v>588</v>
       </c>
       <c r="H121" s="55" t="s">
-        <v>1014</v>
+        <v>985</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -17304,7 +17286,7 @@
         <v>591</v>
       </c>
       <c r="H123" s="55" t="s">
-        <v>1015</v>
+        <v>986</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -17340,7 +17322,7 @@
         <v>593</v>
       </c>
       <c r="H127" s="55" t="s">
-        <v>1016</v>
+        <v>987</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -17358,7 +17340,7 @@
         <v>595</v>
       </c>
       <c r="H128" s="55" t="s">
-        <v>1017</v>
+        <v>988</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -17390,7 +17372,7 @@
         <v>597</v>
       </c>
       <c r="H131" s="55" t="s">
-        <v>1018</v>
+        <v>989</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -17408,7 +17390,7 @@
         <v>599</v>
       </c>
       <c r="H132" s="55" t="s">
-        <v>1019</v>
+        <v>990</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
@@ -17447,7 +17429,7 @@
         <v>601</v>
       </c>
       <c r="H136" s="55" t="s">
-        <v>1020</v>
+        <v>991</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
@@ -17472,7 +17454,7 @@
         <v>604</v>
       </c>
       <c r="H138" s="55" t="s">
-        <v>1021</v>
+        <v>992</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
@@ -17511,7 +17493,7 @@
         <v>606</v>
       </c>
       <c r="H142" s="55" t="s">
-        <v>1022</v>
+        <v>993</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
@@ -17536,7 +17518,7 @@
         <v>609</v>
       </c>
       <c r="H144" s="55" t="s">
-        <v>1023</v>
+        <v>994</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
@@ -17551,7 +17533,7 @@
         <v>611</v>
       </c>
       <c r="H145" s="55" t="s">
-        <v>1024</v>
+        <v>995</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updates to quiestions and adding of NS-options
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
+++ b/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE278141-B582-4D26-AB9A-EE3E6EDB5D65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263F9217-0F90-425B-B93B-22ED7EE95B70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="674" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="674" firstSheet="2" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2784" uniqueCount="1131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2819" uniqueCount="1139">
   <si>
     <t>setting_name</t>
   </si>
@@ -3443,6 +3443,30 @@
   </si>
   <si>
     <t>{REGIDC: data('REGIDC'), VISITDATE: data('CONT'), VISITIDC: opendatakit.getCurrentInstanceId()}</t>
+  </si>
+  <si>
+    <t>dontknow</t>
+  </si>
+  <si>
+    <t>cdg_mns</t>
+  </si>
+  <si>
+    <t>data('cdg_mns') != null</t>
+  </si>
+  <si>
+    <t>fedep_mns</t>
+  </si>
+  <si>
+    <t>data('fedep_mns') != null</t>
+  </si>
+  <si>
+    <t>qvfansi_mns</t>
+  </si>
+  <si>
+    <t>data('qvfansi_mns') != null</t>
+  </si>
+  <si>
+    <t>abmesns</t>
   </si>
 </sst>
 </file>
@@ -4222,7 +4246,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A6BCC52-34B1-45EC-BAB5-A647CE434BBE}">
   <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
@@ -4697,9 +4721,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB23FD29-3338-4879-B1BD-848935333D8A}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
+      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4902,11 +4926,11 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF3D0A7-17A8-4B35-89BF-E7F3088D1597}">
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E82" sqref="E82"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6334,6 +6358,21 @@
       </c>
       <c r="E90" s="57"/>
     </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B91" t="str">
+        <f>"99"</f>
+        <v>99</v>
+      </c>
+      <c r="C91" t="s">
+        <v>100</v>
+      </c>
+      <c r="D91" t="s">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6342,11 +6381,11 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
-  <dimension ref="A1:L204"/>
+  <dimension ref="A1:L208"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A183" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D188" sqref="D188"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A198" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A206" sqref="A206:XFD206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8724,8 +8763,52 @@
         <v>0</v>
       </c>
     </row>
+    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B205" t="s">
+        <v>336</v>
+      </c>
+      <c r="C205" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B206" t="s">
+        <v>336</v>
+      </c>
+      <c r="C206" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B207" t="s">
+        <v>336</v>
+      </c>
+      <c r="C207" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B208" t="s">
+        <v>336</v>
+      </c>
+      <c r="C208" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C206">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C205">
     <sortCondition ref="A88"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9307,9 +9390,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
   <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9911,11 +9994,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB22453C-0017-476B-BA31-56D5A3D2A587}">
-  <dimension ref="A1:K58"/>
+  <dimension ref="A1:K70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B58" sqref="B58"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10280,296 +10363,401 @@
       <c r="J30" s="55"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+      <c r="D31" t="s">
+        <v>336</v>
+      </c>
+      <c r="E31" t="s">
+        <v>1131</v>
+      </c>
+      <c r="F31" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>88</v>
       </c>
-      <c r="C31" t="s">
-        <v>155</v>
-      </c>
-      <c r="I31" s="55"/>
-      <c r="J31" s="55"/>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D32" t="s">
-        <v>25</v>
-      </c>
-      <c r="F32" t="s">
-        <v>156</v>
-      </c>
-      <c r="G32" t="s">
-        <v>143</v>
-      </c>
-      <c r="H32" t="s">
-        <v>157</v>
-      </c>
-      <c r="I32" s="55"/>
-      <c r="J32" s="55"/>
+      <c r="C32" t="s">
+        <v>1133</v>
+      </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>103</v>
-      </c>
-      <c r="I33" s="55"/>
-      <c r="J33" s="55"/>
+      <c r="D33" t="s">
+        <v>126</v>
+      </c>
+      <c r="F33" t="s">
+        <v>152</v>
+      </c>
+      <c r="I33">
+        <v>99</v>
+      </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>47</v>
-      </c>
-      <c r="I34" s="55"/>
-      <c r="J34" s="55"/>
+        <v>103</v>
+      </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>46</v>
+        <v>88</v>
+      </c>
+      <c r="C35" t="s">
+        <v>155</v>
       </c>
       <c r="I35" s="55"/>
       <c r="J35" s="55"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>149</v>
+        <v>25</v>
+      </c>
+      <c r="F36" t="s">
+        <v>156</v>
       </c>
       <c r="G36" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="H36" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I36" s="55"/>
       <c r="J36" s="55"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D37" t="s">
-        <v>25</v>
-      </c>
-      <c r="F37" t="s">
-        <v>160</v>
-      </c>
-      <c r="G37" t="s">
-        <v>153</v>
-      </c>
-      <c r="H37" t="s">
-        <v>154</v>
+      <c r="B37" t="s">
+        <v>103</v>
       </c>
       <c r="I37" s="55"/>
       <c r="J37" s="55"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>88</v>
-      </c>
-      <c r="C38" t="s">
-        <v>155</v>
+        <v>47</v>
       </c>
       <c r="I38" s="55"/>
       <c r="J38" s="55"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D39" t="s">
-        <v>25</v>
-      </c>
-      <c r="F39" t="s">
-        <v>161</v>
-      </c>
-      <c r="G39" t="s">
-        <v>143</v>
-      </c>
-      <c r="H39" t="s">
-        <v>157</v>
+      <c r="B39" t="s">
+        <v>46</v>
       </c>
       <c r="I39" s="55"/>
       <c r="J39" s="55"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>103</v>
+      <c r="D40" t="s">
+        <v>149</v>
+      </c>
+      <c r="G40" t="s">
+        <v>158</v>
+      </c>
+      <c r="H40" t="s">
+        <v>159</v>
       </c>
       <c r="I40" s="55"/>
       <c r="J40" s="55"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>47</v>
+      <c r="D41" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" t="s">
+        <v>160</v>
+      </c>
+      <c r="G41" t="s">
+        <v>153</v>
+      </c>
+      <c r="H41" t="s">
+        <v>154</v>
       </c>
       <c r="I41" s="55"/>
       <c r="J41" s="55"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>46</v>
-      </c>
-      <c r="I42" s="55"/>
-      <c r="J42" s="55"/>
+      <c r="D42" t="s">
+        <v>336</v>
+      </c>
+      <c r="E42" t="s">
+        <v>1131</v>
+      </c>
+      <c r="F42" t="s">
+        <v>1134</v>
+      </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D43" t="s">
-        <v>149</v>
-      </c>
-      <c r="G43" s="54" t="s">
-        <v>908</v>
-      </c>
-      <c r="H43" s="55" t="s">
-        <v>908</v>
-      </c>
-      <c r="I43" s="55"/>
-      <c r="J43" s="55"/>
+      <c r="B43" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1135</v>
+      </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>25</v>
+        <v>126</v>
       </c>
       <c r="F44" t="s">
-        <v>162</v>
-      </c>
-      <c r="G44" t="s">
-        <v>153</v>
-      </c>
-      <c r="H44" t="s">
-        <v>154</v>
-      </c>
-      <c r="I44" s="55"/>
-      <c r="J44" s="55"/>
+        <v>160</v>
+      </c>
+      <c r="I44">
+        <v>99</v>
+      </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>88</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>155</v>
-      </c>
-      <c r="I45" s="55"/>
-      <c r="J45" s="55"/>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D46" t="s">
-        <v>25</v>
-      </c>
-      <c r="F46" t="s">
-        <v>163</v>
-      </c>
-      <c r="G46" t="s">
-        <v>143</v>
-      </c>
-      <c r="H46" t="s">
-        <v>157</v>
       </c>
       <c r="I46" s="55"/>
       <c r="J46" s="55"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>103</v>
+      <c r="D47" t="s">
+        <v>25</v>
+      </c>
+      <c r="F47" t="s">
+        <v>161</v>
+      </c>
+      <c r="G47" t="s">
+        <v>143</v>
+      </c>
+      <c r="H47" t="s">
+        <v>157</v>
       </c>
       <c r="I47" s="55"/>
       <c r="J47" s="55"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>47</v>
+        <v>103</v>
       </c>
       <c r="I48" s="55"/>
       <c r="J48" s="55"/>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I49" s="55"/>
       <c r="J49" s="55"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D50" t="s">
-        <v>22</v>
-      </c>
-      <c r="E50" t="s">
-        <v>93</v>
-      </c>
-      <c r="F50" t="s">
-        <v>164</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="H50" s="55" t="s">
-        <v>909</v>
+      <c r="B50" t="s">
+        <v>46</v>
       </c>
       <c r="I50" s="55"/>
       <c r="J50" s="55"/>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>47</v>
+      <c r="D51" t="s">
+        <v>149</v>
+      </c>
+      <c r="G51" s="54" t="s">
+        <v>908</v>
+      </c>
+      <c r="H51" s="55" t="s">
+        <v>908</v>
       </c>
       <c r="I51" s="55"/>
       <c r="J51" s="55"/>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>46</v>
+      <c r="D52" t="s">
+        <v>25</v>
+      </c>
+      <c r="F52" t="s">
+        <v>162</v>
+      </c>
+      <c r="G52" t="s">
+        <v>153</v>
+      </c>
+      <c r="H52" t="s">
+        <v>154</v>
       </c>
       <c r="I52" s="55"/>
       <c r="J52" s="55"/>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
-        <v>22</v>
+        <v>336</v>
       </c>
       <c r="E53" t="s">
-        <v>166</v>
+        <v>1131</v>
       </c>
       <c r="F53" t="s">
-        <v>167</v>
-      </c>
-      <c r="G53" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="H53" s="55" t="s">
-        <v>910</v>
-      </c>
-      <c r="I53" s="55"/>
-      <c r="J53" s="55"/>
+        <v>1136</v>
+      </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>47</v>
-      </c>
-      <c r="I54" s="55"/>
-      <c r="J54" s="55"/>
+        <v>88</v>
+      </c>
+      <c r="C54" t="s">
+        <v>1137</v>
+      </c>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>46</v>
-      </c>
-      <c r="I55" s="55"/>
-      <c r="J55" s="55"/>
+      <c r="D55" t="s">
+        <v>126</v>
+      </c>
+      <c r="F55" t="s">
+        <v>162</v>
+      </c>
+      <c r="I55">
+        <v>99</v>
+      </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D56" t="s">
-        <v>22</v>
-      </c>
-      <c r="E56" t="s">
-        <v>169</v>
-      </c>
-      <c r="F56" t="s">
-        <v>170</v>
-      </c>
-      <c r="G56" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="H56" s="55" t="s">
-        <v>911</v>
-      </c>
-      <c r="I56" s="55"/>
-      <c r="J56" s="55"/>
+      <c r="B56" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
+        <v>88</v>
+      </c>
+      <c r="C57" t="s">
+        <v>155</v>
+      </c>
+      <c r="I57" s="55"/>
+      <c r="J57" s="55"/>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>25</v>
+      </c>
+      <c r="F58" t="s">
+        <v>163</v>
+      </c>
+      <c r="G58" t="s">
+        <v>143</v>
+      </c>
+      <c r="H58" t="s">
+        <v>157</v>
+      </c>
+      <c r="I58" s="55"/>
+      <c r="J58" s="55"/>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>103</v>
+      </c>
+      <c r="I59" s="55"/>
+      <c r="J59" s="55"/>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
+      <c r="I60" s="55"/>
+      <c r="J60" s="55"/>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>46</v>
+      </c>
+      <c r="I61" s="55"/>
+      <c r="J61" s="55"/>
+    </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>22</v>
+      </c>
+      <c r="E62" t="s">
+        <v>93</v>
+      </c>
+      <c r="F62" t="s">
+        <v>164</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="H62" s="55" t="s">
+        <v>909</v>
+      </c>
+      <c r="I62" s="55"/>
+      <c r="J62" s="55"/>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>47</v>
+      </c>
+      <c r="I63" s="55"/>
+      <c r="J63" s="55"/>
+    </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>46</v>
+      </c>
+      <c r="I64" s="55"/>
+      <c r="J64" s="55"/>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>22</v>
+      </c>
+      <c r="E65" t="s">
+        <v>166</v>
+      </c>
+      <c r="F65" t="s">
+        <v>167</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="H65" s="55" t="s">
+        <v>910</v>
+      </c>
+      <c r="I65" s="55"/>
+      <c r="J65" s="55"/>
+    </row>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>47</v>
+      </c>
+      <c r="I66" s="55"/>
+      <c r="J66" s="55"/>
+    </row>
+    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>46</v>
+      </c>
+      <c r="I67" s="55"/>
+      <c r="J67" s="55"/>
+    </row>
+    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>22</v>
+      </c>
+      <c r="E68" t="s">
+        <v>169</v>
+      </c>
+      <c r="F68" t="s">
+        <v>170</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="H68" s="55" t="s">
+        <v>911</v>
+      </c>
+      <c r="I68" s="55"/>
+      <c r="J68" s="55"/>
+    </row>
+    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
         <v>708</v>
       </c>
     </row>
@@ -10583,7 +10771,7 @@
   <dimension ref="A1:M166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Opdatering til CRIANCA visit
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
+++ b/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263F9217-0F90-425B-B93B-22ED7EE95B70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7508124F-0197-4F90-995F-89F3DF2A8063}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="674" firstSheet="2" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2819" uniqueCount="1139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2873" uniqueCount="1152">
   <si>
     <t>setting_name</t>
   </si>
@@ -3467,6 +3467,45 @@
   </si>
   <si>
     <t>abmesns</t>
+  </si>
+  <si>
+    <t>data('NASESTADO') != '1'</t>
+  </si>
+  <si>
+    <t>data('PRES')</t>
+  </si>
+  <si>
+    <t>data('PRES') != '2' &amp;&amp; data('PRES') !='3'</t>
+  </si>
+  <si>
+    <t>dacomsupns</t>
+  </si>
+  <si>
+    <t>data('dacomsupns') != null</t>
+  </si>
+  <si>
+    <t>data('dacomsupns')</t>
+  </si>
+  <si>
+    <t>dontknowdate</t>
+  </si>
+  <si>
+    <t>data('dapamans')</t>
+  </si>
+  <si>
+    <t>dapamans</t>
+  </si>
+  <si>
+    <t>data('dapamans') != null</t>
+  </si>
+  <si>
+    <t>dasepns</t>
+  </si>
+  <si>
+    <t>data('dasepns') != null</t>
+  </si>
+  <si>
+    <t>data('dasepns')</t>
   </si>
 </sst>
 </file>
@@ -3752,7 +3791,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3837,6 +3876,7 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Normal" xfId="2" xr:uid="{C28CC074-D3A0-48A2-81F3-B6A5CA836B7C}"/>
@@ -4926,17 +4966,17 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF3D0A7-17A8-4B35-89BF-E7F3088D1597}">
-  <dimension ref="A1:E91"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C93" sqref="C93"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" style="50" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="50" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="50" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.42578125" style="50" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43" style="50" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.28515625" style="50" bestFit="1" customWidth="1"/>
@@ -6373,6 +6413,21 @@
         <v>83</v>
       </c>
     </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="50" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B92" s="50" t="str">
+        <f>"D:NS,M:NS,Y:NS"</f>
+        <v>D:NS,M:NS,Y:NS</v>
+      </c>
+      <c r="C92" t="s">
+        <v>100</v>
+      </c>
+      <c r="D92" t="s">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6381,11 +6436,11 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
-  <dimension ref="A1:L208"/>
+  <dimension ref="A1:L211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A198" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A206" sqref="A206:XFD206"/>
+      <pane ySplit="1" topLeftCell="A195" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I210" sqref="I210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8804,6 +8859,39 @@
         <v>336</v>
       </c>
       <c r="C208" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" s="55" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B209" t="s">
+        <v>336</v>
+      </c>
+      <c r="C209" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" s="55" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B210" t="s">
+        <v>336</v>
+      </c>
+      <c r="C210" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" s="57" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B211" t="s">
+        <v>336</v>
+      </c>
+      <c r="C211" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9388,11 +9476,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9494,170 +9582,149 @@
     <row r="5" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
       <c r="B5" s="17" t="s">
-        <v>47</v>
+        <v>88</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>1139</v>
       </c>
       <c r="J5" s="55"/>
     </row>
     <row r="6" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
-      <c r="B6" s="17" t="s">
+      <c r="D6" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>705</v>
+      </c>
+      <c r="I6" s="16">
+        <v>3</v>
+      </c>
+      <c r="J6" s="55"/>
+    </row>
+    <row r="7" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="J7" s="55"/>
+    </row>
+    <row r="8" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="D8" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>705</v>
+      </c>
+      <c r="I8" s="16">
+        <v>11</v>
+      </c>
+      <c r="J8" s="55"/>
+    </row>
+    <row r="9" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="J6" s="55"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" t="s">
-        <v>706</v>
-      </c>
-      <c r="G8" t="s">
-        <v>74</v>
-      </c>
-      <c r="H8" s="55" t="s">
-        <v>75</v>
-      </c>
-      <c r="I8" s="55"/>
-      <c r="J8" s="55"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" t="s">
-        <v>76</v>
-      </c>
-      <c r="F9" t="s">
-        <v>77</v>
-      </c>
-      <c r="G9" t="s">
-        <v>84</v>
-      </c>
-      <c r="H9" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="I9" s="55"/>
       <c r="J9" s="55"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
-        <v>120</v>
-      </c>
-      <c r="F10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" t="s">
-        <v>87</v>
-      </c>
-      <c r="H10" s="55" t="s">
-        <v>86</v>
-      </c>
-      <c r="I10" s="55"/>
+    <row r="10" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="17" t="s">
+        <v>47</v>
+      </c>
       <c r="J10" s="55"/>
-      <c r="L10" t="s">
-        <v>810</v>
-      </c>
-      <c r="M10" t="s">
-        <v>807</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>47</v>
-      </c>
-      <c r="H11" s="55"/>
-      <c r="I11" s="55"/>
+    </row>
+    <row r="11" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="17" t="s">
+        <v>103</v>
+      </c>
       <c r="J11" s="55"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>88</v>
-      </c>
-      <c r="C12" t="s">
-        <v>172</v>
+        <v>46</v>
       </c>
       <c r="H12" s="55"/>
       <c r="I12" s="55"/>
       <c r="J12" s="55"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>46</v>
+      <c r="D13" t="s">
+        <v>126</v>
+      </c>
+      <c r="F13" t="s">
+        <v>705</v>
       </c>
       <c r="H13" s="55"/>
-      <c r="I13" s="55"/>
+      <c r="I13" s="55">
+        <v>11</v>
+      </c>
       <c r="J13" s="55"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="F14" t="s">
-        <v>52</v>
+        <v>706</v>
       </c>
       <c r="G14" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="H14" s="55" t="s">
-        <v>256</v>
+        <v>75</v>
       </c>
       <c r="I14" s="55"/>
       <c r="J14" s="55"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="F15" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="G15" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="H15" s="55" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="I15" s="55"/>
       <c r="J15" s="55"/>
-      <c r="K15" s="12" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>25</v>
+        <v>120</v>
       </c>
       <c r="F16" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="G16" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="H16" s="55" t="s">
-        <v>59</v>
+        <v>86</v>
       </c>
       <c r="I16" s="55"/>
       <c r="J16" s="55"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="L16" t="s">
+        <v>810</v>
+      </c>
+      <c r="M16" t="s">
+        <v>807</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>47</v>
       </c>
@@ -9665,198 +9732,210 @@
       <c r="I17" s="55"/>
       <c r="J17" s="55"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>103</v>
+        <v>88</v>
+      </c>
+      <c r="C18" t="s">
+        <v>172</v>
       </c>
       <c r="H18" s="55"/>
       <c r="I18" s="55"/>
       <c r="J18" s="55"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>88</v>
-      </c>
-      <c r="C19" t="s">
-        <v>249</v>
+        <v>46</v>
       </c>
       <c r="H19" s="55"/>
       <c r="I19" s="55"/>
       <c r="J19" s="55"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>46</v>
-      </c>
-      <c r="H20" s="55"/>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H20" s="55" t="s">
+        <v>256</v>
+      </c>
       <c r="I20" s="55"/>
       <c r="J20" s="55"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="E21" t="s">
-        <v>93</v>
+        <v>54</v>
       </c>
       <c r="F21" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
       <c r="G21" t="s">
-        <v>307</v>
+        <v>56</v>
       </c>
       <c r="H21" s="55" t="s">
-        <v>903</v>
+        <v>56</v>
       </c>
       <c r="I21" s="55"/>
       <c r="J21" s="55"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>88</v>
-      </c>
-      <c r="C22" t="s">
-        <v>698</v>
-      </c>
-      <c r="H22" s="55"/>
+      <c r="K21" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" t="s">
+        <v>58</v>
+      </c>
+      <c r="G22" t="s">
+        <v>59</v>
+      </c>
+      <c r="H22" s="55" t="s">
+        <v>59</v>
+      </c>
       <c r="I22" s="55"/>
       <c r="J22" s="55"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
-        <v>126</v>
-      </c>
-      <c r="F23" t="s">
-        <v>66</v>
-      </c>
-      <c r="G23" t="s">
-        <v>67</v>
-      </c>
-      <c r="H23" s="55" t="s">
-        <v>67</v>
-      </c>
-      <c r="I23" s="55" t="s">
-        <v>699</v>
-      </c>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>47</v>
+      </c>
+      <c r="H23" s="55"/>
+      <c r="I23" s="55"/>
       <c r="J23" s="55"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
-        <v>126</v>
-      </c>
-      <c r="F24" t="s">
-        <v>68</v>
-      </c>
-      <c r="G24" t="s">
-        <v>69</v>
-      </c>
-      <c r="H24" s="55" t="s">
-        <v>69</v>
-      </c>
-      <c r="I24" s="55" t="s">
-        <v>700</v>
-      </c>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>103</v>
+      </c>
+      <c r="H24" s="55"/>
+      <c r="I24" s="55"/>
       <c r="J24" s="55"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
-        <v>126</v>
-      </c>
-      <c r="F25" t="s">
-        <v>70</v>
-      </c>
-      <c r="G25" t="s">
-        <v>71</v>
-      </c>
-      <c r="H25" s="55" t="s">
-        <v>900</v>
-      </c>
-      <c r="I25" s="55" t="s">
-        <v>701</v>
-      </c>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" t="s">
+        <v>249</v>
+      </c>
+      <c r="H25" s="55"/>
+      <c r="I25" s="55"/>
       <c r="J25" s="55"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>103</v>
+        <v>46</v>
       </c>
       <c r="H26" s="55"/>
       <c r="I26" s="55"/>
       <c r="J26" s="55"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>47</v>
-      </c>
-      <c r="H27" s="55"/>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" t="s">
+        <v>93</v>
+      </c>
+      <c r="F27" t="s">
+        <v>113</v>
+      </c>
+      <c r="G27" t="s">
+        <v>307</v>
+      </c>
+      <c r="H27" s="55" t="s">
+        <v>903</v>
+      </c>
       <c r="I27" s="55"/>
       <c r="J27" s="55"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>103</v>
+        <v>88</v>
+      </c>
+      <c r="C28" t="s">
+        <v>698</v>
       </c>
       <c r="H28" s="55"/>
       <c r="I28" s="55"/>
       <c r="J28" s="55"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>46</v>
-      </c>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>126</v>
+      </c>
+      <c r="F29" t="s">
+        <v>66</v>
+      </c>
+      <c r="G29" t="s">
+        <v>67</v>
+      </c>
+      <c r="H29" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="I29" s="55" t="s">
+        <v>699</v>
+      </c>
       <c r="J29" s="55"/>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
-        <v>25</v>
+        <v>126</v>
       </c>
       <c r="F30" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G30" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H30" s="55" t="s">
-        <v>67</v>
-      </c>
-      <c r="I30" s="55"/>
+        <v>69</v>
+      </c>
+      <c r="I30" s="55" t="s">
+        <v>700</v>
+      </c>
       <c r="J30" s="55"/>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>25</v>
+        <v>126</v>
       </c>
       <c r="F31" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G31" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H31" s="55" t="s">
-        <v>69</v>
-      </c>
-      <c r="I31" s="55"/>
+        <v>900</v>
+      </c>
+      <c r="I31" s="55" t="s">
+        <v>701</v>
+      </c>
       <c r="J31" s="55"/>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D32" t="s">
-        <v>25</v>
-      </c>
-      <c r="F32" t="s">
-        <v>70</v>
-      </c>
-      <c r="G32" t="s">
-        <v>71</v>
-      </c>
-      <c r="H32" s="55" t="s">
-        <v>900</v>
-      </c>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>103</v>
+      </c>
+      <c r="H32" s="55"/>
       <c r="I32" s="55"/>
       <c r="J32" s="55"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>47</v>
       </c>
@@ -9864,124 +9943,196 @@
       <c r="I33" s="55"/>
       <c r="J33" s="55"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>46</v>
+        <v>103</v>
       </c>
       <c r="H34" s="55"/>
       <c r="I34" s="55"/>
       <c r="J34" s="55"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D35" t="s">
-        <v>72</v>
-      </c>
-      <c r="F35" t="s">
-        <v>89</v>
-      </c>
-      <c r="G35" t="s">
-        <v>90</v>
-      </c>
-      <c r="H35" s="55" t="s">
-        <v>91</v>
-      </c>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>46</v>
+      </c>
+      <c r="H35" s="55"/>
       <c r="I35" s="55"/>
       <c r="J35" s="55"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>47</v>
-      </c>
-      <c r="H36" s="55"/>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" t="s">
+        <v>66</v>
+      </c>
+      <c r="G36" t="s">
+        <v>67</v>
+      </c>
+      <c r="H36" s="55" t="s">
+        <v>67</v>
+      </c>
       <c r="I36" s="55"/>
       <c r="J36" s="55"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>46</v>
-      </c>
-      <c r="H37" s="55"/>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G37" t="s">
+        <v>69</v>
+      </c>
+      <c r="H37" s="55" t="s">
+        <v>69</v>
+      </c>
       <c r="I37" s="55"/>
       <c r="J37" s="55"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>22</v>
-      </c>
-      <c r="E38" t="s">
-        <v>93</v>
+        <v>25</v>
       </c>
       <c r="F38" t="s">
-        <v>94</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>95</v>
+        <v>70</v>
+      </c>
+      <c r="G38" t="s">
+        <v>71</v>
       </c>
       <c r="H38" s="55" t="s">
-        <v>904</v>
+        <v>900</v>
       </c>
       <c r="I38" s="55"/>
       <c r="J38" s="55"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>88</v>
-      </c>
-      <c r="C39" t="s">
-        <v>101</v>
+        <v>47</v>
       </c>
       <c r="H39" s="55"/>
       <c r="I39" s="55"/>
       <c r="J39" s="55"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D40" t="s">
-        <v>72</v>
-      </c>
-      <c r="F40" t="s">
-        <v>102</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="H40" s="55" t="s">
-        <v>905</v>
-      </c>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>46</v>
+      </c>
+      <c r="H40" s="55"/>
       <c r="I40" s="55"/>
       <c r="J40" s="55"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>72</v>
+      </c>
+      <c r="F41" t="s">
+        <v>89</v>
+      </c>
+      <c r="G41" t="s">
+        <v>90</v>
+      </c>
+      <c r="H41" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="I41" s="55"/>
+      <c r="J41" s="55"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
+      <c r="H42" s="55"/>
+      <c r="I42" s="55"/>
+      <c r="J42" s="55"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
+        <v>46</v>
+      </c>
+      <c r="H43" s="55"/>
+      <c r="I43" s="55"/>
+      <c r="J43" s="55"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>22</v>
+      </c>
+      <c r="E44" t="s">
+        <v>93</v>
+      </c>
+      <c r="F44" t="s">
+        <v>94</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H44" s="55" t="s">
+        <v>904</v>
+      </c>
+      <c r="I44" s="55"/>
+      <c r="J44" s="55"/>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>88</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C45" t="s">
+        <v>101</v>
+      </c>
+      <c r="H45" s="55"/>
+      <c r="I45" s="55"/>
+      <c r="J45" s="55"/>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>72</v>
+      </c>
+      <c r="F46" t="s">
+        <v>102</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="H46" s="55" t="s">
+        <v>905</v>
+      </c>
+      <c r="I46" s="55"/>
+      <c r="J46" s="55"/>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="14"/>
+      <c r="B49" t="s">
+        <v>88</v>
+      </c>
+      <c r="C49" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
         <v>670</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="14"/>
-      <c r="B45" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="14"/>
+      <c r="B51" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
         <v>708</v>
       </c>
     </row>
@@ -10768,11 +10919,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35657444-F5E1-4936-AB00-D82A0F63E5F4}">
-  <dimension ref="A1:M166"/>
+  <dimension ref="A1:M182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E84" sqref="E84"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F47" activeCellId="2" sqref="F85 F60 F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10785,7 +10936,7 @@
     <col min="6" max="6" width="17.42578125" style="55" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31.7109375" style="55" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="36.28515625" style="55" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" style="55" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" style="55" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.42578125" style="55" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="46.85546875" style="55" customWidth="1"/>
     <col min="12" max="12" width="38.28515625" style="55" customWidth="1"/>
@@ -10841,7 +10992,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="61"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="55" t="s">
         <v>88</v>
       </c>
@@ -10850,6 +11001,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="57"/>
       <c r="D4" s="55" t="s">
         <v>149</v>
       </c>
@@ -10861,12 +11013,13 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="57"/>
       <c r="B5" s="55" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="61"/>
+      <c r="A6" s="57"/>
       <c r="B6" s="55" t="s">
         <v>88</v>
       </c>
@@ -10875,6 +11028,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="57"/>
       <c r="D7" s="55" t="s">
         <v>149</v>
       </c>
@@ -10886,12 +11040,13 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="57"/>
       <c r="B8" s="55" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="61"/>
+      <c r="A9" s="57"/>
       <c r="B9" s="55" t="s">
         <v>88</v>
       </c>
@@ -10900,6 +11055,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="57"/>
       <c r="D10" s="55" t="s">
         <v>149</v>
       </c>
@@ -10911,12 +11067,13 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="57"/>
       <c r="B11" s="55" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="61"/>
+      <c r="A12" s="57"/>
       <c r="B12" s="55" t="s">
         <v>88</v>
       </c>
@@ -10925,6 +11082,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="57"/>
       <c r="D13" s="55" t="s">
         <v>149</v>
       </c>
@@ -10936,12 +11094,13 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="57"/>
       <c r="B14" s="55" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="61"/>
+      <c r="A15" s="57"/>
       <c r="B15" s="55" t="s">
         <v>88</v>
       </c>
@@ -10950,6 +11109,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="57"/>
       <c r="D16" s="55" t="s">
         <v>149</v>
       </c>
@@ -10961,12 +11121,13 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="57"/>
       <c r="B17" s="55" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="61"/>
+      <c r="A18" s="57"/>
       <c r="B18" s="55" t="s">
         <v>88</v>
       </c>
@@ -10975,6 +11136,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="57"/>
       <c r="D19" s="55" t="s">
         <v>149</v>
       </c>
@@ -10986,12 +11148,13 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="57"/>
       <c r="B20" s="55" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="61"/>
+      <c r="A21" s="57"/>
       <c r="D21" s="55" t="s">
         <v>149</v>
       </c>
@@ -11003,6 +11166,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="57"/>
       <c r="D22" s="55" t="s">
         <v>149</v>
       </c>
@@ -11014,7 +11178,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="61"/>
+      <c r="A23" s="57"/>
       <c r="D23" s="55" t="s">
         <v>22</v>
       </c>
@@ -11032,7 +11196,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="61"/>
+      <c r="A24" s="57"/>
       <c r="B24" s="55" t="s">
         <v>88</v>
       </c>
@@ -11041,7 +11205,7 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="61"/>
+      <c r="A25" s="57"/>
       <c r="D25" s="55" t="s">
         <v>120</v>
       </c>
@@ -11065,311 +11229,297 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="61"/>
-      <c r="B26" s="55" t="s">
+      <c r="A26" s="57"/>
+      <c r="D26" s="57" t="s">
+        <v>126</v>
+      </c>
+      <c r="F26" s="55" t="s">
+        <v>705</v>
+      </c>
+      <c r="I26" s="55" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="57"/>
+      <c r="B27" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="C26" s="55" t="s">
+      <c r="C27" s="55" t="s">
         <v>271</v>
       </c>
-      <c r="K26" s="57"/>
-      <c r="L26" s="57"/>
-      <c r="M26" s="57"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="61"/>
-      <c r="D27" s="55" t="s">
+      <c r="K27" s="57"/>
+      <c r="L27" s="57"/>
+      <c r="M27" s="57"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="57"/>
+      <c r="D28" s="55" t="s">
         <v>72</v>
       </c>
-      <c r="F27" s="55" t="s">
+      <c r="F28" s="55" t="s">
         <v>272</v>
       </c>
-      <c r="G27" s="55" t="s">
+      <c r="G28" s="55" t="s">
         <v>273</v>
       </c>
-      <c r="H27" s="55" t="s">
+      <c r="H28" s="55" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="61"/>
-      <c r="B28" s="55" t="s">
-        <v>103</v>
-      </c>
-    </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="61"/>
+      <c r="A29" s="57"/>
       <c r="B29" s="55" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="61"/>
+      <c r="A30" s="57"/>
       <c r="B30" s="55" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>126</v>
+      </c>
+      <c r="F32" t="s">
+        <v>705</v>
+      </c>
+      <c r="I32">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="61"/>
+      <c r="B34" s="55" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="63"/>
-      <c r="B31" s="55" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="63"/>
-      <c r="D32" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="E32" s="55" t="s">
-        <v>276</v>
-      </c>
-      <c r="F32" s="55" t="s">
-        <v>277</v>
-      </c>
-      <c r="G32" s="55" t="s">
-        <v>278</v>
-      </c>
-      <c r="H32" s="55" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="63"/>
-      <c r="B33" s="55" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="63"/>
-      <c r="B34" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="C34" s="55" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="63"/>
       <c r="B35" s="55" t="s">
-        <v>662</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="63"/>
-      <c r="B36" s="55" t="s">
-        <v>103</v>
+      <c r="D36" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" s="55" t="s">
+        <v>276</v>
+      </c>
+      <c r="F36" s="55" t="s">
+        <v>277</v>
+      </c>
+      <c r="G36" s="55" t="s">
+        <v>278</v>
+      </c>
+      <c r="H36" s="55" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="63"/>
       <c r="B37" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="C37" s="55" t="s">
-        <v>282</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="63"/>
       <c r="B38" s="55" t="s">
         <v>88</v>
       </c>
       <c r="C38" s="55" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="64"/>
+      <c r="A39" s="63"/>
       <c r="B39" s="55" t="s">
-        <v>46</v>
+        <v>662</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="64"/>
-      <c r="D40" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="E40" s="55" t="s">
-        <v>93</v>
-      </c>
-      <c r="F40" s="55" t="s">
-        <v>110</v>
-      </c>
-      <c r="G40" s="55" t="s">
-        <v>284</v>
-      </c>
-      <c r="H40" s="55" t="s">
-        <v>912</v>
+      <c r="A40" s="63"/>
+      <c r="B40" s="55" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="64"/>
       <c r="B41" s="55" t="s">
         <v>88</v>
       </c>
       <c r="C41" s="55" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="64"/>
-      <c r="D42" s="55" t="s">
-        <v>120</v>
-      </c>
-      <c r="F42" s="55" t="s">
-        <v>111</v>
-      </c>
-      <c r="G42" s="55" t="s">
-        <v>286</v>
-      </c>
-      <c r="H42" s="55" t="s">
-        <v>913</v>
-      </c>
-      <c r="K42" s="55" t="s">
-        <v>1007</v>
-      </c>
-      <c r="L42" s="55" t="s">
-        <v>895</v>
-      </c>
-      <c r="M42" s="55" t="s">
-        <v>895</v>
+      <c r="B42" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="55" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="64"/>
-      <c r="D43" s="55" t="s">
-        <v>25</v>
-      </c>
-      <c r="F43" s="55" t="s">
-        <v>112</v>
-      </c>
-      <c r="G43" s="55" t="s">
-        <v>287</v>
-      </c>
-      <c r="H43" s="55" t="s">
-        <v>914</v>
+      <c r="B43" s="55" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="64"/>
-      <c r="B44" s="55" t="s">
-        <v>103</v>
+      <c r="D44" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="E44" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="F44" s="55" t="s">
+        <v>110</v>
+      </c>
+      <c r="G44" s="55" t="s">
+        <v>284</v>
+      </c>
+      <c r="H44" s="55" t="s">
+        <v>912</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="64"/>
       <c r="B45" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C45" s="55" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="64"/>
+      <c r="D46" s="55" t="s">
+        <v>120</v>
+      </c>
+      <c r="F46" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="G46" s="55" t="s">
+        <v>286</v>
+      </c>
+      <c r="H46" s="55" t="s">
+        <v>913</v>
+      </c>
+      <c r="K46" s="55" t="s">
+        <v>1007</v>
+      </c>
+      <c r="L46" s="55" t="s">
+        <v>895</v>
+      </c>
+      <c r="M46" s="55" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="64"/>
+      <c r="D47" s="55" t="s">
+        <v>336</v>
+      </c>
+      <c r="E47" s="50" t="s">
+        <v>1145</v>
+      </c>
+      <c r="F47" s="55" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="64"/>
+      <c r="B48" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C48" s="55" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="64"/>
+      <c r="D49" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="F49" s="55" t="s">
+        <v>112</v>
+      </c>
+      <c r="G49" s="55" t="s">
+        <v>287</v>
+      </c>
+      <c r="H49" s="55" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="64"/>
+      <c r="D50" s="57" t="s">
+        <v>126</v>
+      </c>
+      <c r="F50" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="I50" s="76" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="64"/>
+      <c r="B51" s="55" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="64"/>
+      <c r="B52" s="55" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" s="64"/>
+      <c r="B53" s="55" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B46" s="55" t="s">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B54" s="55" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B47" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="C47" s="55" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="65"/>
-      <c r="B48" s="55" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" s="65"/>
-      <c r="D49" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="E49" s="55" t="s">
-        <v>93</v>
-      </c>
-      <c r="F49" s="55" t="s">
-        <v>123</v>
-      </c>
-      <c r="G49" s="55" t="s">
-        <v>289</v>
-      </c>
-      <c r="H49" s="55" t="s">
-        <v>915</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" s="65"/>
-      <c r="B50" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="C50" s="55" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" s="65"/>
-      <c r="D51" s="55" t="s">
-        <v>120</v>
-      </c>
-      <c r="F51" s="55" t="s">
-        <v>125</v>
-      </c>
-      <c r="G51" s="55" t="s">
-        <v>291</v>
-      </c>
-      <c r="H51" s="55" t="s">
-        <v>916</v>
-      </c>
-      <c r="K51" s="55" t="s">
-        <v>893</v>
-      </c>
-      <c r="L51" s="55" t="s">
-        <v>896</v>
-      </c>
-      <c r="M51" s="55" t="s">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="65"/>
-      <c r="D52" s="55" t="s">
-        <v>25</v>
-      </c>
-      <c r="F52" s="55" t="s">
-        <v>124</v>
-      </c>
-      <c r="G52" s="55" t="s">
-        <v>292</v>
-      </c>
-      <c r="H52" s="55" t="s">
-        <v>917</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="65"/>
-      <c r="B53" s="55" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="65"/>
-      <c r="B54" s="55" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B55" s="55" t="s">
-        <v>103</v>
+        <v>88</v>
+      </c>
+      <c r="C55" s="55" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="66"/>
+      <c r="A56" s="65"/>
       <c r="B56" s="55" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" s="66"/>
+      <c r="A57" s="65"/>
       <c r="D57" s="55" t="s">
         <v>22</v>
       </c>
@@ -11377,136 +11527,127 @@
         <v>93</v>
       </c>
       <c r="F57" s="55" t="s">
-        <v>293</v>
+        <v>123</v>
       </c>
       <c r="G57" s="55" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="H57" s="55" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A58" s="66"/>
-      <c r="D58" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="E58" s="55" t="s">
-        <v>295</v>
-      </c>
-      <c r="F58" s="55" t="s">
-        <v>296</v>
-      </c>
-      <c r="G58" s="55" t="s">
-        <v>297</v>
-      </c>
-      <c r="H58" s="55" t="s">
-        <v>919</v>
+      <c r="A58" s="65"/>
+      <c r="B58" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C58" s="55" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A59" s="66"/>
-      <c r="B59" s="55" t="s">
+      <c r="A59" s="65"/>
+      <c r="D59" s="55" t="s">
+        <v>120</v>
+      </c>
+      <c r="F59" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="G59" s="55" t="s">
+        <v>291</v>
+      </c>
+      <c r="H59" s="55" t="s">
+        <v>916</v>
+      </c>
+      <c r="K59" s="55" t="s">
+        <v>893</v>
+      </c>
+      <c r="L59" s="55" t="s">
+        <v>896</v>
+      </c>
+      <c r="M59" s="55" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="65"/>
+      <c r="D60" s="55" t="s">
+        <v>336</v>
+      </c>
+      <c r="E60" s="50" t="s">
+        <v>1145</v>
+      </c>
+      <c r="F60" s="55" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" s="65"/>
+      <c r="B61" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="C59" s="55" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A60" s="66"/>
-      <c r="D60" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="E60" s="55" t="s">
-        <v>299</v>
-      </c>
-      <c r="F60" s="55" t="s">
-        <v>300</v>
-      </c>
-      <c r="G60" s="55" t="s">
-        <v>301</v>
-      </c>
-      <c r="H60" s="55" t="s">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" s="66"/>
-      <c r="B61" s="55" t="s">
+      <c r="C61" s="55" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" s="65"/>
+      <c r="D62" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="F62" s="55" t="s">
+        <v>124</v>
+      </c>
+      <c r="G62" s="55" t="s">
+        <v>292</v>
+      </c>
+      <c r="H62" s="55" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" s="65"/>
+      <c r="D63" s="57" t="s">
+        <v>126</v>
+      </c>
+      <c r="F63" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="I63" s="55" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="65"/>
+      <c r="B64" s="55" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62" s="66"/>
-      <c r="B62" s="55" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" s="67"/>
-      <c r="B63" s="55" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A64" s="67"/>
-      <c r="D64" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="E64" s="55" t="s">
-        <v>93</v>
-      </c>
-      <c r="F64" s="55" t="s">
-        <v>302</v>
-      </c>
-      <c r="G64" s="55" t="s">
-        <v>303</v>
-      </c>
-      <c r="H64" s="55" t="s">
-        <v>921</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A65" s="67"/>
-      <c r="D65" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="E65" s="55" t="s">
-        <v>93</v>
-      </c>
-      <c r="F65" s="55" t="s">
-        <v>304</v>
-      </c>
-      <c r="G65" s="55" t="s">
-        <v>305</v>
-      </c>
-      <c r="H65" s="55" t="s">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A66" s="67"/>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="65"/>
+      <c r="B65" s="55" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="65"/>
       <c r="B66" s="55" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B67" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="C67" s="55" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A68" s="68"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="66"/>
       <c r="B68" s="55" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A69" s="68"/>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="66"/>
       <c r="D69" s="55" t="s">
         <v>22</v>
       </c>
@@ -11514,512 +11655,586 @@
         <v>93</v>
       </c>
       <c r="F69" s="55" t="s">
+        <v>293</v>
+      </c>
+      <c r="G69" s="55" t="s">
+        <v>294</v>
+      </c>
+      <c r="H69" s="55" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="66"/>
+      <c r="D70" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="E70" s="55" t="s">
+        <v>295</v>
+      </c>
+      <c r="F70" s="55" t="s">
+        <v>296</v>
+      </c>
+      <c r="G70" s="55" t="s">
+        <v>297</v>
+      </c>
+      <c r="H70" s="55" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="66"/>
+      <c r="B71" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C71" s="55" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="66"/>
+      <c r="D72" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="E72" s="55" t="s">
+        <v>299</v>
+      </c>
+      <c r="F72" s="55" t="s">
+        <v>300</v>
+      </c>
+      <c r="G72" s="55" t="s">
+        <v>301</v>
+      </c>
+      <c r="H72" s="55" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="66"/>
+      <c r="B73" s="55" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="66"/>
+      <c r="B74" s="55" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="67"/>
+      <c r="B75" s="55" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="67"/>
+      <c r="D76" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="E76" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="F76" s="55" t="s">
+        <v>302</v>
+      </c>
+      <c r="G76" s="55" t="s">
+        <v>303</v>
+      </c>
+      <c r="H76" s="55" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="67"/>
+      <c r="D77" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="E77" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="F77" s="55" t="s">
+        <v>304</v>
+      </c>
+      <c r="G77" s="55" t="s">
+        <v>305</v>
+      </c>
+      <c r="H77" s="55" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="67"/>
+      <c r="B78" s="55" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B79" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C79" s="55" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="68"/>
+      <c r="B80" s="55" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A81" s="68"/>
+      <c r="D81" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="E81" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="F81" s="55" t="s">
         <v>113</v>
       </c>
-      <c r="G69" s="55" t="s">
+      <c r="G81" s="55" t="s">
         <v>307</v>
       </c>
-      <c r="H69" s="55" t="s">
+      <c r="H81" s="55" t="s">
         <v>923</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A70" s="68"/>
-      <c r="B70" s="55" t="s">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A82" s="68"/>
+      <c r="B82" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="C70" s="55" t="s">
+      <c r="C82" s="55" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A71" s="68"/>
-      <c r="D71" s="55" t="s">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A83" s="68"/>
+      <c r="D83" s="55" t="s">
+        <v>72</v>
+      </c>
+      <c r="F83" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="G83" s="55" t="s">
+        <v>311</v>
+      </c>
+      <c r="H83" s="55" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A84" s="68"/>
+      <c r="D84" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="F71" s="55" t="s">
+      <c r="F84" s="55" t="s">
         <v>114</v>
       </c>
-      <c r="G71" s="55" t="s">
+      <c r="G84" s="55" t="s">
         <v>309</v>
       </c>
-      <c r="H71" s="55" t="s">
+      <c r="H84" s="55" t="s">
         <v>924</v>
       </c>
-      <c r="K71" s="55" t="s">
+      <c r="K84" s="55" t="s">
         <v>894</v>
       </c>
-      <c r="L71" s="55" t="s">
+      <c r="L84" s="55" t="s">
         <v>897</v>
       </c>
-      <c r="M71" s="55" t="s">
+      <c r="M84" s="55" t="s">
         <v>897</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A72" s="68"/>
-      <c r="D72" s="55" t="s">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A85" s="68"/>
+      <c r="D85" s="57" t="s">
+        <v>336</v>
+      </c>
+      <c r="E85" s="55" t="s">
+        <v>1145</v>
+      </c>
+      <c r="F85" s="57" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A86" s="68"/>
+      <c r="B86" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C86" s="55" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A87" s="68"/>
+      <c r="D87" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="F72" s="55" t="s">
+      <c r="F87" s="55" t="s">
         <v>115</v>
       </c>
-      <c r="G72" s="55" t="s">
+      <c r="G87" s="55" t="s">
         <v>310</v>
       </c>
-      <c r="H72" s="55" t="s">
+      <c r="H87" s="55" t="s">
         <v>925</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A73" s="68"/>
-      <c r="D73" s="55" t="s">
-        <v>72</v>
-      </c>
-      <c r="F73" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="G73" s="55" t="s">
-        <v>311</v>
-      </c>
-      <c r="H73" s="55" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A74" s="68"/>
-      <c r="B74" s="55" t="s">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A88" s="68"/>
+      <c r="D88" s="57" t="s">
+        <v>126</v>
+      </c>
+      <c r="F88" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="I88" s="55" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A89" s="68"/>
+      <c r="B89" s="55" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A75" s="68"/>
-      <c r="B75" s="55" t="s">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A90" s="68"/>
+      <c r="B90" s="55" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A91" s="68"/>
+      <c r="B91" s="55" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B76" s="55" t="s">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B92" s="55" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B77" s="55" t="s">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B93" s="55" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A78" s="69"/>
-      <c r="B78" s="55" t="s">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A94" s="69"/>
+      <c r="B94" s="55" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A79" s="69"/>
-      <c r="D79" s="55" t="s">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A95" s="69"/>
+      <c r="D95" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="E79" s="55" t="s">
+      <c r="E95" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="F79" s="55" t="s">
+      <c r="F95" s="55" t="s">
         <v>312</v>
       </c>
-      <c r="G79" s="55" t="s">
+      <c r="G95" s="55" t="s">
         <v>313</v>
       </c>
-      <c r="H79" s="55" t="s">
+      <c r="H95" s="55" t="s">
         <v>927</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A80" s="69"/>
-      <c r="B80" s="55" t="s">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A96" s="69"/>
+      <c r="B96" s="55" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B81" s="55" t="s">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B97" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="C81" s="55" t="s">
+      <c r="C97" s="55" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A82" s="70"/>
-      <c r="B82" s="55" t="s">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A98" s="70"/>
+      <c r="B98" s="55" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A83" s="70"/>
-      <c r="D83" s="55" t="s">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A99" s="70"/>
+      <c r="D99" s="55" t="s">
         <v>149</v>
       </c>
-      <c r="G83" s="55" t="s">
+      <c r="G99" s="55" t="s">
         <v>194</v>
       </c>
-      <c r="H83" s="55" t="s">
+      <c r="H99" s="55" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A84" s="70"/>
-      <c r="D84" s="55" t="s">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A100" s="70"/>
+      <c r="D100" s="55" t="s">
         <v>281</v>
       </c>
-      <c r="E84" s="55" t="s">
+      <c r="E100" s="55" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A85" s="70"/>
-      <c r="B85" s="55" t="s">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A101" s="70"/>
+      <c r="B101" s="55" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B86" s="55" t="s">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B102" s="55" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A87" s="71"/>
-      <c r="B87" s="71" t="s">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A103" s="71"/>
+      <c r="B103" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="C87" s="55" t="s">
+      <c r="C103" s="55" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A88" s="72"/>
-      <c r="B88" s="55" t="s">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A104" s="72"/>
+      <c r="B104" s="55" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A89" s="72"/>
-      <c r="D89" s="55" t="s">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A105" s="72"/>
+      <c r="D105" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="F89" s="55" t="s">
+      <c r="F105" s="55" t="s">
         <v>317</v>
       </c>
-      <c r="G89" s="55" t="s">
+      <c r="G105" s="55" t="s">
         <v>318</v>
       </c>
-      <c r="H89" s="55" t="s">
+      <c r="H105" s="55" t="s">
         <v>1103</v>
       </c>
-      <c r="K89" s="55" t="s">
+      <c r="K105" s="55" t="s">
         <v>809</v>
       </c>
-      <c r="L89" s="55" t="s">
+      <c r="L105" s="55" t="s">
         <v>808</v>
       </c>
-      <c r="M89" s="62" t="s">
+      <c r="M105" s="62" t="s">
         <v>808</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A90" s="72"/>
-      <c r="B90" s="55" t="s">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A106" s="72"/>
+      <c r="B106" s="55" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A91" s="73"/>
-      <c r="B91" s="55" t="s">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A107" s="73"/>
+      <c r="B107" s="55" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A92" s="73"/>
-      <c r="D92" s="55" t="s">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A108" s="73"/>
+      <c r="D108" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="E92" s="55" t="s">
+      <c r="E108" s="55" t="s">
         <v>319</v>
       </c>
-      <c r="F92" s="55" t="s">
+      <c r="F108" s="55" t="s">
         <v>320</v>
       </c>
-      <c r="G92" s="55" t="s">
+      <c r="G108" s="55" t="s">
         <v>321</v>
       </c>
-      <c r="H92" s="55" t="s">
+      <c r="H108" s="55" t="s">
         <v>928</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A93" s="73"/>
-      <c r="B93" s="55" t="s">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A109" s="73"/>
+      <c r="B109" s="55" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A94" s="63"/>
-      <c r="B94" s="63" t="s">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A110" s="63"/>
+      <c r="B110" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="C94" s="55" t="s">
+      <c r="C110" s="55" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A95" s="74"/>
-      <c r="B95" s="55" t="s">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A111" s="74"/>
+      <c r="B111" s="55" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A96" s="74"/>
-      <c r="D96" s="55" t="s">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A112" s="74"/>
+      <c r="D112" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="F96" s="55" t="s">
+      <c r="F112" s="55" t="s">
         <v>323</v>
       </c>
-      <c r="G96" s="55" t="s">
+      <c r="G112" s="55" t="s">
         <v>324</v>
       </c>
-      <c r="H96" s="55" t="s">
+      <c r="H112" s="55" t="s">
         <v>929</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="74"/>
-      <c r="D97" s="55" t="s">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A113" s="74"/>
+      <c r="D113" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="F97" s="55" t="s">
+      <c r="F113" s="55" t="s">
         <v>325</v>
       </c>
-      <c r="G97" s="55" t="s">
+      <c r="G113" s="55" t="s">
         <v>326</v>
       </c>
-      <c r="H97" s="55" t="s">
+      <c r="H113" s="55" t="s">
         <v>930</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A98" s="74"/>
-      <c r="B98" s="55" t="s">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A114" s="74"/>
+      <c r="B114" s="55" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99" s="63"/>
-      <c r="B99" s="63" t="s">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" s="63"/>
+      <c r="B115" s="63" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" s="66"/>
-      <c r="B100" s="55" t="s">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A116" s="66"/>
+      <c r="B116" s="55" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="66"/>
-      <c r="D101" s="55" t="s">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A117" s="66"/>
+      <c r="D117" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="E101" s="55" t="s">
+      <c r="E117" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="F101" s="55" t="s">
+      <c r="F117" s="55" t="s">
         <v>327</v>
       </c>
-      <c r="G101" s="55" t="s">
+      <c r="G117" s="55" t="s">
         <v>328</v>
       </c>
-      <c r="H101" s="55" t="s">
+      <c r="H117" s="55" t="s">
         <v>931</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" s="61"/>
-      <c r="B102" s="61" t="s">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A118" s="61"/>
+      <c r="B118" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="C102" s="55" t="s">
+      <c r="C118" s="55" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A103" s="66"/>
-      <c r="D103" s="55" t="s">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A119" s="66"/>
+      <c r="D119" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="E103" s="55" t="s">
+      <c r="E119" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="F103" s="55" t="s">
+      <c r="F119" s="55" t="s">
         <v>330</v>
       </c>
-      <c r="G103" s="55" t="s">
+      <c r="G119" s="55" t="s">
         <v>331</v>
       </c>
-      <c r="H103" s="55" t="s">
+      <c r="H119" s="55" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A104" s="61"/>
-      <c r="B104" s="61" t="s">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A120" s="61"/>
+      <c r="B120" s="61" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A105" s="66"/>
-      <c r="B105" s="55" t="s">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A121" s="66"/>
+      <c r="B121" s="55" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A106" s="71"/>
-      <c r="B106" s="71" t="s">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A122" s="71"/>
+      <c r="B122" s="71" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B107" s="55" t="s">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B123" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="C107" s="55" t="s">
+      <c r="C123" s="55" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A108" s="70"/>
-      <c r="B108" s="55" t="s">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A124" s="70"/>
+      <c r="B124" s="55" t="s">
         <v>663</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B109" s="55" t="s">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B125" s="55" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A110" s="75"/>
-      <c r="B110" s="75" t="s">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A126" s="75"/>
+      <c r="B126" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="C110" s="75" t="s">
+      <c r="C126" s="75" t="s">
         <v>727</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A111" s="57"/>
-      <c r="B111" s="57" t="s">
-        <v>728</v>
-      </c>
-      <c r="C111" s="57"/>
-      <c r="D111" s="57"/>
-      <c r="E111" s="57"/>
-      <c r="F111" s="57"/>
-      <c r="G111" s="57"/>
-      <c r="H111" s="57"/>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A112" s="57"/>
-      <c r="B112" s="57" t="s">
-        <v>103</v>
-      </c>
-      <c r="C112" s="57"/>
-      <c r="D112" s="57"/>
-      <c r="E112" s="57"/>
-      <c r="F112" s="57"/>
-      <c r="G112" s="57"/>
-      <c r="H112" s="57"/>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B113" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="C113" s="55" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A114" s="73"/>
-      <c r="B114" s="55" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A115" s="73"/>
-      <c r="D115" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="E115" s="55" t="s">
-        <v>93</v>
-      </c>
-      <c r="F115" s="55" t="s">
-        <v>375</v>
-      </c>
-      <c r="G115" s="62" t="s">
-        <v>376</v>
-      </c>
-      <c r="H115" s="55" t="s">
-        <v>948</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A116" s="73"/>
-      <c r="B116" s="55" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A117" s="57"/>
-      <c r="B117" s="57" t="s">
-        <v>103</v>
-      </c>
-      <c r="C117" s="57"/>
-      <c r="D117" s="57"/>
-      <c r="E117" s="57"/>
-      <c r="F117" s="57"/>
-      <c r="G117" s="57"/>
-      <c r="H117" s="57"/>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A124" s="57"/>
-      <c r="B124" s="57"/>
-      <c r="C124" s="57"/>
-      <c r="D124" s="57"/>
-      <c r="E124" s="57"/>
-      <c r="F124" s="57"/>
-      <c r="G124" s="57"/>
-      <c r="H124" s="57"/>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A125" s="57"/>
-      <c r="B125" s="57"/>
-      <c r="C125" s="57"/>
-      <c r="D125" s="57"/>
-      <c r="E125" s="57"/>
-      <c r="F125" s="57"/>
-      <c r="G125" s="57"/>
-      <c r="H125" s="57"/>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A126" s="57"/>
-      <c r="B126" s="57"/>
-      <c r="C126" s="57"/>
-      <c r="D126" s="57"/>
-      <c r="E126" s="57"/>
-      <c r="F126" s="57"/>
-      <c r="G126" s="57"/>
-      <c r="H126" s="57"/>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="57"/>
-      <c r="B127" s="57"/>
+      <c r="B127" s="57" t="s">
+        <v>728</v>
+      </c>
       <c r="C127" s="57"/>
       <c r="D127" s="57"/>
       <c r="E127" s="57"/>
@@ -12029,7 +12244,9 @@
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="57"/>
-      <c r="B128" s="57"/>
+      <c r="B128" s="57" t="s">
+        <v>103</v>
+      </c>
       <c r="C128" s="57"/>
       <c r="D128" s="57"/>
       <c r="E128" s="57"/>
@@ -12038,114 +12255,54 @@
       <c r="H128" s="57"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A129" s="57"/>
-      <c r="B129" s="57"/>
-      <c r="C129" s="57"/>
-      <c r="D129" s="57"/>
-      <c r="E129" s="57"/>
-      <c r="F129" s="57"/>
-      <c r="G129" s="57"/>
-      <c r="H129" s="57"/>
+      <c r="B129" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C129" s="55" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A130" s="57"/>
-      <c r="B130" s="57"/>
-      <c r="C130" s="57"/>
-      <c r="D130" s="57"/>
-      <c r="E130" s="57"/>
-      <c r="F130" s="57"/>
-      <c r="G130" s="57"/>
-      <c r="H130" s="57"/>
+      <c r="A130" s="73"/>
+      <c r="B130" s="55" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A131" s="57"/>
-      <c r="B131" s="57"/>
-      <c r="C131" s="57"/>
-      <c r="D131" s="57"/>
-      <c r="E131" s="57"/>
-      <c r="F131" s="57"/>
-      <c r="G131" s="57"/>
-      <c r="H131" s="57"/>
+      <c r="A131" s="73"/>
+      <c r="D131" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="E131" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="F131" s="55" t="s">
+        <v>375</v>
+      </c>
+      <c r="G131" s="62" t="s">
+        <v>376</v>
+      </c>
+      <c r="H131" s="55" t="s">
+        <v>948</v>
+      </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A132" s="57"/>
-      <c r="B132" s="57"/>
-      <c r="C132" s="57"/>
-      <c r="D132" s="57"/>
-      <c r="E132" s="57"/>
-      <c r="F132" s="57"/>
-      <c r="G132" s="57"/>
-      <c r="H132" s="57"/>
+      <c r="A132" s="73"/>
+      <c r="B132" s="55" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="57"/>
-      <c r="B133" s="57"/>
+      <c r="B133" s="57" t="s">
+        <v>103</v>
+      </c>
       <c r="C133" s="57"/>
       <c r="D133" s="57"/>
       <c r="E133" s="57"/>
       <c r="F133" s="57"/>
       <c r="G133" s="57"/>
       <c r="H133" s="57"/>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A134" s="57"/>
-      <c r="B134" s="57"/>
-      <c r="C134" s="57"/>
-      <c r="D134" s="57"/>
-      <c r="E134" s="57"/>
-      <c r="F134" s="57"/>
-      <c r="G134" s="57"/>
-      <c r="H134" s="57"/>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A135" s="57"/>
-      <c r="B135" s="57"/>
-      <c r="C135" s="57"/>
-      <c r="D135" s="57"/>
-      <c r="E135" s="57"/>
-      <c r="F135" s="57"/>
-      <c r="G135" s="57"/>
-      <c r="H135" s="57"/>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A136" s="57"/>
-      <c r="B136" s="57"/>
-      <c r="C136" s="57"/>
-      <c r="D136" s="57"/>
-      <c r="E136" s="57"/>
-      <c r="F136" s="57"/>
-      <c r="G136" s="57"/>
-      <c r="H136" s="57"/>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A137" s="57"/>
-      <c r="B137" s="57"/>
-      <c r="C137" s="57"/>
-      <c r="D137" s="57"/>
-      <c r="E137" s="57"/>
-      <c r="F137" s="57"/>
-      <c r="G137" s="57"/>
-      <c r="H137" s="57"/>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A138" s="57"/>
-      <c r="B138" s="57"/>
-      <c r="C138" s="57"/>
-      <c r="D138" s="57"/>
-      <c r="E138" s="57"/>
-      <c r="F138" s="57"/>
-      <c r="G138" s="57"/>
-      <c r="H138" s="57"/>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A139" s="57"/>
-      <c r="B139" s="57"/>
-      <c r="C139" s="57"/>
-      <c r="D139" s="57"/>
-      <c r="E139" s="57"/>
-      <c r="F139" s="57"/>
-      <c r="G139" s="57"/>
-      <c r="H139" s="57"/>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="57"/>
@@ -12416,6 +12573,166 @@
       <c r="F166" s="57"/>
       <c r="G166" s="57"/>
       <c r="H166" s="57"/>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A167" s="57"/>
+      <c r="B167" s="57"/>
+      <c r="C167" s="57"/>
+      <c r="D167" s="57"/>
+      <c r="E167" s="57"/>
+      <c r="F167" s="57"/>
+      <c r="G167" s="57"/>
+      <c r="H167" s="57"/>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A168" s="57"/>
+      <c r="B168" s="57"/>
+      <c r="C168" s="57"/>
+      <c r="D168" s="57"/>
+      <c r="E168" s="57"/>
+      <c r="F168" s="57"/>
+      <c r="G168" s="57"/>
+      <c r="H168" s="57"/>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A169" s="57"/>
+      <c r="B169" s="57"/>
+      <c r="C169" s="57"/>
+      <c r="D169" s="57"/>
+      <c r="E169" s="57"/>
+      <c r="F169" s="57"/>
+      <c r="G169" s="57"/>
+      <c r="H169" s="57"/>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A170" s="57"/>
+      <c r="B170" s="57"/>
+      <c r="C170" s="57"/>
+      <c r="D170" s="57"/>
+      <c r="E170" s="57"/>
+      <c r="F170" s="57"/>
+      <c r="G170" s="57"/>
+      <c r="H170" s="57"/>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A171" s="57"/>
+      <c r="B171" s="57"/>
+      <c r="C171" s="57"/>
+      <c r="D171" s="57"/>
+      <c r="E171" s="57"/>
+      <c r="F171" s="57"/>
+      <c r="G171" s="57"/>
+      <c r="H171" s="57"/>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A172" s="57"/>
+      <c r="B172" s="57"/>
+      <c r="C172" s="57"/>
+      <c r="D172" s="57"/>
+      <c r="E172" s="57"/>
+      <c r="F172" s="57"/>
+      <c r="G172" s="57"/>
+      <c r="H172" s="57"/>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A173" s="57"/>
+      <c r="B173" s="57"/>
+      <c r="C173" s="57"/>
+      <c r="D173" s="57"/>
+      <c r="E173" s="57"/>
+      <c r="F173" s="57"/>
+      <c r="G173" s="57"/>
+      <c r="H173" s="57"/>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A174" s="57"/>
+      <c r="B174" s="57"/>
+      <c r="C174" s="57"/>
+      <c r="D174" s="57"/>
+      <c r="E174" s="57"/>
+      <c r="F174" s="57"/>
+      <c r="G174" s="57"/>
+      <c r="H174" s="57"/>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A175" s="57"/>
+      <c r="B175" s="57"/>
+      <c r="C175" s="57"/>
+      <c r="D175" s="57"/>
+      <c r="E175" s="57"/>
+      <c r="F175" s="57"/>
+      <c r="G175" s="57"/>
+      <c r="H175" s="57"/>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A176" s="57"/>
+      <c r="B176" s="57"/>
+      <c r="C176" s="57"/>
+      <c r="D176" s="57"/>
+      <c r="E176" s="57"/>
+      <c r="F176" s="57"/>
+      <c r="G176" s="57"/>
+      <c r="H176" s="57"/>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A177" s="57"/>
+      <c r="B177" s="57"/>
+      <c r="C177" s="57"/>
+      <c r="D177" s="57"/>
+      <c r="E177" s="57"/>
+      <c r="F177" s="57"/>
+      <c r="G177" s="57"/>
+      <c r="H177" s="57"/>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A178" s="57"/>
+      <c r="B178" s="57"/>
+      <c r="C178" s="57"/>
+      <c r="D178" s="57"/>
+      <c r="E178" s="57"/>
+      <c r="F178" s="57"/>
+      <c r="G178" s="57"/>
+      <c r="H178" s="57"/>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A179" s="57"/>
+      <c r="B179" s="57"/>
+      <c r="C179" s="57"/>
+      <c r="D179" s="57"/>
+      <c r="E179" s="57"/>
+      <c r="F179" s="57"/>
+      <c r="G179" s="57"/>
+      <c r="H179" s="57"/>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A180" s="57"/>
+      <c r="B180" s="57"/>
+      <c r="C180" s="57"/>
+      <c r="D180" s="57"/>
+      <c r="E180" s="57"/>
+      <c r="F180" s="57"/>
+      <c r="G180" s="57"/>
+      <c r="H180" s="57"/>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A181" s="57"/>
+      <c r="B181" s="57"/>
+      <c r="C181" s="57"/>
+      <c r="D181" s="57"/>
+      <c r="E181" s="57"/>
+      <c r="F181" s="57"/>
+      <c r="G181" s="57"/>
+      <c r="H181" s="57"/>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A182" s="57"/>
+      <c r="B182" s="57"/>
+      <c r="C182" s="57"/>
+      <c r="D182" s="57"/>
+      <c r="E182" s="57"/>
+      <c r="F182" s="57"/>
+      <c r="G182" s="57"/>
+      <c r="H182" s="57"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New function to adate: helperText
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
+++ b/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8339B7-6EED-4D91-8150-AB9AF6258DC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B68FCD-68BA-4519-980A-71DDC35EFCBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="806" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="806" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -3717,9 +3717,6 @@
     <t>&lt;font color = "red"&gt;Sarampo 1 &lt;b&gt;{{calculates.displaySARAMPO1}}&lt;/b&gt;&lt;/font&gt;</t>
   </si>
   <si>
-    <t>A vacina sarampo 1não pode estar no futuro</t>
-  </si>
-  <si>
     <t>Yellow fever</t>
   </si>
   <si>
@@ -4747,6 +4744,9 @@
   </si>
   <si>
     <t>data('VISITTYPE') == 'move'</t>
+  </si>
+  <si>
+    <t>A vacina sarampo 1 não pode estar no futuro</t>
   </si>
 </sst>
 </file>
@@ -5554,9 +5554,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A7F4833-88F1-44B1-8A75-76AFCBB7BC62}">
   <dimension ref="A1:L892"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G60" sqref="G60"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A720" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L732" sqref="L732"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5654,7 +5654,7 @@
         <v>1150</v>
       </c>
       <c r="J5" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="K5" t="s">
         <v>886</v>
@@ -5741,7 +5741,7 @@
         <v>357</v>
       </c>
       <c r="J14" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="K14" t="s">
         <v>886</v>
@@ -5817,7 +5817,7 @@
         <v>1142</v>
       </c>
       <c r="J22" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="K22" t="s">
         <v>1151</v>
@@ -5904,7 +5904,7 @@
         <v>366</v>
       </c>
       <c r="J31" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="K31" t="s">
         <v>1151</v>
@@ -5966,7 +5966,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="B39" t="s">
         <v>87</v>
@@ -5987,7 +5987,7 @@
         <v>87</v>
       </c>
       <c r="C41" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -6024,7 +6024,7 @@
         <v>87</v>
       </c>
       <c r="C45" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -6089,7 +6089,7 @@
         <v>1150</v>
       </c>
       <c r="J51" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="K51" t="s">
         <v>886</v>
@@ -6143,7 +6143,7 @@
         <v>87</v>
       </c>
       <c r="C57" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.25">
@@ -6205,7 +6205,7 @@
         <v>357</v>
       </c>
       <c r="J64" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="K64" t="s">
         <v>886</v>
@@ -6281,7 +6281,7 @@
         <v>1142</v>
       </c>
       <c r="J72" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="K72" t="s">
         <v>1151</v>
@@ -6335,7 +6335,7 @@
         <v>87</v>
       </c>
       <c r="C78" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="79" spans="2:12" x14ac:dyDescent="0.25">
@@ -6397,7 +6397,7 @@
         <v>366</v>
       </c>
       <c r="J85" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="K85" t="s">
         <v>1151</v>
@@ -6504,7 +6504,7 @@
         <v>1152</v>
       </c>
       <c r="J97" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="K97" t="s">
         <v>1154</v>
@@ -6591,7 +6591,7 @@
         <v>372</v>
       </c>
       <c r="J106" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="K106" t="s">
         <v>1154</v>
@@ -6667,7 +6667,7 @@
         <v>1159</v>
       </c>
       <c r="J114" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="K114" t="s">
         <v>1162</v>
@@ -6778,7 +6778,7 @@
         <v>377</v>
       </c>
       <c r="J126" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="K126" t="s">
         <v>1162</v>
@@ -6854,7 +6854,7 @@
         <v>1164</v>
       </c>
       <c r="J134" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="K134" t="s">
         <v>1167</v>
@@ -6965,7 +6965,7 @@
         <v>381</v>
       </c>
       <c r="J146" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="K146" t="s">
         <v>1167</v>
@@ -7041,7 +7041,7 @@
         <v>1169</v>
       </c>
       <c r="J154" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="K154" t="s">
         <v>1172</v>
@@ -7152,7 +7152,7 @@
         <v>385</v>
       </c>
       <c r="J166" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="K166" t="s">
         <v>1172</v>
@@ -7214,7 +7214,7 @@
     </row>
     <row r="174" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A174" s="78" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="B174" t="s">
         <v>87</v>
@@ -7235,7 +7235,7 @@
         <v>87</v>
       </c>
       <c r="C176" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
@@ -7272,7 +7272,7 @@
         <v>87</v>
       </c>
       <c r="C180" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
@@ -7309,7 +7309,7 @@
         <v>87</v>
       </c>
       <c r="C184" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
@@ -7346,7 +7346,7 @@
         <v>87</v>
       </c>
       <c r="C188" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
@@ -7411,7 +7411,7 @@
         <v>1152</v>
       </c>
       <c r="J194" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="K194" t="s">
         <v>1154</v>
@@ -7527,7 +7527,7 @@
         <v>372</v>
       </c>
       <c r="J207" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="K207" t="s">
         <v>1154</v>
@@ -7603,7 +7603,7 @@
         <v>1159</v>
       </c>
       <c r="J215" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="K215" t="s">
         <v>1162</v>
@@ -7743,7 +7743,7 @@
         <v>377</v>
       </c>
       <c r="J231" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="K231" t="s">
         <v>1162</v>
@@ -7819,7 +7819,7 @@
         <v>1164</v>
       </c>
       <c r="J239" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="K239" t="s">
         <v>1167</v>
@@ -7959,7 +7959,7 @@
         <v>381</v>
       </c>
       <c r="J255" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="K255" t="s">
         <v>1167</v>
@@ -8035,7 +8035,7 @@
         <v>1169</v>
       </c>
       <c r="J263" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="K263" t="s">
         <v>1172</v>
@@ -8175,7 +8175,7 @@
         <v>385</v>
       </c>
       <c r="J279" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="K279" t="s">
         <v>1172</v>
@@ -8282,7 +8282,7 @@
         <v>1182</v>
       </c>
       <c r="J291" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="K291" t="s">
         <v>1174</v>
@@ -8369,7 +8369,7 @@
         <v>389</v>
       </c>
       <c r="J300" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="K300" t="s">
         <v>1174</v>
@@ -8445,7 +8445,7 @@
         <v>1186</v>
       </c>
       <c r="J308" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="K308" t="s">
         <v>1176</v>
@@ -8556,7 +8556,7 @@
         <v>394</v>
       </c>
       <c r="J320" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="K320" t="s">
         <v>1176</v>
@@ -8632,7 +8632,7 @@
         <v>1189</v>
       </c>
       <c r="J328" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="K328" t="s">
         <v>1178</v>
@@ -8743,7 +8743,7 @@
         <v>398</v>
       </c>
       <c r="J340" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="K340" t="s">
         <v>1178</v>
@@ -8819,7 +8819,7 @@
         <v>1192</v>
       </c>
       <c r="J348" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="K348" t="s">
         <v>1180</v>
@@ -8930,7 +8930,7 @@
         <v>402</v>
       </c>
       <c r="J360" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="K360" t="s">
         <v>1180</v>
@@ -8992,7 +8992,7 @@
     </row>
     <row r="368" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A368" s="24" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="B368" t="s">
         <v>87</v>
@@ -9013,7 +9013,7 @@
         <v>87</v>
       </c>
       <c r="C370" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="371" spans="1:9" x14ac:dyDescent="0.25">
@@ -9050,7 +9050,7 @@
         <v>87</v>
       </c>
       <c r="C374" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="375" spans="1:9" x14ac:dyDescent="0.25">
@@ -9087,7 +9087,7 @@
         <v>87</v>
       </c>
       <c r="C378" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="379" spans="1:9" x14ac:dyDescent="0.25">
@@ -9124,7 +9124,7 @@
         <v>87</v>
       </c>
       <c r="C382" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="383" spans="1:9" x14ac:dyDescent="0.25">
@@ -9161,7 +9161,7 @@
         <v>87</v>
       </c>
       <c r="C386" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="387" spans="1:9" x14ac:dyDescent="0.25">
@@ -9198,7 +9198,7 @@
         <v>87</v>
       </c>
       <c r="C390" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="391" spans="1:9" x14ac:dyDescent="0.25">
@@ -9235,7 +9235,7 @@
         <v>87</v>
       </c>
       <c r="C394" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="395" spans="1:9" x14ac:dyDescent="0.25">
@@ -9272,7 +9272,7 @@
         <v>87</v>
       </c>
       <c r="C398" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="399" spans="1:9" x14ac:dyDescent="0.25">
@@ -9337,7 +9337,7 @@
         <v>1182</v>
       </c>
       <c r="J404" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="K404" t="s">
         <v>1174</v>
@@ -9391,7 +9391,7 @@
         <v>87</v>
       </c>
       <c r="C410" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="411" spans="1:12" x14ac:dyDescent="0.25">
@@ -9453,7 +9453,7 @@
         <v>389</v>
       </c>
       <c r="J417" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="K417" t="s">
         <v>1174</v>
@@ -9529,7 +9529,7 @@
         <v>1186</v>
       </c>
       <c r="J425" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="K425" t="s">
         <v>1176</v>
@@ -9607,7 +9607,7 @@
         <v>87</v>
       </c>
       <c r="C434" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="435" spans="2:12" x14ac:dyDescent="0.25">
@@ -9669,7 +9669,7 @@
         <v>394</v>
       </c>
       <c r="J441" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="K441" t="s">
         <v>1176</v>
@@ -9745,7 +9745,7 @@
         <v>1189</v>
       </c>
       <c r="J449" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="K449" t="s">
         <v>1178</v>
@@ -9823,7 +9823,7 @@
         <v>87</v>
       </c>
       <c r="C458" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="459" spans="2:12" x14ac:dyDescent="0.25">
@@ -9885,7 +9885,7 @@
         <v>398</v>
       </c>
       <c r="J465" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="K465" t="s">
         <v>1178</v>
@@ -9961,7 +9961,7 @@
         <v>1192</v>
       </c>
       <c r="J473" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="K473" t="s">
         <v>1180</v>
@@ -10039,7 +10039,7 @@
         <v>87</v>
       </c>
       <c r="C482" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="483" spans="2:12" x14ac:dyDescent="0.25">
@@ -10101,7 +10101,7 @@
         <v>402</v>
       </c>
       <c r="J489" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="K489" t="s">
         <v>1180</v>
@@ -10208,7 +10208,7 @@
         <v>1195</v>
       </c>
       <c r="J501" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="K501" t="s">
         <v>1205</v>
@@ -10295,7 +10295,7 @@
         <v>406</v>
       </c>
       <c r="J510" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="K510" t="s">
         <v>1205</v>
@@ -10371,7 +10371,7 @@
         <v>1199</v>
       </c>
       <c r="J518" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="K518" t="s">
         <v>1207</v>
@@ -10482,7 +10482,7 @@
         <v>411</v>
       </c>
       <c r="J530" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="K530" t="s">
         <v>1207</v>
@@ -10558,7 +10558,7 @@
         <v>1202</v>
       </c>
       <c r="J538" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="K538" t="s">
         <v>1209</v>
@@ -10669,7 +10669,7 @@
         <v>415</v>
       </c>
       <c r="J550" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="K550" t="s">
         <v>1133</v>
@@ -10745,7 +10745,7 @@
         <v>419</v>
       </c>
       <c r="J558" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="K558" t="s">
         <v>1134</v>
@@ -10856,7 +10856,7 @@
         <v>419</v>
       </c>
       <c r="J570" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="K570" t="s">
         <v>1134</v>
@@ -10918,7 +10918,7 @@
     </row>
     <row r="578" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A578" s="78" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="B578" t="s">
         <v>87</v>
@@ -10939,7 +10939,7 @@
         <v>87</v>
       </c>
       <c r="C580" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="581" spans="1:9" x14ac:dyDescent="0.25">
@@ -10976,7 +10976,7 @@
         <v>87</v>
       </c>
       <c r="C584" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="585" spans="1:9" x14ac:dyDescent="0.25">
@@ -11013,7 +11013,7 @@
         <v>87</v>
       </c>
       <c r="C588" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="589" spans="1:9" x14ac:dyDescent="0.25">
@@ -11050,7 +11050,7 @@
         <v>87</v>
       </c>
       <c r="C592" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="593" spans="1:9" x14ac:dyDescent="0.25">
@@ -11087,7 +11087,7 @@
         <v>87</v>
       </c>
       <c r="C596" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="597" spans="1:9" x14ac:dyDescent="0.25">
@@ -11124,7 +11124,7 @@
         <v>87</v>
       </c>
       <c r="C600" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="601" spans="1:9" x14ac:dyDescent="0.25">
@@ -11161,7 +11161,7 @@
         <v>87</v>
       </c>
       <c r="C604" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="605" spans="1:9" x14ac:dyDescent="0.25">
@@ -11198,7 +11198,7 @@
         <v>87</v>
       </c>
       <c r="C608" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="609" spans="1:12" x14ac:dyDescent="0.25">
@@ -11235,7 +11235,7 @@
         <v>87</v>
       </c>
       <c r="C612" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="613" spans="1:12" x14ac:dyDescent="0.25">
@@ -11272,7 +11272,7 @@
         <v>87</v>
       </c>
       <c r="C616" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="617" spans="1:12" x14ac:dyDescent="0.25">
@@ -11337,7 +11337,7 @@
         <v>1195</v>
       </c>
       <c r="J622" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="K622" t="s">
         <v>1205</v>
@@ -11391,7 +11391,7 @@
         <v>87</v>
       </c>
       <c r="C628" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="629" spans="2:12" x14ac:dyDescent="0.25">
@@ -11453,7 +11453,7 @@
         <v>406</v>
       </c>
       <c r="J635" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="K635" t="s">
         <v>1205</v>
@@ -11529,7 +11529,7 @@
         <v>1199</v>
       </c>
       <c r="J643" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="K643" t="s">
         <v>1207</v>
@@ -11607,7 +11607,7 @@
         <v>87</v>
       </c>
       <c r="C652" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="653" spans="2:12" x14ac:dyDescent="0.25">
@@ -11669,7 +11669,7 @@
         <v>411</v>
       </c>
       <c r="J659" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="K659" t="s">
         <v>1207</v>
@@ -11745,7 +11745,7 @@
         <v>1202</v>
       </c>
       <c r="J667" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="K667" t="s">
         <v>1209</v>
@@ -11823,7 +11823,7 @@
         <v>87</v>
       </c>
       <c r="C676" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="677" spans="2:12" x14ac:dyDescent="0.25">
@@ -11885,7 +11885,7 @@
         <v>415</v>
       </c>
       <c r="J683" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="K683" t="s">
         <v>1133</v>
@@ -11961,7 +11961,7 @@
         <v>419</v>
       </c>
       <c r="J691" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="K691" t="s">
         <v>1134</v>
@@ -12039,7 +12039,7 @@
         <v>87</v>
       </c>
       <c r="C700" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="701" spans="2:12" x14ac:dyDescent="0.25">
@@ -12101,7 +12101,7 @@
         <v>419</v>
       </c>
       <c r="J707" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="K707" t="s">
         <v>1134</v>
@@ -12202,19 +12202,19 @@
         <v>423</v>
       </c>
       <c r="G719" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="H719" t="s">
         <v>1214</v>
       </c>
       <c r="J719" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="K719" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="L719" t="s">
-        <v>1217</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="720" spans="1:12" x14ac:dyDescent="0.25">
@@ -12270,7 +12270,7 @@
         <v>143</v>
       </c>
       <c r="G726" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="H726" t="s">
         <v>1215</v>
@@ -12286,7 +12286,7 @@
         <v>143</v>
       </c>
       <c r="G728" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="H728" t="s">
         <v>1216</v>
@@ -12324,13 +12324,13 @@
         <v>423</v>
       </c>
       <c r="J732" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="K732" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="L732" t="s">
-        <v>1217</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="733" spans="2:12" x14ac:dyDescent="0.25">
@@ -12394,19 +12394,19 @@
         <v>428</v>
       </c>
       <c r="G740" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="H740" t="s">
+        <v>1225</v>
+      </c>
+      <c r="J740" t="s">
+        <v>1300</v>
+      </c>
+      <c r="K740" t="s">
+        <v>1224</v>
+      </c>
+      <c r="L740" t="s">
         <v>1226</v>
-      </c>
-      <c r="J740" t="s">
-        <v>1301</v>
-      </c>
-      <c r="K740" t="s">
-        <v>1225</v>
-      </c>
-      <c r="L740" t="s">
-        <v>1227</v>
       </c>
     </row>
     <row r="741" spans="2:12" x14ac:dyDescent="0.25">
@@ -12462,10 +12462,10 @@
         <v>143</v>
       </c>
       <c r="G747" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="H747" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="748" spans="2:12" x14ac:dyDescent="0.25">
@@ -12478,10 +12478,10 @@
         <v>143</v>
       </c>
       <c r="G749" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="H749" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="750" spans="2:12" x14ac:dyDescent="0.25">
@@ -12516,13 +12516,13 @@
         <v>428</v>
       </c>
       <c r="J753" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="K753" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="L753" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="754" spans="1:12" x14ac:dyDescent="0.25">
@@ -12578,7 +12578,7 @@
     </row>
     <row r="761" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A761" s="24" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="B761" t="s">
         <v>87</v>
@@ -12599,7 +12599,7 @@
         <v>87</v>
       </c>
       <c r="C763" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="764" spans="1:12" x14ac:dyDescent="0.25">
@@ -12636,7 +12636,7 @@
         <v>87</v>
       </c>
       <c r="C767" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="768" spans="1:12" x14ac:dyDescent="0.25">
@@ -12673,7 +12673,7 @@
         <v>87</v>
       </c>
       <c r="C771" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="D771" s="43"/>
       <c r="E771" s="43"/>
@@ -12714,7 +12714,7 @@
         <v>87</v>
       </c>
       <c r="C775" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="776" spans="1:12" x14ac:dyDescent="0.25">
@@ -12773,19 +12773,19 @@
         <v>423</v>
       </c>
       <c r="G781" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="H781" t="s">
         <v>1214</v>
       </c>
       <c r="J781" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="K781" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="L781" t="s">
-        <v>1217</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="782" spans="1:12" x14ac:dyDescent="0.25">
@@ -12833,7 +12833,7 @@
         <v>87</v>
       </c>
       <c r="C787" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="788" spans="2:12" x14ac:dyDescent="0.25">
@@ -12841,7 +12841,7 @@
         <v>143</v>
       </c>
       <c r="G788" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="H788" t="s">
         <v>1215</v>
@@ -12857,7 +12857,7 @@
         <v>143</v>
       </c>
       <c r="G790" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="H790" t="s">
         <v>1216</v>
@@ -12895,13 +12895,13 @@
         <v>423</v>
       </c>
       <c r="J794" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="K794" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="L794" t="s">
-        <v>1217</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="795" spans="2:12" x14ac:dyDescent="0.25">
@@ -12965,19 +12965,19 @@
         <v>428</v>
       </c>
       <c r="G802" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="H802" t="s">
+        <v>1225</v>
+      </c>
+      <c r="J802" t="s">
+        <v>1300</v>
+      </c>
+      <c r="K802" t="s">
+        <v>1224</v>
+      </c>
+      <c r="L802" t="s">
         <v>1226</v>
-      </c>
-      <c r="J802" t="s">
-        <v>1301</v>
-      </c>
-      <c r="K802" t="s">
-        <v>1225</v>
-      </c>
-      <c r="L802" t="s">
-        <v>1227</v>
       </c>
     </row>
     <row r="803" spans="2:12" x14ac:dyDescent="0.25">
@@ -13025,7 +13025,7 @@
         <v>87</v>
       </c>
       <c r="C808" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="809" spans="2:12" x14ac:dyDescent="0.25">
@@ -13033,10 +13033,10 @@
         <v>143</v>
       </c>
       <c r="G809" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="H809" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="810" spans="2:12" x14ac:dyDescent="0.25">
@@ -13049,10 +13049,10 @@
         <v>143</v>
       </c>
       <c r="G811" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="H811" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="812" spans="2:12" x14ac:dyDescent="0.25">
@@ -13087,13 +13087,13 @@
         <v>428</v>
       </c>
       <c r="J815" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="K815" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="L815" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="816" spans="2:12" x14ac:dyDescent="0.25">
@@ -13177,13 +13177,13 @@
         <v>578</v>
       </c>
       <c r="F826" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G826" t="s">
         <v>1412</v>
       </c>
-      <c r="G826" t="s">
+      <c r="H826" t="s">
         <v>1413</v>
-      </c>
-      <c r="H826" t="s">
-        <v>1414</v>
       </c>
     </row>
     <row r="827" spans="1:9" x14ac:dyDescent="0.25">
@@ -13196,7 +13196,7 @@
         <v>87</v>
       </c>
       <c r="C828" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="829" spans="1:9" x14ac:dyDescent="0.25">
@@ -13220,13 +13220,13 @@
         <v>117</v>
       </c>
       <c r="F831" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="G831" t="s">
+        <v>1415</v>
+      </c>
+      <c r="H831" t="s">
         <v>1416</v>
-      </c>
-      <c r="H831" t="s">
-        <v>1417</v>
       </c>
     </row>
     <row r="832" spans="1:9" x14ac:dyDescent="0.25">
@@ -13234,13 +13234,13 @@
         <v>72</v>
       </c>
       <c r="F832" t="s">
+        <v>1418</v>
+      </c>
+      <c r="G832" t="s">
         <v>1419</v>
       </c>
-      <c r="G832" t="s">
+      <c r="H832" t="s">
         <v>1420</v>
-      </c>
-      <c r="H832" t="s">
-        <v>1421</v>
       </c>
     </row>
     <row r="833" spans="2:8" x14ac:dyDescent="0.25">
@@ -13255,7 +13255,7 @@
     </row>
     <row r="835" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B835" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="836" spans="2:8" x14ac:dyDescent="0.25">
@@ -13287,13 +13287,13 @@
         <v>578</v>
       </c>
       <c r="F839" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="G839" t="s">
+        <v>1412</v>
+      </c>
+      <c r="H839" t="s">
         <v>1413</v>
-      </c>
-      <c r="H839" t="s">
-        <v>1414</v>
       </c>
     </row>
     <row r="840" spans="2:8" x14ac:dyDescent="0.25">
@@ -13306,7 +13306,7 @@
         <v>87</v>
       </c>
       <c r="C841" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="842" spans="2:8" x14ac:dyDescent="0.25">
@@ -13330,13 +13330,13 @@
         <v>117</v>
       </c>
       <c r="F844" t="s">
+        <v>1424</v>
+      </c>
+      <c r="G844" t="s">
         <v>1425</v>
       </c>
-      <c r="G844" t="s">
+      <c r="H844" t="s">
         <v>1426</v>
-      </c>
-      <c r="H844" t="s">
-        <v>1427</v>
       </c>
     </row>
     <row r="845" spans="2:8" x14ac:dyDescent="0.25">
@@ -13344,13 +13344,13 @@
         <v>72</v>
       </c>
       <c r="F845" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="G845" t="s">
+        <v>1419</v>
+      </c>
+      <c r="H845" t="s">
         <v>1420</v>
-      </c>
-      <c r="H845" t="s">
-        <v>1421</v>
       </c>
     </row>
     <row r="846" spans="2:8" x14ac:dyDescent="0.25">
@@ -13365,7 +13365,7 @@
     </row>
     <row r="848" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B848" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="849" spans="2:8" x14ac:dyDescent="0.25">
@@ -13397,13 +13397,13 @@
         <v>578</v>
       </c>
       <c r="F852" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="G852" t="s">
+        <v>1412</v>
+      </c>
+      <c r="H852" t="s">
         <v>1413</v>
-      </c>
-      <c r="H852" t="s">
-        <v>1414</v>
       </c>
     </row>
     <row r="853" spans="2:8" x14ac:dyDescent="0.25">
@@ -13416,7 +13416,7 @@
         <v>87</v>
       </c>
       <c r="C854" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="855" spans="2:8" x14ac:dyDescent="0.25">
@@ -13440,13 +13440,13 @@
         <v>117</v>
       </c>
       <c r="F857" t="s">
+        <v>1430</v>
+      </c>
+      <c r="G857" t="s">
         <v>1431</v>
       </c>
-      <c r="G857" t="s">
+      <c r="H857" t="s">
         <v>1432</v>
-      </c>
-      <c r="H857" t="s">
-        <v>1433</v>
       </c>
     </row>
     <row r="858" spans="2:8" x14ac:dyDescent="0.25">
@@ -13454,13 +13454,13 @@
         <v>72</v>
       </c>
       <c r="F858" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="G858" t="s">
+        <v>1419</v>
+      </c>
+      <c r="H858" t="s">
         <v>1420</v>
-      </c>
-      <c r="H858" t="s">
-        <v>1421</v>
       </c>
     </row>
     <row r="859" spans="2:8" x14ac:dyDescent="0.25">
@@ -13475,7 +13475,7 @@
     </row>
     <row r="861" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B861" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="862" spans="2:8" x14ac:dyDescent="0.25">
@@ -13507,13 +13507,13 @@
         <v>578</v>
       </c>
       <c r="F865" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="G865" t="s">
+        <v>1412</v>
+      </c>
+      <c r="H865" t="s">
         <v>1413</v>
-      </c>
-      <c r="H865" t="s">
-        <v>1414</v>
       </c>
     </row>
     <row r="866" spans="2:8" x14ac:dyDescent="0.25">
@@ -13526,7 +13526,7 @@
         <v>87</v>
       </c>
       <c r="C867" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="868" spans="2:8" x14ac:dyDescent="0.25">
@@ -13550,13 +13550,13 @@
         <v>117</v>
       </c>
       <c r="F870" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="G870" t="s">
+        <v>1436</v>
+      </c>
+      <c r="H870" t="s">
         <v>1437</v>
-      </c>
-      <c r="H870" t="s">
-        <v>1438</v>
       </c>
     </row>
     <row r="871" spans="2:8" x14ac:dyDescent="0.25">
@@ -13564,13 +13564,13 @@
         <v>72</v>
       </c>
       <c r="F871" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="G871" t="s">
+        <v>1419</v>
+      </c>
+      <c r="H871" t="s">
         <v>1420</v>
-      </c>
-      <c r="H871" t="s">
-        <v>1421</v>
       </c>
     </row>
     <row r="872" spans="2:8" x14ac:dyDescent="0.25">
@@ -13585,7 +13585,7 @@
     </row>
     <row r="874" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B874" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="875" spans="2:8" x14ac:dyDescent="0.25">
@@ -13617,13 +13617,13 @@
         <v>578</v>
       </c>
       <c r="F878" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="G878" t="s">
+        <v>1412</v>
+      </c>
+      <c r="H878" t="s">
         <v>1413</v>
-      </c>
-      <c r="H878" t="s">
-        <v>1414</v>
       </c>
     </row>
     <row r="879" spans="2:8" x14ac:dyDescent="0.25">
@@ -13636,7 +13636,7 @@
         <v>87</v>
       </c>
       <c r="C880" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="881" spans="1:9" x14ac:dyDescent="0.25">
@@ -13660,13 +13660,13 @@
         <v>117</v>
       </c>
       <c r="F883" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="G883" t="s">
+        <v>1442</v>
+      </c>
+      <c r="H883" t="s">
         <v>1443</v>
-      </c>
-      <c r="H883" t="s">
-        <v>1444</v>
       </c>
     </row>
     <row r="884" spans="1:9" x14ac:dyDescent="0.25">
@@ -13674,13 +13674,13 @@
         <v>72</v>
       </c>
       <c r="F884" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="G884" t="s">
+        <v>1419</v>
+      </c>
+      <c r="H884" t="s">
         <v>1420</v>
-      </c>
-      <c r="H884" t="s">
-        <v>1421</v>
       </c>
     </row>
     <row r="885" spans="1:9" x14ac:dyDescent="0.25">
@@ -13695,7 +13695,7 @@
     </row>
     <row r="887" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B887" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="888" spans="1:9" x14ac:dyDescent="0.25">
@@ -14144,7 +14144,7 @@
         <v>742</v>
       </c>
       <c r="J29" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="K29" t="s">
         <v>1136</v>
@@ -14207,7 +14207,7 @@
         <v>742</v>
       </c>
       <c r="J34" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="K34" t="s">
         <v>1136</v>
@@ -15885,7 +15885,7 @@
         <v>674</v>
       </c>
       <c r="B22" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -15893,7 +15893,7 @@
         <v>675</v>
       </c>
       <c r="B23" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -15901,7 +15901,7 @@
         <v>676</v>
       </c>
       <c r="B24" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -15909,7 +15909,7 @@
         <v>677</v>
       </c>
       <c r="B25" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -15917,7 +15917,7 @@
         <v>678</v>
       </c>
       <c r="B26" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -15925,7 +15925,7 @@
         <v>679</v>
       </c>
       <c r="B27" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -15933,7 +15933,7 @@
         <v>680</v>
       </c>
       <c r="B28" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -15941,7 +15941,7 @@
         <v>681</v>
       </c>
       <c r="B29" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -15949,7 +15949,7 @@
         <v>682</v>
       </c>
       <c r="B30" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -15957,7 +15957,7 @@
         <v>683</v>
       </c>
       <c r="B31" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -15965,7 +15965,7 @@
         <v>684</v>
       </c>
       <c r="B32" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -15973,7 +15973,7 @@
         <v>685</v>
       </c>
       <c r="B33" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -15981,7 +15981,7 @@
         <v>686</v>
       </c>
       <c r="B34" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -15989,7 +15989,7 @@
         <v>687</v>
       </c>
       <c r="B35" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -15997,7 +15997,7 @@
         <v>688</v>
       </c>
       <c r="B36" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -16005,7 +16005,7 @@
         <v>690</v>
       </c>
       <c r="B37" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -16013,7 +16013,7 @@
         <v>691</v>
       </c>
       <c r="B38" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -16021,7 +16021,7 @@
         <v>692</v>
       </c>
       <c r="B39" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -16029,7 +16029,7 @@
         <v>693</v>
       </c>
       <c r="B40" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -16037,7 +16037,7 @@
         <v>694</v>
       </c>
       <c r="B41" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -16045,7 +16045,7 @@
         <v>695</v>
       </c>
       <c r="B42" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -16053,7 +16053,7 @@
         <v>696</v>
       </c>
       <c r="B43" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -16061,7 +16061,7 @@
         <v>697</v>
       </c>
       <c r="B44" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -16069,7 +16069,7 @@
         <v>698</v>
       </c>
       <c r="B45" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -16077,7 +16077,7 @@
         <v>699</v>
       </c>
       <c r="B46" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -16085,7 +16085,7 @@
         <v>973</v>
       </c>
       <c r="B47" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -16093,7 +16093,7 @@
         <v>788</v>
       </c>
       <c r="B48" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -16109,7 +16109,7 @@
         <v>790</v>
       </c>
       <c r="B50" s="43" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -16117,7 +16117,7 @@
         <v>791</v>
       </c>
       <c r="B51" s="43" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -16125,7 +16125,7 @@
         <v>792</v>
       </c>
       <c r="B52" s="43" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -16133,7 +16133,7 @@
         <v>793</v>
       </c>
       <c r="B53" s="43" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -16141,7 +16141,7 @@
         <v>794</v>
       </c>
       <c r="B54" s="43" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -16149,7 +16149,7 @@
         <v>795</v>
       </c>
       <c r="B55" s="43" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -16157,7 +16157,7 @@
         <v>796</v>
       </c>
       <c r="B56" s="43" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -16165,7 +16165,7 @@
         <v>797</v>
       </c>
       <c r="B57" s="43" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -16173,7 +16173,7 @@
         <v>798</v>
       </c>
       <c r="B58" s="43" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -16181,7 +16181,7 @@
         <v>799</v>
       </c>
       <c r="B59" s="43" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -16189,7 +16189,7 @@
         <v>800</v>
       </c>
       <c r="B60" s="43" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -16197,7 +16197,7 @@
         <v>801</v>
       </c>
       <c r="B61" s="43" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -16205,7 +16205,7 @@
         <v>802</v>
       </c>
       <c r="B62" s="43" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -16213,7 +16213,7 @@
         <v>803</v>
       </c>
       <c r="B63" s="43" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -16221,7 +16221,7 @@
         <v>804</v>
       </c>
       <c r="B64" s="43" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -16229,7 +16229,7 @@
         <v>805</v>
       </c>
       <c r="B65" s="43" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -16237,7 +16237,7 @@
         <v>806</v>
       </c>
       <c r="B66" s="43" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -16245,7 +16245,7 @@
         <v>807</v>
       </c>
       <c r="B67" s="43" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -16253,7 +16253,7 @@
         <v>808</v>
       </c>
       <c r="B68" s="43" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -16261,7 +16261,7 @@
         <v>809</v>
       </c>
       <c r="B69" s="43" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -16269,7 +16269,7 @@
         <v>810</v>
       </c>
       <c r="B70" s="43" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -16277,7 +16277,7 @@
         <v>811</v>
       </c>
       <c r="B71" s="43" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -16285,7 +16285,7 @@
         <v>812</v>
       </c>
       <c r="B72" s="43" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -16293,7 +16293,7 @@
         <v>813</v>
       </c>
       <c r="B73" s="43" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -16301,7 +16301,7 @@
         <v>814</v>
       </c>
       <c r="B74" s="43" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -16309,7 +16309,7 @@
         <v>972</v>
       </c>
       <c r="B75" s="43" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -16317,7 +16317,7 @@
         <v>815</v>
       </c>
       <c r="B76" s="43" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
     </row>
   </sheetData>
@@ -16468,7 +16468,7 @@
         <v>166</v>
       </c>
       <c r="D8" s="48" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="E8" s="48"/>
     </row>
@@ -17046,10 +17046,10 @@
         <v>2</v>
       </c>
       <c r="C45" s="43" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="D45" s="51" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="E45" s="51"/>
     </row>
@@ -17681,10 +17681,10 @@
         <v>D:NS,M:NS,Y:NS</v>
       </c>
       <c r="C86" t="s">
+        <v>1465</v>
+      </c>
+      <c r="D86" t="s">
         <v>1466</v>
-      </c>
-      <c r="D86" t="s">
-        <v>1467</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -17719,23 +17719,23 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="B89" t="str">
         <f>"88"</f>
         <v>88</v>
       </c>
       <c r="C89" t="s">
+        <v>1328</v>
+      </c>
+      <c r="D89" t="s">
         <v>1329</v>
-      </c>
-      <c r="D89" t="s">
-        <v>1330</v>
       </c>
       <c r="E89" s="48"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="B90" t="str">
         <f>"99"</f>
@@ -17751,87 +17751,87 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="B91" t="str">
         <f>"99"</f>
         <v>99</v>
       </c>
       <c r="C91" t="s">
+        <v>1461</v>
+      </c>
+      <c r="D91" t="s">
         <v>1462</v>
-      </c>
-      <c r="D91" t="s">
-        <v>1463</v>
       </c>
       <c r="E91" s="48"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="B92" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C92" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D92" t="s">
         <v>1371</v>
-      </c>
-      <c r="D92" t="s">
-        <v>1372</v>
       </c>
       <c r="E92" s="48"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="B93" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C93" t="s">
+        <v>1372</v>
+      </c>
+      <c r="D93" t="s">
         <v>1373</v>
-      </c>
-      <c r="D93" t="s">
-        <v>1374</v>
       </c>
       <c r="E93" s="48"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="B94" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
       <c r="C94" t="s">
+        <v>1374</v>
+      </c>
+      <c r="D94" t="s">
         <v>1375</v>
-      </c>
-      <c r="D94" t="s">
-        <v>1376</v>
       </c>
       <c r="E94" s="48"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="B95" t="str">
         <f>"4"</f>
         <v>4</v>
       </c>
       <c r="C95" t="s">
+        <v>1376</v>
+      </c>
+      <c r="D95" t="s">
         <v>1377</v>
-      </c>
-      <c r="D95" t="s">
-        <v>1378</v>
       </c>
       <c r="E95" s="48"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="B96" t="str">
         <f>"9"</f>
@@ -17847,52 +17847,52 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="B97" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C97" t="s">
+        <v>1378</v>
+      </c>
+      <c r="D97" t="s">
         <v>1379</v>
-      </c>
-      <c r="D97" t="s">
-        <v>1380</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="B98" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C98" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="D98" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="B99" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
       <c r="C99" t="s">
+        <v>1381</v>
+      </c>
+      <c r="D99" t="s">
         <v>1382</v>
-      </c>
-      <c r="D99" t="s">
-        <v>1383</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="B100" t="str">
         <f>"9"</f>
@@ -17907,22 +17907,22 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="46" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="B101" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C101" s="43" t="s">
+        <v>1479</v>
+      </c>
+      <c r="D101" s="43" t="s">
         <v>1480</v>
-      </c>
-      <c r="D101" s="43" t="s">
-        <v>1481</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="46" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="B102" t="str">
         <f>"2"</f>
@@ -17937,7 +17937,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="46" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="B103" t="str">
         <f>"3"</f>
@@ -17947,7 +17947,7 @@
         <v>167</v>
       </c>
       <c r="D103" s="43" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
     </row>
   </sheetData>
@@ -18224,24 +18224,24 @@
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1310</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1311</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1312</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B2" t="s">
         <v>1313</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>1314</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1315</v>
       </c>
     </row>
   </sheetData>
@@ -18531,7 +18531,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="B25" t="s">
         <v>22</v>
@@ -18806,7 +18806,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="B50" t="s">
         <v>117</v>
@@ -18817,7 +18817,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="B51" t="s">
         <v>318</v>
@@ -18828,7 +18828,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="B52" t="s">
         <v>117</v>
@@ -18839,7 +18839,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="B53" t="s">
         <v>318</v>
@@ -18850,7 +18850,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="B54" t="s">
         <v>117</v>
@@ -18861,7 +18861,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="B55" t="s">
         <v>318</v>
@@ -18872,7 +18872,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="B56" t="s">
         <v>117</v>
@@ -18883,7 +18883,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="B57" t="s">
         <v>318</v>
@@ -18908,7 +18908,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="B60" t="s">
         <v>22</v>
@@ -18922,7 +18922,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="B61" t="s">
         <v>22</v>
@@ -18933,7 +18933,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="B62" t="s">
         <v>72</v>
@@ -18944,7 +18944,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="B63" t="s">
         <v>22</v>
@@ -18955,7 +18955,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="B64" t="s">
         <v>117</v>
@@ -18966,7 +18966,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="B65" t="s">
         <v>22</v>
@@ -18977,7 +18977,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="B66" t="s">
         <v>22</v>
@@ -18988,7 +18988,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="B67" t="s">
         <v>72</v>
@@ -18999,7 +18999,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="B69" t="s">
         <v>22</v>
@@ -19008,12 +19008,12 @@
         <v>1</v>
       </c>
       <c r="D69" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="B70" t="s">
         <v>22</v>
@@ -19024,7 +19024,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="B71" t="s">
         <v>72</v>
@@ -19035,7 +19035,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="B72" t="s">
         <v>25</v>
@@ -19046,7 +19046,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="B73" t="s">
         <v>25</v>
@@ -19057,7 +19057,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="B74" t="s">
         <v>25</v>
@@ -19068,7 +19068,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="B75" t="s">
         <v>72</v>
@@ -19079,7 +19079,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="B76" t="s">
         <v>123</v>
@@ -19104,7 +19104,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="46" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
       <c r="B79" s="48" t="s">
         <v>50</v>
@@ -19115,7 +19115,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="46" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="B80" s="48" t="s">
         <v>50</v>
@@ -19126,7 +19126,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="46" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="B81" s="48" t="s">
         <v>50</v>
@@ -19137,7 +19137,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="46" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="B82" s="46" t="s">
         <v>22</v>
@@ -19286,7 +19286,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="B95" s="46" t="s">
         <v>117</v>
@@ -19297,7 +19297,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="46" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="B96" s="48" t="s">
         <v>25</v>
@@ -19308,7 +19308,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="48" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="B97" s="48" t="s">
         <v>318</v>
@@ -19319,7 +19319,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="46" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="B98" s="48" t="s">
         <v>25</v>
@@ -19330,7 +19330,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="46" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="B99" s="46" t="s">
         <v>318</v>
@@ -19451,7 +19451,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="48" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="B110" s="48" t="s">
         <v>25</v>
@@ -19820,7 +19820,7 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="B144" t="s">
         <v>22</v>
@@ -19834,7 +19834,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="B145" t="s">
         <v>22</v>
@@ -19845,7 +19845,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="B146" t="s">
         <v>22</v>
@@ -19856,7 +19856,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="B147" t="s">
         <v>22</v>
@@ -19867,7 +19867,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="B148" t="s">
         <v>22</v>
@@ -20610,7 +20610,7 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="B211" t="s">
         <v>117</v>
@@ -20621,7 +20621,7 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="B212" t="s">
         <v>72</v>
@@ -20632,7 +20632,7 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="B213" t="s">
         <v>117</v>
@@ -20643,7 +20643,7 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B214" t="s">
         <v>72</v>
@@ -20654,7 +20654,7 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="B215" t="s">
         <v>117</v>
@@ -20665,7 +20665,7 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="B216" t="s">
         <v>72</v>
@@ -20676,7 +20676,7 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="B217" t="s">
         <v>117</v>
@@ -20687,7 +20687,7 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="B218" t="s">
         <v>72</v>
@@ -20698,7 +20698,7 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="B219" t="s">
         <v>117</v>
@@ -20709,7 +20709,7 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="B220" t="s">
         <v>72</v>
@@ -21657,12 +21657,12 @@
         <v>87</v>
       </c>
       <c r="C5" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -21879,7 +21879,7 @@
         <v>953</v>
       </c>
       <c r="H15" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="I15" s="46"/>
     </row>
@@ -22015,10 +22015,10 @@
         <v>116</v>
       </c>
       <c r="G26" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="H26" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="I26" s="46"/>
     </row>
@@ -22207,7 +22207,7 @@
         <v>953</v>
       </c>
       <c r="H44" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="I44" s="46"/>
     </row>
@@ -22898,10 +22898,10 @@
         <v>116</v>
       </c>
       <c r="G47" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="H47" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="I47" s="46"/>
     </row>
@@ -23068,12 +23068,12 @@
         <v>87</v>
       </c>
       <c r="C64" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -23087,7 +23087,7 @@
         <v>87</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -23354,13 +23354,13 @@
         <v>92</v>
       </c>
       <c r="F20" t="s">
+        <v>1385</v>
+      </c>
+      <c r="G20" t="s">
         <v>1386</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>1387</v>
-      </c>
-      <c r="H20" t="s">
-        <v>1388</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
@@ -23445,7 +23445,7 @@
         <v>87</v>
       </c>
       <c r="C29" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
@@ -23469,10 +23469,10 @@
         <v>143</v>
       </c>
       <c r="G32" t="s">
+        <v>1389</v>
+      </c>
+      <c r="H32" t="s">
         <v>1390</v>
-      </c>
-      <c r="H32" t="s">
-        <v>1391</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
@@ -23480,13 +23480,13 @@
         <v>117</v>
       </c>
       <c r="F33" t="s">
+        <v>1391</v>
+      </c>
+      <c r="G33" t="s">
         <v>1392</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>1393</v>
-      </c>
-      <c r="H33" t="s">
-        <v>1394</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
@@ -23497,7 +23497,7 @@
         <v>359</v>
       </c>
       <c r="F34" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
@@ -23505,7 +23505,7 @@
         <v>87</v>
       </c>
       <c r="C35" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
@@ -23513,7 +23513,7 @@
         <v>123</v>
       </c>
       <c r="F36" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="I36" t="s">
         <v>362</v>
@@ -23529,13 +23529,13 @@
         <v>117</v>
       </c>
       <c r="F38" t="s">
+        <v>1396</v>
+      </c>
+      <c r="G38" t="s">
         <v>1397</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>1398</v>
-      </c>
-      <c r="H38" t="s">
-        <v>1399</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
@@ -23546,7 +23546,7 @@
         <v>359</v>
       </c>
       <c r="F39" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
@@ -23554,7 +23554,7 @@
         <v>87</v>
       </c>
       <c r="C40" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
@@ -23562,7 +23562,7 @@
         <v>123</v>
       </c>
       <c r="F41" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="I41" t="s">
         <v>362</v>
@@ -23578,13 +23578,13 @@
         <v>117</v>
       </c>
       <c r="F43" t="s">
+        <v>1401</v>
+      </c>
+      <c r="G43" t="s">
         <v>1402</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>1403</v>
-      </c>
-      <c r="H43" t="s">
-        <v>1404</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
@@ -23595,7 +23595,7 @@
         <v>359</v>
       </c>
       <c r="F44" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
@@ -23603,7 +23603,7 @@
         <v>87</v>
       </c>
       <c r="C45" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
@@ -23611,7 +23611,7 @@
         <v>123</v>
       </c>
       <c r="F46" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="I46" t="s">
         <v>362</v>
@@ -23627,13 +23627,13 @@
         <v>117</v>
       </c>
       <c r="F48" t="s">
+        <v>1406</v>
+      </c>
+      <c r="G48" t="s">
         <v>1407</v>
       </c>
-      <c r="G48" t="s">
+      <c r="H48" t="s">
         <v>1408</v>
-      </c>
-      <c r="H48" t="s">
-        <v>1409</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
@@ -23644,7 +23644,7 @@
         <v>359</v>
       </c>
       <c r="F49" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
@@ -23652,7 +23652,7 @@
         <v>87</v>
       </c>
       <c r="C50" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
@@ -23660,7 +23660,7 @@
         <v>123</v>
       </c>
       <c r="F51" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="I51" t="s">
         <v>362</v>
@@ -23752,10 +23752,10 @@
         <v>136</v>
       </c>
       <c r="G61" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H61" s="50" t="s">
         <v>1384</v>
-      </c>
-      <c r="H61" s="50" t="s">
-        <v>1385</v>
       </c>
       <c r="I61" s="46"/>
     </row>
@@ -23815,7 +23815,7 @@
         <v>318</v>
       </c>
       <c r="E67" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="F67" t="s">
         <v>819</v>
@@ -23826,7 +23826,7 @@
         <v>87</v>
       </c>
       <c r="C68" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.25">
@@ -23837,7 +23837,7 @@
         <v>145</v>
       </c>
       <c r="I69" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.25">
@@ -23850,7 +23850,7 @@
         <v>87</v>
       </c>
       <c r="C71" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.25">
@@ -23861,7 +23861,7 @@
         <v>145</v>
       </c>
       <c r="I72" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.25">
@@ -23955,7 +23955,7 @@
         <v>318</v>
       </c>
       <c r="E82" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="F82" t="s">
         <v>820</v>
@@ -23966,7 +23966,7 @@
         <v>87</v>
       </c>
       <c r="C83" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.25">
@@ -23977,7 +23977,7 @@
         <v>152</v>
       </c>
       <c r="I84" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
@@ -23990,7 +23990,7 @@
         <v>87</v>
       </c>
       <c r="C86" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
@@ -24001,7 +24001,7 @@
         <v>152</v>
       </c>
       <c r="I87" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
@@ -24095,7 +24095,7 @@
         <v>318</v>
       </c>
       <c r="E97" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="F97" t="s">
         <v>821</v>
@@ -24106,7 +24106,7 @@
         <v>87</v>
       </c>
       <c r="C98" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
@@ -24117,7 +24117,7 @@
         <v>154</v>
       </c>
       <c r="I99" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.25">
@@ -24130,7 +24130,7 @@
         <v>87</v>
       </c>
       <c r="C101" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.25">
@@ -24141,7 +24141,7 @@
         <v>154</v>
       </c>
       <c r="I102" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.25">
@@ -24621,12 +24621,12 @@
         <v>87</v>
       </c>
       <c r="C149" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
@@ -24697,7 +24697,7 @@
         <v>23</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -24710,10 +24710,10 @@
         <v>143</v>
       </c>
       <c r="G3" t="s">
+        <v>1348</v>
+      </c>
+      <c r="H3" t="s">
         <v>1349</v>
-      </c>
-      <c r="H3" t="s">
-        <v>1350</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -24721,16 +24721,16 @@
         <v>22</v>
       </c>
       <c r="E4" t="s">
+        <v>1350</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1344</v>
+      </c>
+      <c r="G4" t="s">
         <v>1351</v>
       </c>
-      <c r="F4" t="s">
-        <v>1345</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>1352</v>
-      </c>
-      <c r="H4" t="s">
-        <v>1353</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -24738,16 +24738,16 @@
         <v>22</v>
       </c>
       <c r="E5" t="s">
+        <v>1353</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1339</v>
+      </c>
+      <c r="G5" t="s">
         <v>1354</v>
       </c>
-      <c r="F5" t="s">
-        <v>1340</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>1355</v>
-      </c>
-      <c r="H5" t="s">
-        <v>1356</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -24765,10 +24765,10 @@
         <v>143</v>
       </c>
       <c r="G8" t="s">
+        <v>1348</v>
+      </c>
+      <c r="H8" t="s">
         <v>1349</v>
-      </c>
-      <c r="H8" t="s">
-        <v>1350</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -24779,13 +24779,13 @@
         <v>92</v>
       </c>
       <c r="F9" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="G9" t="s">
+        <v>1356</v>
+      </c>
+      <c r="H9" t="s">
         <v>1357</v>
-      </c>
-      <c r="H9" t="s">
-        <v>1358</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -24796,13 +24796,13 @@
         <v>92</v>
       </c>
       <c r="F10" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="G10" t="s">
+        <v>1358</v>
+      </c>
+      <c r="H10" t="s">
         <v>1359</v>
-      </c>
-      <c r="H10" t="s">
-        <v>1360</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -24820,10 +24820,10 @@
         <v>143</v>
       </c>
       <c r="G13" t="s">
+        <v>1348</v>
+      </c>
+      <c r="H13" t="s">
         <v>1349</v>
-      </c>
-      <c r="H13" t="s">
-        <v>1350</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -24834,13 +24834,13 @@
         <v>92</v>
       </c>
       <c r="F14" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="G14" t="s">
+        <v>1360</v>
+      </c>
+      <c r="H14" t="s">
         <v>1361</v>
-      </c>
-      <c r="H14" t="s">
-        <v>1362</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -24848,16 +24848,16 @@
         <v>72</v>
       </c>
       <c r="F15" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="G15" t="s">
+        <v>1362</v>
+      </c>
+      <c r="H15" t="s">
         <v>1363</v>
       </c>
-      <c r="H15" t="s">
+      <c r="J15" t="s">
         <v>1364</v>
-      </c>
-      <c r="J15" t="s">
-        <v>1365</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -24875,10 +24875,10 @@
         <v>143</v>
       </c>
       <c r="G18" t="s">
+        <v>1348</v>
+      </c>
+      <c r="H18" t="s">
         <v>1349</v>
-      </c>
-      <c r="H18" t="s">
-        <v>1350</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -24886,13 +24886,13 @@
         <v>72</v>
       </c>
       <c r="F19" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="G19" t="s">
+        <v>1365</v>
+      </c>
+      <c r="H19" t="s">
         <v>1366</v>
-      </c>
-      <c r="H19" t="s">
-        <v>1367</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -24900,10 +24900,10 @@
         <v>123</v>
       </c>
       <c r="F20" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="I20" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
@@ -24925,7 +24925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC340D6-1B78-4739-B457-F02D66D016E5}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A36" sqref="A36:XFD36"/>
     </sheetView>
@@ -24990,7 +24990,7 @@
         <v>143</v>
       </c>
       <c r="G3" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -24998,7 +24998,7 @@
         <v>143</v>
       </c>
       <c r="G4" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -25006,7 +25006,7 @@
         <v>143</v>
       </c>
       <c r="G5" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -25014,7 +25014,7 @@
         <v>143</v>
       </c>
       <c r="G6" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -25022,7 +25022,7 @@
         <v>143</v>
       </c>
       <c r="G7" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -25030,7 +25030,7 @@
         <v>143</v>
       </c>
       <c r="G8" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -25041,10 +25041,10 @@
         <v>578</v>
       </c>
       <c r="F9" t="s">
+        <v>1532</v>
+      </c>
+      <c r="G9" t="s">
         <v>1533</v>
-      </c>
-      <c r="G9" t="s">
-        <v>1534</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -25057,7 +25057,7 @@
         <v>87</v>
       </c>
       <c r="C11" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -25070,7 +25070,7 @@
         <v>143</v>
       </c>
       <c r="G13" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -25078,7 +25078,7 @@
         <v>143</v>
       </c>
       <c r="G14" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -25086,7 +25086,7 @@
         <v>143</v>
       </c>
       <c r="G15" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -25094,7 +25094,7 @@
         <v>143</v>
       </c>
       <c r="G16" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
@@ -25102,7 +25102,7 @@
         <v>143</v>
       </c>
       <c r="G17" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
@@ -25113,13 +25113,13 @@
         <v>578</v>
       </c>
       <c r="F18" t="s">
+        <v>1538</v>
+      </c>
+      <c r="G18" t="s">
         <v>1539</v>
       </c>
-      <c r="G18" t="s">
-        <v>1540</v>
-      </c>
       <c r="I18" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -25128,10 +25128,10 @@
       </c>
       <c r="E19" s="43"/>
       <c r="F19" t="s">
+        <v>1557</v>
+      </c>
+      <c r="G19" t="s">
         <v>1558</v>
-      </c>
-      <c r="G19" t="s">
-        <v>1559</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -25144,7 +25144,7 @@
         <v>87</v>
       </c>
       <c r="C21" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
@@ -25157,7 +25157,7 @@
         <v>143</v>
       </c>
       <c r="G23" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
@@ -25165,10 +25165,10 @@
         <v>72</v>
       </c>
       <c r="F24" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="G24" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
@@ -25176,10 +25176,10 @@
         <v>25</v>
       </c>
       <c r="F25" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="G25" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
@@ -25187,10 +25187,10 @@
         <v>25</v>
       </c>
       <c r="F26" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="G26" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
@@ -25198,10 +25198,10 @@
         <v>25</v>
       </c>
       <c r="F27" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="G27" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
@@ -25227,7 +25227,7 @@
         <v>116</v>
       </c>
       <c r="I31" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
@@ -25238,7 +25238,7 @@
         <v>66</v>
       </c>
       <c r="I32" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
@@ -25249,7 +25249,7 @@
         <v>68</v>
       </c>
       <c r="I33" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
@@ -25260,7 +25260,7 @@
         <v>70</v>
       </c>
       <c r="I34" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
@@ -25271,7 +25271,7 @@
         <v>115</v>
       </c>
       <c r="I35" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
@@ -25279,7 +25279,7 @@
         <v>143</v>
       </c>
       <c r="G36" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
@@ -25287,7 +25287,7 @@
         <v>143</v>
       </c>
       <c r="G37" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
@@ -25395,7 +25395,7 @@
         <v>249</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -25656,7 +25656,7 @@
         <v>257</v>
       </c>
       <c r="J28" s="46" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="K28" s="46" t="s">
         <v>1139</v>
@@ -25926,7 +25926,7 @@
         <v>705</v>
       </c>
       <c r="J55" s="46" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="K55" s="46" t="s">
         <v>962</v>
@@ -26047,7 +26047,7 @@
         <v>275</v>
       </c>
       <c r="H67" s="46" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
@@ -26074,7 +26074,7 @@
         <v>707</v>
       </c>
       <c r="J69" s="46" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="K69" s="46" t="s">
         <v>963</v>
@@ -26187,7 +26187,7 @@
         <v>280</v>
       </c>
       <c r="H80" s="46" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -26390,7 +26390,7 @@
         <v>713</v>
       </c>
       <c r="J97" s="46" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="K97" s="46" t="s">
         <v>964</v>
@@ -26541,7 +26541,7 @@
         <v>87</v>
       </c>
       <c r="C113" s="46" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.25">
@@ -26562,13 +26562,13 @@
         <v>117</v>
       </c>
       <c r="F116" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="G116" t="s">
+        <v>1463</v>
+      </c>
+      <c r="H116" t="s">
         <v>1464</v>
-      </c>
-      <c r="H116" t="s">
-        <v>1465</v>
       </c>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.25">
@@ -26579,7 +26579,7 @@
         <v>828</v>
       </c>
       <c r="F117" s="46" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="118" spans="2:9" x14ac:dyDescent="0.25">
@@ -26587,7 +26587,7 @@
         <v>87</v>
       </c>
       <c r="C118" s="46" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.25">
@@ -26595,10 +26595,10 @@
         <v>123</v>
       </c>
       <c r="F119" s="46" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="I119" s="46" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="120" spans="2:9" x14ac:dyDescent="0.25">
@@ -26606,13 +26606,13 @@
         <v>25</v>
       </c>
       <c r="F120" s="46" t="s">
+        <v>1452</v>
+      </c>
+      <c r="G120" s="46" t="s">
         <v>1453</v>
       </c>
-      <c r="G120" s="46" t="s">
-        <v>1454</v>
-      </c>
       <c r="H120" s="46" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="121" spans="2:9" x14ac:dyDescent="0.25">
@@ -26620,13 +26620,13 @@
         <v>25</v>
       </c>
       <c r="F121" s="46" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="G121" s="46" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="H121" s="46" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="122" spans="2:9" x14ac:dyDescent="0.25">
@@ -26634,10 +26634,10 @@
         <v>318</v>
       </c>
       <c r="E122" s="46" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="F122" s="48" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="123" spans="2:9" x14ac:dyDescent="0.25">
@@ -26645,7 +26645,7 @@
         <v>87</v>
       </c>
       <c r="C123" s="46" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="D123" s="48"/>
     </row>
@@ -26654,7 +26654,7 @@
         <v>123</v>
       </c>
       <c r="F124" s="46" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="I124" s="46">
         <v>99</v>
@@ -26665,7 +26665,7 @@
         <v>123</v>
       </c>
       <c r="F125" s="46" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="I125" s="46">
         <v>99</v>
@@ -26865,7 +26865,7 @@
         <v>87</v>
       </c>
       <c r="C148" s="46" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.25">
@@ -27131,7 +27131,7 @@
         <v>87</v>
       </c>
       <c r="C174" s="46" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
@@ -27169,13 +27169,13 @@
         <v>578</v>
       </c>
       <c r="F178" s="46" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="G178" s="48" t="s">
+        <v>1482</v>
+      </c>
+      <c r="H178" s="46" t="s">
         <v>1483</v>
-      </c>
-      <c r="H178" s="46" t="s">
-        <v>1484</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
@@ -27188,7 +27188,7 @@
         <v>87</v>
       </c>
       <c r="C180" s="46" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
@@ -27215,13 +27215,13 @@
         <v>92</v>
       </c>
       <c r="F183" s="46" t="s">
+        <v>1470</v>
+      </c>
+      <c r="G183" s="48" t="s">
         <v>1471</v>
       </c>
-      <c r="G183" s="48" t="s">
+      <c r="H183" s="46" t="s">
         <v>1472</v>
-      </c>
-      <c r="H183" s="46" t="s">
-        <v>1473</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
@@ -27232,13 +27232,13 @@
         <v>92</v>
       </c>
       <c r="F184" s="46" t="s">
+        <v>1473</v>
+      </c>
+      <c r="G184" s="48" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H184" s="46" t="s">
         <v>1474</v>
-      </c>
-      <c r="G184" s="48" t="s">
-        <v>1476</v>
-      </c>
-      <c r="H184" s="46" t="s">
-        <v>1475</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
@@ -27246,16 +27246,16 @@
         <v>50</v>
       </c>
       <c r="E185" s="46" t="s">
+        <v>1476</v>
+      </c>
+      <c r="F185" s="46" t="s">
         <v>1477</v>
-      </c>
-      <c r="F185" s="46" t="s">
-        <v>1478</v>
       </c>
       <c r="G185" s="48" t="s">
         <v>126</v>
       </c>
       <c r="H185" s="48" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
@@ -27310,7 +27310,7 @@
         <v>87</v>
       </c>
       <c r="C192" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="I192" s="46"/>
     </row>
@@ -27319,7 +27319,7 @@
         <v>123</v>
       </c>
       <c r="F193" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="I193" s="46">
         <v>1</v>
@@ -27336,7 +27336,7 @@
         <v>87</v>
       </c>
       <c r="C195" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="196" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
@@ -27923,7 +27923,7 @@
         <v>835</v>
       </c>
       <c r="H5" s="46" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -28045,7 +28045,7 @@
         <v>721</v>
       </c>
       <c r="K16" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="L16" t="s">
         <v>1130</v>
@@ -28427,7 +28427,7 @@
         <v>729</v>
       </c>
       <c r="K52" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="L52" t="s">
         <v>1130</v>

</xml_diff>